<commit_message>
SO for bidirectiona setting change
</commit_message>
<xml_diff>
--- a/I2C2SPI.xlsx
+++ b/I2C2SPI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="-15" windowWidth="13785" windowHeight="7020" activeTab="2"/>
+    <workbookView xWindow="345" yWindow="-15" windowWidth="13785" windowHeight="7020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pin assign" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="166">
   <si>
     <t>IO11</t>
   </si>
@@ -581,11 +581,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Bidirectional SO support for reading
-0x85:SI, 0x75:SO</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>0x85</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -691,6 +686,24 @@
   </si>
   <si>
     <t>0x00</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x3B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xFC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bidirectional SO support for reading
+0x85:read by SI, 0x75:read by SO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bidirectional SO support for reading
+0xFC:SO is output only, 0xB4:SO is bidirectional</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1384,6 +1397,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1393,19 +1418,25 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1414,25 +1445,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1749,7 +1762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
@@ -1827,7 +1842,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>78</v>
@@ -1862,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>78</v>
@@ -1895,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>78</v>
@@ -1930,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>78</v>
@@ -1998,7 +2013,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>77</v>
@@ -2060,7 +2075,7 @@
         <v>22</v>
       </c>
       <c r="J11" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>78</v>
@@ -2299,9 +2314,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H17"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -2334,10 +2351,10 @@
         <v>82</v>
       </c>
       <c r="D3" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3" s="53" t="s">
         <v>72</v>
@@ -2348,10 +2365,10 @@
       <c r="C4" s="54"/>
       <c r="D4" s="51"/>
       <c r="E4" s="52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="2:8">
@@ -2359,27 +2376,27 @@
       <c r="C5" s="44"/>
       <c r="D5" s="56"/>
       <c r="E5" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="53" t="s">
         <v>140</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="27">
       <c r="B6" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>82</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" s="52" t="s">
         <v>75</v>
       </c>
       <c r="F6" s="49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="27">
@@ -2390,13 +2407,13 @@
         <v>83</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E7" s="52" t="s">
         <v>74</v>
       </c>
       <c r="F7" s="49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H7" s="57"/>
     </row>
@@ -2408,97 +2425,103 @@
         <v>83</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="27">
+      <c r="B9" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="53" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="27">
-      <c r="B9" s="34" t="s">
+      <c r="F9" s="53" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="27">
+      <c r="B10" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C10" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D10" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E10" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F10" s="53" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="81">
-      <c r="B10" s="50" t="s">
+    <row r="11" spans="2:8" ht="81">
+      <c r="B11" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C11" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="E10" s="34" t="s">
+      <c r="D11" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="81">
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F12" s="49" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="81">
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="F11" s="49" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="55" t="s">
+    <row r="13" spans="2:8">
+      <c r="B13" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C13" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D13" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E13" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="62" t="s">
+      <c r="F13" s="62" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="58"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="63" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" s="58"/>
       <c r="C14" s="60"/>
-      <c r="D14" s="58"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -2506,10 +2529,10 @@
       <c r="C15" s="60"/>
       <c r="D15" s="58"/>
       <c r="E15" s="51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" s="63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -2517,20 +2540,31 @@
       <c r="C16" s="60"/>
       <c r="D16" s="58"/>
       <c r="E16" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="58"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="63" t="s">
+      <c r="F17" s="63" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="59"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="56" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" s="59"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F18" s="59" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2544,7 +2578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:BL116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="67" zoomScaleNormal="67" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5"/>
   <cols>
@@ -2563,22 +2597,22 @@
       <c r="I4" t="s">
         <v>123</v>
       </c>
-      <c r="O4" s="99" t="s">
+      <c r="O4" s="105" t="s">
         <v>121</v>
       </c>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="100" t="s">
+      <c r="P4" s="105"/>
+      <c r="Q4" s="105"/>
+      <c r="R4" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="98" t="s">
-        <v>154</v>
-      </c>
-      <c r="V4" s="98"/>
-      <c r="W4" s="98"/>
-      <c r="X4" s="98"/>
+      <c r="S4" s="106"/>
+      <c r="T4" s="106"/>
+      <c r="U4" s="107" t="s">
+        <v>153</v>
+      </c>
+      <c r="V4" s="107"/>
+      <c r="W4" s="107"/>
+      <c r="X4" s="107"/>
     </row>
     <row r="5" spans="3:64">
       <c r="C5" s="71" t="s">
@@ -2586,124 +2620,124 @@
       </c>
     </row>
     <row r="6" spans="3:64">
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97">
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91">
         <v>1</v>
       </c>
-      <c r="H6" s="97"/>
-      <c r="I6" s="97">
+      <c r="H6" s="91"/>
+      <c r="I6" s="91">
         <v>2</v>
       </c>
-      <c r="J6" s="97"/>
-      <c r="K6" s="97">
+      <c r="J6" s="91"/>
+      <c r="K6" s="91">
         <v>3</v>
       </c>
-      <c r="L6" s="97"/>
-      <c r="M6" s="97">
+      <c r="L6" s="91"/>
+      <c r="M6" s="91">
         <v>4</v>
       </c>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97">
+      <c r="N6" s="91"/>
+      <c r="O6" s="91">
         <v>5</v>
       </c>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="97">
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91">
         <v>6</v>
       </c>
-      <c r="R6" s="97"/>
-      <c r="S6" s="97">
+      <c r="R6" s="91"/>
+      <c r="S6" s="91">
         <v>7</v>
       </c>
-      <c r="T6" s="97"/>
-      <c r="U6" s="97">
+      <c r="T6" s="91"/>
+      <c r="U6" s="91">
         <v>8</v>
       </c>
-      <c r="V6" s="97"/>
-      <c r="W6" s="97" t="s">
+      <c r="V6" s="91"/>
+      <c r="W6" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="X6" s="97"/>
-      <c r="Y6" s="97">
+      <c r="X6" s="91"/>
+      <c r="Y6" s="91">
         <v>1</v>
       </c>
-      <c r="Z6" s="97"/>
-      <c r="AA6" s="97">
+      <c r="Z6" s="91"/>
+      <c r="AA6" s="91">
         <v>2</v>
       </c>
-      <c r="AB6" s="97"/>
-      <c r="AC6" s="97">
+      <c r="AB6" s="91"/>
+      <c r="AC6" s="91">
         <v>3</v>
       </c>
-      <c r="AD6" s="97"/>
-      <c r="AE6" s="97">
+      <c r="AD6" s="91"/>
+      <c r="AE6" s="91">
         <v>4</v>
       </c>
-      <c r="AF6" s="97"/>
-      <c r="AG6" s="97">
+      <c r="AF6" s="91"/>
+      <c r="AG6" s="91">
         <v>5</v>
       </c>
-      <c r="AH6" s="97"/>
-      <c r="AI6" s="97">
+      <c r="AH6" s="91"/>
+      <c r="AI6" s="91">
         <v>6</v>
       </c>
-      <c r="AJ6" s="97"/>
-      <c r="AK6" s="97">
+      <c r="AJ6" s="91"/>
+      <c r="AK6" s="91">
         <v>7</v>
       </c>
-      <c r="AL6" s="97"/>
-      <c r="AM6" s="97">
+      <c r="AL6" s="91"/>
+      <c r="AM6" s="91">
         <v>8</v>
       </c>
-      <c r="AN6" s="97"/>
-      <c r="AO6" s="97" t="s">
+      <c r="AN6" s="91"/>
+      <c r="AO6" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="AP6" s="97"/>
-      <c r="AQ6" s="97">
+      <c r="AP6" s="91"/>
+      <c r="AQ6" s="91">
         <v>1</v>
       </c>
-      <c r="AR6" s="97"/>
-      <c r="AS6" s="97">
+      <c r="AR6" s="91"/>
+      <c r="AS6" s="91">
         <v>2</v>
       </c>
-      <c r="AT6" s="97"/>
-      <c r="AU6" s="97">
+      <c r="AT6" s="91"/>
+      <c r="AU6" s="91">
         <v>3</v>
       </c>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97">
+      <c r="AV6" s="91"/>
+      <c r="AW6" s="91">
         <v>4</v>
       </c>
-      <c r="AX6" s="97"/>
-      <c r="AY6" s="97">
+      <c r="AX6" s="91"/>
+      <c r="AY6" s="91">
         <v>5</v>
       </c>
-      <c r="AZ6" s="97"/>
-      <c r="BA6" s="97">
+      <c r="AZ6" s="91"/>
+      <c r="BA6" s="91">
         <v>6</v>
       </c>
-      <c r="BB6" s="97"/>
-      <c r="BC6" s="97">
+      <c r="BB6" s="91"/>
+      <c r="BC6" s="91">
         <v>7</v>
       </c>
-      <c r="BD6" s="97"/>
-      <c r="BE6" s="97">
+      <c r="BD6" s="91"/>
+      <c r="BE6" s="91">
         <v>8</v>
       </c>
-      <c r="BF6" s="97"/>
-      <c r="BG6" s="97" t="s">
+      <c r="BF6" s="91"/>
+      <c r="BG6" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="BH6" s="97"/>
-      <c r="BJ6" s="97" t="s">
+      <c r="BH6" s="91"/>
+      <c r="BJ6" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="BK6" s="97"/>
-      <c r="BL6" s="97"/>
+      <c r="BK6" s="91"/>
+      <c r="BL6" s="91"/>
     </row>
     <row r="8" spans="3:64">
       <c r="C8" t="s">
@@ -2778,76 +2812,76 @@
       <c r="D10" s="78"/>
       <c r="E10" s="78"/>
       <c r="F10" s="79"/>
-      <c r="G10" s="91" t="s">
+      <c r="G10" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="92"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="92"/>
-      <c r="O10" s="92"/>
-      <c r="P10" s="93"/>
-      <c r="Q10" s="91" t="s">
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="96"/>
+      <c r="O10" s="96"/>
+      <c r="P10" s="97"/>
+      <c r="Q10" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="R10" s="92"/>
-      <c r="S10" s="92"/>
-      <c r="T10" s="93"/>
-      <c r="U10" s="91" t="s">
+      <c r="R10" s="96"/>
+      <c r="S10" s="96"/>
+      <c r="T10" s="97"/>
+      <c r="U10" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="V10" s="93"/>
-      <c r="W10" s="101" t="s">
+      <c r="V10" s="97"/>
+      <c r="W10" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="X10" s="102"/>
-      <c r="Y10" s="91" t="s">
+      <c r="X10" s="101"/>
+      <c r="Y10" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="Z10" s="92"/>
-      <c r="AA10" s="92"/>
-      <c r="AB10" s="92"/>
-      <c r="AC10" s="92"/>
-      <c r="AD10" s="92"/>
-      <c r="AE10" s="92"/>
-      <c r="AF10" s="92"/>
-      <c r="AG10" s="92"/>
-      <c r="AH10" s="92"/>
-      <c r="AI10" s="92"/>
-      <c r="AJ10" s="92"/>
-      <c r="AK10" s="92"/>
-      <c r="AL10" s="92"/>
-      <c r="AM10" s="92"/>
-      <c r="AN10" s="93"/>
-      <c r="AO10" s="101" t="s">
+      <c r="Z10" s="96"/>
+      <c r="AA10" s="96"/>
+      <c r="AB10" s="96"/>
+      <c r="AC10" s="96"/>
+      <c r="AD10" s="96"/>
+      <c r="AE10" s="96"/>
+      <c r="AF10" s="96"/>
+      <c r="AG10" s="96"/>
+      <c r="AH10" s="96"/>
+      <c r="AI10" s="96"/>
+      <c r="AJ10" s="96"/>
+      <c r="AK10" s="96"/>
+      <c r="AL10" s="96"/>
+      <c r="AM10" s="96"/>
+      <c r="AN10" s="97"/>
+      <c r="AO10" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="AP10" s="102"/>
-      <c r="AQ10" s="91" t="s">
+      <c r="AP10" s="101"/>
+      <c r="AQ10" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="AR10" s="92"/>
-      <c r="AS10" s="92"/>
-      <c r="AT10" s="92"/>
-      <c r="AU10" s="92"/>
-      <c r="AV10" s="92"/>
-      <c r="AW10" s="92"/>
-      <c r="AX10" s="92"/>
-      <c r="AY10" s="92"/>
-      <c r="AZ10" s="92"/>
-      <c r="BA10" s="92"/>
-      <c r="BB10" s="92"/>
-      <c r="BC10" s="92"/>
-      <c r="BD10" s="92"/>
-      <c r="BE10" s="92"/>
-      <c r="BF10" s="93"/>
-      <c r="BG10" s="101" t="s">
+      <c r="AR10" s="96"/>
+      <c r="AS10" s="96"/>
+      <c r="AT10" s="96"/>
+      <c r="AU10" s="96"/>
+      <c r="AV10" s="96"/>
+      <c r="AW10" s="96"/>
+      <c r="AX10" s="96"/>
+      <c r="AY10" s="96"/>
+      <c r="AZ10" s="96"/>
+      <c r="BA10" s="96"/>
+      <c r="BB10" s="96"/>
+      <c r="BC10" s="96"/>
+      <c r="BD10" s="96"/>
+      <c r="BE10" s="96"/>
+      <c r="BF10" s="97"/>
+      <c r="BG10" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="BH10" s="105"/>
+      <c r="BH10" s="104"/>
       <c r="BI10" s="82"/>
       <c r="BJ10" s="81"/>
       <c r="BK10" s="80"/>
@@ -2989,75 +3023,75 @@
       <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="95">
+      <c r="D16" s="93">
         <v>0</v>
       </c>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="95"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="95"/>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
-      <c r="P16" s="95"/>
-      <c r="Q16" s="95"/>
-      <c r="R16" s="95"/>
-      <c r="S16" s="95"/>
-      <c r="T16" s="95"/>
-      <c r="U16" s="95"/>
-      <c r="V16" s="95"/>
-      <c r="W16" s="95"/>
-      <c r="X16" s="95"/>
-      <c r="Y16" s="95"/>
-      <c r="Z16" s="96"/>
-      <c r="AA16" s="94" t="s">
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="93"/>
+      <c r="T16" s="93"/>
+      <c r="U16" s="93"/>
+      <c r="V16" s="93"/>
+      <c r="W16" s="93"/>
+      <c r="X16" s="93"/>
+      <c r="Y16" s="93"/>
+      <c r="Z16" s="94"/>
+      <c r="AA16" s="92" t="s">
         <v>112</v>
       </c>
-      <c r="AB16" s="95"/>
-      <c r="AC16" s="95"/>
-      <c r="AD16" s="95"/>
-      <c r="AE16" s="95"/>
-      <c r="AF16" s="95"/>
-      <c r="AG16" s="95"/>
-      <c r="AH16" s="95"/>
-      <c r="AI16" s="95"/>
-      <c r="AJ16" s="95"/>
-      <c r="AK16" s="95"/>
-      <c r="AL16" s="95"/>
-      <c r="AM16" s="95"/>
-      <c r="AN16" s="95"/>
-      <c r="AO16" s="95"/>
-      <c r="AP16" s="95"/>
-      <c r="AQ16" s="96"/>
+      <c r="AB16" s="93"/>
+      <c r="AC16" s="93"/>
+      <c r="AD16" s="93"/>
+      <c r="AE16" s="93"/>
+      <c r="AF16" s="93"/>
+      <c r="AG16" s="93"/>
+      <c r="AH16" s="93"/>
+      <c r="AI16" s="93"/>
+      <c r="AJ16" s="93"/>
+      <c r="AK16" s="93"/>
+      <c r="AL16" s="93"/>
+      <c r="AM16" s="93"/>
+      <c r="AN16" s="93"/>
+      <c r="AO16" s="93"/>
+      <c r="AP16" s="93"/>
+      <c r="AQ16" s="94"/>
       <c r="AR16" s="77"/>
-      <c r="AS16" s="94" t="s">
+      <c r="AS16" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="AT16" s="95"/>
-      <c r="AU16" s="95"/>
-      <c r="AV16" s="95"/>
-      <c r="AW16" s="95"/>
-      <c r="AX16" s="95"/>
-      <c r="AY16" s="95"/>
-      <c r="AZ16" s="95"/>
-      <c r="BA16" s="95"/>
-      <c r="BB16" s="95"/>
-      <c r="BC16" s="95"/>
-      <c r="BD16" s="95"/>
-      <c r="BE16" s="95"/>
-      <c r="BF16" s="95"/>
-      <c r="BG16" s="95"/>
-      <c r="BH16" s="95"/>
-      <c r="BI16" s="96"/>
+      <c r="AT16" s="93"/>
+      <c r="AU16" s="93"/>
+      <c r="AV16" s="93"/>
+      <c r="AW16" s="93"/>
+      <c r="AX16" s="93"/>
+      <c r="AY16" s="93"/>
+      <c r="AZ16" s="93"/>
+      <c r="BA16" s="93"/>
+      <c r="BB16" s="93"/>
+      <c r="BC16" s="93"/>
+      <c r="BD16" s="93"/>
+      <c r="BE16" s="93"/>
+      <c r="BF16" s="93"/>
+      <c r="BG16" s="93"/>
+      <c r="BH16" s="93"/>
+      <c r="BI16" s="94"/>
       <c r="BJ16" s="77"/>
-      <c r="BK16" s="94">
+      <c r="BK16" s="92">
         <v>0</v>
       </c>
-      <c r="BL16" s="95"/>
+      <c r="BL16" s="93"/>
     </row>
     <row r="18" spans="3:64">
       <c r="C18" t="s">
@@ -3086,45 +3120,45 @@
       <c r="X18" s="74"/>
       <c r="Y18" s="74"/>
       <c r="Z18" s="74"/>
-      <c r="AA18" s="91" t="s">
+      <c r="AA18" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="AB18" s="92"/>
-      <c r="AC18" s="92"/>
-      <c r="AD18" s="92"/>
-      <c r="AE18" s="92"/>
-      <c r="AF18" s="92"/>
-      <c r="AG18" s="92"/>
-      <c r="AH18" s="92"/>
-      <c r="AI18" s="92"/>
-      <c r="AJ18" s="92"/>
-      <c r="AK18" s="92"/>
-      <c r="AL18" s="92"/>
-      <c r="AM18" s="92"/>
-      <c r="AN18" s="92"/>
-      <c r="AO18" s="92"/>
-      <c r="AP18" s="92"/>
-      <c r="AQ18" s="93"/>
+      <c r="AB18" s="96"/>
+      <c r="AC18" s="96"/>
+      <c r="AD18" s="96"/>
+      <c r="AE18" s="96"/>
+      <c r="AF18" s="96"/>
+      <c r="AG18" s="96"/>
+      <c r="AH18" s="96"/>
+      <c r="AI18" s="96"/>
+      <c r="AJ18" s="96"/>
+      <c r="AK18" s="96"/>
+      <c r="AL18" s="96"/>
+      <c r="AM18" s="96"/>
+      <c r="AN18" s="96"/>
+      <c r="AO18" s="96"/>
+      <c r="AP18" s="96"/>
+      <c r="AQ18" s="97"/>
       <c r="AR18" s="74"/>
-      <c r="AS18" s="91" t="s">
+      <c r="AS18" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="AT18" s="92"/>
-      <c r="AU18" s="92"/>
-      <c r="AV18" s="92"/>
-      <c r="AW18" s="92"/>
-      <c r="AX18" s="92"/>
-      <c r="AY18" s="92"/>
-      <c r="AZ18" s="92"/>
-      <c r="BA18" s="92"/>
-      <c r="BB18" s="92"/>
-      <c r="BC18" s="92"/>
-      <c r="BD18" s="92"/>
-      <c r="BE18" s="92"/>
-      <c r="BF18" s="92"/>
-      <c r="BG18" s="92"/>
-      <c r="BH18" s="92"/>
-      <c r="BI18" s="93"/>
+      <c r="AT18" s="96"/>
+      <c r="AU18" s="96"/>
+      <c r="AV18" s="96"/>
+      <c r="AW18" s="96"/>
+      <c r="AX18" s="96"/>
+      <c r="AY18" s="96"/>
+      <c r="AZ18" s="96"/>
+      <c r="BA18" s="96"/>
+      <c r="BB18" s="96"/>
+      <c r="BC18" s="96"/>
+      <c r="BD18" s="96"/>
+      <c r="BE18" s="96"/>
+      <c r="BF18" s="96"/>
+      <c r="BG18" s="96"/>
+      <c r="BH18" s="96"/>
+      <c r="BI18" s="97"/>
       <c r="BJ18" s="74"/>
       <c r="BK18" s="89"/>
       <c r="BL18" s="88"/>
@@ -3201,102 +3235,102 @@
       </c>
     </row>
     <row r="24" spans="3:64">
-      <c r="D24" s="97" t="s">
+      <c r="D24" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="97">
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="91">
         <v>1</v>
       </c>
-      <c r="H24" s="97"/>
-      <c r="I24" s="97">
+      <c r="H24" s="91"/>
+      <c r="I24" s="91">
         <v>2</v>
       </c>
-      <c r="J24" s="97"/>
-      <c r="K24" s="97">
+      <c r="J24" s="91"/>
+      <c r="K24" s="91">
         <v>3</v>
       </c>
-      <c r="L24" s="97"/>
-      <c r="M24" s="97">
+      <c r="L24" s="91"/>
+      <c r="M24" s="91">
         <v>4</v>
       </c>
-      <c r="N24" s="97"/>
-      <c r="O24" s="97">
+      <c r="N24" s="91"/>
+      <c r="O24" s="91">
         <v>5</v>
       </c>
-      <c r="P24" s="97"/>
-      <c r="Q24" s="97">
+      <c r="P24" s="91"/>
+      <c r="Q24" s="91">
         <v>6</v>
       </c>
-      <c r="R24" s="97"/>
-      <c r="S24" s="97">
+      <c r="R24" s="91"/>
+      <c r="S24" s="91">
         <v>7</v>
       </c>
-      <c r="T24" s="97"/>
-      <c r="U24" s="97">
+      <c r="T24" s="91"/>
+      <c r="U24" s="91">
         <v>8</v>
       </c>
-      <c r="V24" s="97"/>
-      <c r="W24" s="97" t="s">
+      <c r="V24" s="91"/>
+      <c r="W24" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="X24" s="97"/>
-      <c r="Y24" s="97">
+      <c r="X24" s="91"/>
+      <c r="Y24" s="91">
         <v>1</v>
       </c>
-      <c r="Z24" s="97"/>
-      <c r="AA24" s="97">
+      <c r="Z24" s="91"/>
+      <c r="AA24" s="91">
         <v>2</v>
       </c>
-      <c r="AB24" s="97"/>
-      <c r="AC24" s="97">
+      <c r="AB24" s="91"/>
+      <c r="AC24" s="91">
         <v>3</v>
       </c>
-      <c r="AD24" s="97"/>
-      <c r="AE24" s="97">
+      <c r="AD24" s="91"/>
+      <c r="AE24" s="91">
         <v>4</v>
       </c>
-      <c r="AF24" s="97"/>
-      <c r="AG24" s="97">
+      <c r="AF24" s="91"/>
+      <c r="AG24" s="91">
         <v>5</v>
       </c>
-      <c r="AH24" s="97"/>
-      <c r="AI24" s="97">
+      <c r="AH24" s="91"/>
+      <c r="AI24" s="91">
         <v>6</v>
       </c>
-      <c r="AJ24" s="97"/>
-      <c r="AK24" s="97">
+      <c r="AJ24" s="91"/>
+      <c r="AK24" s="91">
         <v>7</v>
       </c>
-      <c r="AL24" s="97"/>
-      <c r="AM24" s="97">
+      <c r="AL24" s="91"/>
+      <c r="AM24" s="91">
         <v>8</v>
       </c>
-      <c r="AN24" s="97"/>
-      <c r="AO24" s="97" t="s">
+      <c r="AN24" s="91"/>
+      <c r="AO24" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="AP24" s="97"/>
-      <c r="AQ24" s="97" t="s">
+      <c r="AP24" s="91"/>
+      <c r="AQ24" s="91" t="s">
         <v>134</v>
       </c>
-      <c r="AR24" s="97"/>
-      <c r="AS24" s="97"/>
-      <c r="AU24" s="97"/>
-      <c r="AV24" s="97"/>
-      <c r="AW24" s="97"/>
-      <c r="AX24" s="97"/>
-      <c r="AY24" s="97"/>
-      <c r="AZ24" s="97"/>
-      <c r="BA24" s="97"/>
-      <c r="BB24" s="97"/>
-      <c r="BC24" s="97"/>
-      <c r="BD24" s="97"/>
-      <c r="BE24" s="97"/>
-      <c r="BF24" s="97"/>
-      <c r="BG24" s="97"/>
-      <c r="BH24" s="97"/>
+      <c r="AR24" s="91"/>
+      <c r="AS24" s="91"/>
+      <c r="AU24" s="91"/>
+      <c r="AV24" s="91"/>
+      <c r="AW24" s="91"/>
+      <c r="AX24" s="91"/>
+      <c r="AY24" s="91"/>
+      <c r="AZ24" s="91"/>
+      <c r="BA24" s="91"/>
+      <c r="BB24" s="91"/>
+      <c r="BC24" s="91"/>
+      <c r="BD24" s="91"/>
+      <c r="BE24" s="91"/>
+      <c r="BF24" s="91"/>
+      <c r="BG24" s="91"/>
+      <c r="BH24" s="91"/>
     </row>
     <row r="26" spans="3:64">
       <c r="C26" t="s">
@@ -3352,54 +3386,54 @@
       <c r="D28" s="78"/>
       <c r="E28" s="78"/>
       <c r="F28" s="79"/>
-      <c r="G28" s="91" t="s">
+      <c r="G28" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="92"/>
-      <c r="M28" s="92"/>
-      <c r="N28" s="92"/>
-      <c r="O28" s="92"/>
-      <c r="P28" s="93"/>
-      <c r="Q28" s="91" t="s">
+      <c r="H28" s="96"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="96"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="96"/>
+      <c r="N28" s="96"/>
+      <c r="O28" s="96"/>
+      <c r="P28" s="97"/>
+      <c r="Q28" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="R28" s="92"/>
-      <c r="S28" s="92"/>
-      <c r="T28" s="93"/>
-      <c r="U28" s="91" t="s">
+      <c r="R28" s="96"/>
+      <c r="S28" s="96"/>
+      <c r="T28" s="97"/>
+      <c r="U28" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="V28" s="93"/>
-      <c r="W28" s="101" t="s">
+      <c r="V28" s="97"/>
+      <c r="W28" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="X28" s="102"/>
-      <c r="Y28" s="91" t="s">
+      <c r="X28" s="101"/>
+      <c r="Y28" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="Z28" s="92"/>
-      <c r="AA28" s="92"/>
-      <c r="AB28" s="92"/>
-      <c r="AC28" s="92"/>
-      <c r="AD28" s="92"/>
-      <c r="AE28" s="92"/>
-      <c r="AF28" s="92"/>
-      <c r="AG28" s="92"/>
-      <c r="AH28" s="92"/>
-      <c r="AI28" s="92"/>
-      <c r="AJ28" s="92"/>
-      <c r="AK28" s="92"/>
-      <c r="AL28" s="92"/>
-      <c r="AM28" s="92"/>
-      <c r="AN28" s="93"/>
-      <c r="AO28" s="101" t="s">
+      <c r="Z28" s="96"/>
+      <c r="AA28" s="96"/>
+      <c r="AB28" s="96"/>
+      <c r="AC28" s="96"/>
+      <c r="AD28" s="96"/>
+      <c r="AE28" s="96"/>
+      <c r="AF28" s="96"/>
+      <c r="AG28" s="96"/>
+      <c r="AH28" s="96"/>
+      <c r="AI28" s="96"/>
+      <c r="AJ28" s="96"/>
+      <c r="AK28" s="96"/>
+      <c r="AL28" s="96"/>
+      <c r="AM28" s="96"/>
+      <c r="AN28" s="97"/>
+      <c r="AO28" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="AP28" s="102"/>
+      <c r="AP28" s="101"/>
       <c r="AQ28" s="80"/>
       <c r="AR28" s="78"/>
       <c r="AS28" s="79"/>
@@ -3502,54 +3536,54 @@
       <c r="C34" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="95">
+      <c r="D34" s="93">
         <v>0</v>
       </c>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="95"/>
-      <c r="K34" s="95"/>
-      <c r="L34" s="95"/>
-      <c r="M34" s="95"/>
-      <c r="N34" s="95"/>
-      <c r="O34" s="95"/>
-      <c r="P34" s="95"/>
-      <c r="Q34" s="95"/>
-      <c r="R34" s="95"/>
-      <c r="S34" s="95"/>
-      <c r="T34" s="95"/>
-      <c r="U34" s="95"/>
-      <c r="V34" s="95"/>
-      <c r="W34" s="95"/>
-      <c r="X34" s="95"/>
-      <c r="Y34" s="95"/>
-      <c r="Z34" s="96"/>
-      <c r="AA34" s="94" t="s">
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="93"/>
+      <c r="N34" s="93"/>
+      <c r="O34" s="93"/>
+      <c r="P34" s="93"/>
+      <c r="Q34" s="93"/>
+      <c r="R34" s="93"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="93"/>
+      <c r="V34" s="93"/>
+      <c r="W34" s="93"/>
+      <c r="X34" s="93"/>
+      <c r="Y34" s="93"/>
+      <c r="Z34" s="94"/>
+      <c r="AA34" s="92" t="s">
         <v>112</v>
       </c>
-      <c r="AB34" s="95"/>
-      <c r="AC34" s="95"/>
-      <c r="AD34" s="95"/>
-      <c r="AE34" s="95"/>
-      <c r="AF34" s="95"/>
-      <c r="AG34" s="95"/>
-      <c r="AH34" s="95"/>
-      <c r="AI34" s="95"/>
-      <c r="AJ34" s="95"/>
-      <c r="AK34" s="95"/>
-      <c r="AL34" s="95"/>
-      <c r="AM34" s="95"/>
-      <c r="AN34" s="95"/>
-      <c r="AO34" s="95"/>
-      <c r="AP34" s="95"/>
-      <c r="AQ34" s="96"/>
-      <c r="AR34" s="94">
+      <c r="AB34" s="93"/>
+      <c r="AC34" s="93"/>
+      <c r="AD34" s="93"/>
+      <c r="AE34" s="93"/>
+      <c r="AF34" s="93"/>
+      <c r="AG34" s="93"/>
+      <c r="AH34" s="93"/>
+      <c r="AI34" s="93"/>
+      <c r="AJ34" s="93"/>
+      <c r="AK34" s="93"/>
+      <c r="AL34" s="93"/>
+      <c r="AM34" s="93"/>
+      <c r="AN34" s="93"/>
+      <c r="AO34" s="93"/>
+      <c r="AP34" s="93"/>
+      <c r="AQ34" s="94"/>
+      <c r="AR34" s="92">
         <v>0</v>
       </c>
-      <c r="AS34" s="95"/>
+      <c r="AS34" s="93"/>
     </row>
     <row r="36" spans="3:64">
       <c r="C36" t="s">
@@ -3578,25 +3612,25 @@
       <c r="X36" s="74"/>
       <c r="Y36" s="74"/>
       <c r="Z36" s="74"/>
-      <c r="AA36" s="91" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB36" s="92"/>
-      <c r="AC36" s="92"/>
-      <c r="AD36" s="92"/>
-      <c r="AE36" s="92"/>
-      <c r="AF36" s="92"/>
-      <c r="AG36" s="92"/>
-      <c r="AH36" s="92"/>
-      <c r="AI36" s="92"/>
-      <c r="AJ36" s="92"/>
-      <c r="AK36" s="92"/>
-      <c r="AL36" s="92"/>
-      <c r="AM36" s="92"/>
-      <c r="AN36" s="92"/>
-      <c r="AO36" s="92"/>
-      <c r="AP36" s="92"/>
-      <c r="AQ36" s="93"/>
+      <c r="AA36" s="95" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB36" s="96"/>
+      <c r="AC36" s="96"/>
+      <c r="AD36" s="96"/>
+      <c r="AE36" s="96"/>
+      <c r="AF36" s="96"/>
+      <c r="AG36" s="96"/>
+      <c r="AH36" s="96"/>
+      <c r="AI36" s="96"/>
+      <c r="AJ36" s="96"/>
+      <c r="AK36" s="96"/>
+      <c r="AL36" s="96"/>
+      <c r="AM36" s="96"/>
+      <c r="AN36" s="96"/>
+      <c r="AO36" s="96"/>
+      <c r="AP36" s="96"/>
+      <c r="AQ36" s="97"/>
       <c r="AR36" s="74"/>
       <c r="AS36" s="74"/>
     </row>
@@ -3648,119 +3682,119 @@
       <c r="AS38" s="83"/>
     </row>
     <row r="41" spans="3:64">
-      <c r="G41" s="97">
+      <c r="G41" s="91">
         <v>1</v>
       </c>
-      <c r="H41" s="97"/>
-      <c r="I41" s="97">
+      <c r="H41" s="91"/>
+      <c r="I41" s="91">
         <v>2</v>
       </c>
-      <c r="J41" s="97"/>
-      <c r="K41" s="97">
+      <c r="J41" s="91"/>
+      <c r="K41" s="91">
         <v>3</v>
       </c>
-      <c r="L41" s="97"/>
-      <c r="M41" s="97">
+      <c r="L41" s="91"/>
+      <c r="M41" s="91">
         <v>4</v>
       </c>
-      <c r="N41" s="97"/>
-      <c r="O41" s="97">
+      <c r="N41" s="91"/>
+      <c r="O41" s="91">
         <v>5</v>
       </c>
-      <c r="P41" s="97"/>
-      <c r="Q41" s="97">
+      <c r="P41" s="91"/>
+      <c r="Q41" s="91">
         <v>6</v>
       </c>
-      <c r="R41" s="97"/>
-      <c r="S41" s="97">
+      <c r="R41" s="91"/>
+      <c r="S41" s="91">
         <v>7</v>
       </c>
-      <c r="T41" s="97"/>
-      <c r="U41" s="97">
+      <c r="T41" s="91"/>
+      <c r="U41" s="91">
         <v>8</v>
       </c>
-      <c r="V41" s="97"/>
-      <c r="W41" s="97" t="s">
+      <c r="V41" s="91"/>
+      <c r="W41" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="X41" s="97"/>
-      <c r="Y41" s="97">
+      <c r="X41" s="91"/>
+      <c r="Y41" s="91">
         <v>1</v>
       </c>
-      <c r="Z41" s="97"/>
-      <c r="AA41" s="97">
+      <c r="Z41" s="91"/>
+      <c r="AA41" s="91">
         <v>2</v>
       </c>
-      <c r="AB41" s="97"/>
-      <c r="AC41" s="97">
+      <c r="AB41" s="91"/>
+      <c r="AC41" s="91">
         <v>3</v>
       </c>
-      <c r="AD41" s="97"/>
-      <c r="AE41" s="97">
+      <c r="AD41" s="91"/>
+      <c r="AE41" s="91">
         <v>4</v>
       </c>
-      <c r="AF41" s="97"/>
-      <c r="AG41" s="97">
+      <c r="AF41" s="91"/>
+      <c r="AG41" s="91">
         <v>5</v>
       </c>
-      <c r="AH41" s="97"/>
-      <c r="AI41" s="97">
+      <c r="AH41" s="91"/>
+      <c r="AI41" s="91">
         <v>6</v>
       </c>
-      <c r="AJ41" s="97"/>
-      <c r="AK41" s="97">
+      <c r="AJ41" s="91"/>
+      <c r="AK41" s="91">
         <v>7</v>
       </c>
-      <c r="AL41" s="97"/>
-      <c r="AM41" s="97">
+      <c r="AL41" s="91"/>
+      <c r="AM41" s="91">
         <v>8</v>
       </c>
-      <c r="AN41" s="97"/>
-      <c r="AO41" s="97" t="s">
+      <c r="AN41" s="91"/>
+      <c r="AO41" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="AP41" s="97"/>
-      <c r="AQ41" s="97">
+      <c r="AP41" s="91"/>
+      <c r="AQ41" s="91">
         <v>1</v>
       </c>
-      <c r="AR41" s="97"/>
-      <c r="AS41" s="97">
+      <c r="AR41" s="91"/>
+      <c r="AS41" s="91">
         <v>2</v>
       </c>
-      <c r="AT41" s="97"/>
-      <c r="AU41" s="97">
+      <c r="AT41" s="91"/>
+      <c r="AU41" s="91">
         <v>3</v>
       </c>
-      <c r="AV41" s="97"/>
-      <c r="AW41" s="97">
+      <c r="AV41" s="91"/>
+      <c r="AW41" s="91">
         <v>4</v>
       </c>
-      <c r="AX41" s="97"/>
-      <c r="AY41" s="97">
+      <c r="AX41" s="91"/>
+      <c r="AY41" s="91">
         <v>5</v>
       </c>
-      <c r="AZ41" s="97"/>
-      <c r="BA41" s="97">
+      <c r="AZ41" s="91"/>
+      <c r="BA41" s="91">
         <v>6</v>
       </c>
-      <c r="BB41" s="97"/>
-      <c r="BC41" s="97">
+      <c r="BB41" s="91"/>
+      <c r="BC41" s="91">
         <v>7</v>
       </c>
-      <c r="BD41" s="97"/>
-      <c r="BE41" s="97">
+      <c r="BD41" s="91"/>
+      <c r="BE41" s="91">
         <v>8</v>
       </c>
-      <c r="BF41" s="97"/>
-      <c r="BG41" s="97" t="s">
+      <c r="BF41" s="91"/>
+      <c r="BG41" s="91" t="s">
         <v>125</v>
       </c>
-      <c r="BH41" s="97"/>
-      <c r="BI41" s="97" t="s">
+      <c r="BH41" s="91"/>
+      <c r="BI41" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="BJ41" s="97"/>
-      <c r="BK41" s="97"/>
+      <c r="BJ41" s="91"/>
+      <c r="BK41" s="91"/>
       <c r="BL41" s="72"/>
     </row>
     <row r="43" spans="3:64">
@@ -3827,76 +3861,76 @@
     <row r="45" spans="3:64">
       <c r="E45" s="1"/>
       <c r="F45" s="81"/>
-      <c r="G45" s="91" t="s">
+      <c r="G45" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="H45" s="92"/>
-      <c r="I45" s="92"/>
-      <c r="J45" s="92"/>
-      <c r="K45" s="92"/>
-      <c r="L45" s="92"/>
-      <c r="M45" s="92"/>
-      <c r="N45" s="92"/>
-      <c r="O45" s="92"/>
-      <c r="P45" s="93"/>
-      <c r="Q45" s="91" t="s">
+      <c r="H45" s="96"/>
+      <c r="I45" s="96"/>
+      <c r="J45" s="96"/>
+      <c r="K45" s="96"/>
+      <c r="L45" s="96"/>
+      <c r="M45" s="96"/>
+      <c r="N45" s="96"/>
+      <c r="O45" s="96"/>
+      <c r="P45" s="97"/>
+      <c r="Q45" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="R45" s="92"/>
-      <c r="S45" s="92"/>
-      <c r="T45" s="93"/>
-      <c r="U45" s="91" t="s">
+      <c r="R45" s="96"/>
+      <c r="S45" s="96"/>
+      <c r="T45" s="97"/>
+      <c r="U45" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="V45" s="93"/>
-      <c r="W45" s="101" t="s">
+      <c r="V45" s="97"/>
+      <c r="W45" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="X45" s="102"/>
-      <c r="Y45" s="94" t="s">
+      <c r="X45" s="101"/>
+      <c r="Y45" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="Z45" s="95"/>
-      <c r="AA45" s="95"/>
-      <c r="AB45" s="95"/>
-      <c r="AC45" s="95"/>
-      <c r="AD45" s="95"/>
-      <c r="AE45" s="95"/>
-      <c r="AF45" s="95"/>
-      <c r="AG45" s="95"/>
-      <c r="AH45" s="95"/>
-      <c r="AI45" s="95"/>
-      <c r="AJ45" s="95"/>
-      <c r="AK45" s="95"/>
-      <c r="AL45" s="95"/>
-      <c r="AM45" s="95"/>
-      <c r="AN45" s="96"/>
-      <c r="AO45" s="103" t="s">
+      <c r="Z45" s="93"/>
+      <c r="AA45" s="93"/>
+      <c r="AB45" s="93"/>
+      <c r="AC45" s="93"/>
+      <c r="AD45" s="93"/>
+      <c r="AE45" s="93"/>
+      <c r="AF45" s="93"/>
+      <c r="AG45" s="93"/>
+      <c r="AH45" s="93"/>
+      <c r="AI45" s="93"/>
+      <c r="AJ45" s="93"/>
+      <c r="AK45" s="93"/>
+      <c r="AL45" s="93"/>
+      <c r="AM45" s="93"/>
+      <c r="AN45" s="94"/>
+      <c r="AO45" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="AP45" s="104"/>
-      <c r="AQ45" s="94" t="s">
+      <c r="AP45" s="103"/>
+      <c r="AQ45" s="92" t="s">
         <v>131</v>
       </c>
-      <c r="AR45" s="95"/>
-      <c r="AS45" s="95"/>
-      <c r="AT45" s="95"/>
-      <c r="AU45" s="95"/>
-      <c r="AV45" s="95"/>
-      <c r="AW45" s="95"/>
-      <c r="AX45" s="95"/>
-      <c r="AY45" s="95"/>
-      <c r="AZ45" s="95"/>
-      <c r="BA45" s="95"/>
-      <c r="BB45" s="95"/>
-      <c r="BC45" s="95"/>
-      <c r="BD45" s="95"/>
-      <c r="BE45" s="95"/>
-      <c r="BF45" s="96"/>
-      <c r="BG45" s="106" t="s">
+      <c r="AR45" s="93"/>
+      <c r="AS45" s="93"/>
+      <c r="AT45" s="93"/>
+      <c r="AU45" s="93"/>
+      <c r="AV45" s="93"/>
+      <c r="AW45" s="93"/>
+      <c r="AX45" s="93"/>
+      <c r="AY45" s="93"/>
+      <c r="AZ45" s="93"/>
+      <c r="BA45" s="93"/>
+      <c r="BB45" s="93"/>
+      <c r="BC45" s="93"/>
+      <c r="BD45" s="93"/>
+      <c r="BE45" s="93"/>
+      <c r="BF45" s="94"/>
+      <c r="BG45" s="98" t="s">
         <v>119</v>
       </c>
-      <c r="BH45" s="107"/>
+      <c r="BH45" s="99"/>
       <c r="BI45" s="82"/>
       <c r="BJ45" s="81"/>
       <c r="BK45" s="80"/>
@@ -4025,27 +4059,27 @@
       <c r="BL49" s="85"/>
     </row>
     <row r="51" spans="3:64">
-      <c r="F51" s="95">
+      <c r="F51" s="93">
         <v>0</v>
       </c>
-      <c r="G51" s="95"/>
-      <c r="H51" s="95"/>
-      <c r="I51" s="95"/>
-      <c r="J51" s="95"/>
-      <c r="K51" s="95"/>
-      <c r="L51" s="95"/>
-      <c r="M51" s="95"/>
-      <c r="N51" s="95"/>
-      <c r="O51" s="95"/>
-      <c r="P51" s="95"/>
-      <c r="Q51" s="95"/>
-      <c r="R51" s="95"/>
-      <c r="S51" s="95"/>
-      <c r="T51" s="95"/>
-      <c r="U51" s="95"/>
-      <c r="V51" s="95"/>
-      <c r="W51" s="95"/>
-      <c r="X51" s="96"/>
+      <c r="G51" s="93"/>
+      <c r="H51" s="93"/>
+      <c r="I51" s="93"/>
+      <c r="J51" s="93"/>
+      <c r="K51" s="93"/>
+      <c r="L51" s="93"/>
+      <c r="M51" s="93"/>
+      <c r="N51" s="93"/>
+      <c r="O51" s="93"/>
+      <c r="P51" s="93"/>
+      <c r="Q51" s="93"/>
+      <c r="R51" s="93"/>
+      <c r="S51" s="93"/>
+      <c r="T51" s="93"/>
+      <c r="U51" s="93"/>
+      <c r="V51" s="93"/>
+      <c r="W51" s="93"/>
+      <c r="X51" s="94"/>
       <c r="Y51" s="90"/>
       <c r="Z51" s="88"/>
       <c r="AA51" s="88"/>
@@ -4084,10 +4118,10 @@
       <c r="BH51" s="88"/>
       <c r="BI51" s="88"/>
       <c r="BJ51" s="88"/>
-      <c r="BK51" s="94">
+      <c r="BK51" s="92">
         <v>0</v>
       </c>
-      <c r="BL51" s="95"/>
+      <c r="BL51" s="93"/>
     </row>
     <row r="53" spans="3:64">
       <c r="F53" s="73"/>
@@ -4111,45 +4145,45 @@
       <c r="X53" s="74"/>
       <c r="Y53" s="74"/>
       <c r="Z53" s="74"/>
-      <c r="AA53" s="91" t="s">
-        <v>152</v>
-      </c>
-      <c r="AB53" s="92"/>
-      <c r="AC53" s="92"/>
-      <c r="AD53" s="92"/>
-      <c r="AE53" s="92"/>
-      <c r="AF53" s="92"/>
-      <c r="AG53" s="92"/>
-      <c r="AH53" s="92"/>
-      <c r="AI53" s="92"/>
-      <c r="AJ53" s="92"/>
-      <c r="AK53" s="92"/>
-      <c r="AL53" s="92"/>
-      <c r="AM53" s="92"/>
-      <c r="AN53" s="92"/>
-      <c r="AO53" s="92"/>
-      <c r="AP53" s="92"/>
-      <c r="AQ53" s="93"/>
+      <c r="AA53" s="95" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB53" s="96"/>
+      <c r="AC53" s="96"/>
+      <c r="AD53" s="96"/>
+      <c r="AE53" s="96"/>
+      <c r="AF53" s="96"/>
+      <c r="AG53" s="96"/>
+      <c r="AH53" s="96"/>
+      <c r="AI53" s="96"/>
+      <c r="AJ53" s="96"/>
+      <c r="AK53" s="96"/>
+      <c r="AL53" s="96"/>
+      <c r="AM53" s="96"/>
+      <c r="AN53" s="96"/>
+      <c r="AO53" s="96"/>
+      <c r="AP53" s="96"/>
+      <c r="AQ53" s="97"/>
       <c r="AR53" s="74"/>
-      <c r="AS53" s="91" t="s">
+      <c r="AS53" s="95" t="s">
         <v>133</v>
       </c>
-      <c r="AT53" s="92"/>
-      <c r="AU53" s="92"/>
-      <c r="AV53" s="92"/>
-      <c r="AW53" s="92"/>
-      <c r="AX53" s="92"/>
-      <c r="AY53" s="92"/>
-      <c r="AZ53" s="92"/>
-      <c r="BA53" s="92"/>
-      <c r="BB53" s="92"/>
-      <c r="BC53" s="92"/>
-      <c r="BD53" s="92"/>
-      <c r="BE53" s="92"/>
-      <c r="BF53" s="92"/>
-      <c r="BG53" s="92"/>
-      <c r="BH53" s="92"/>
-      <c r="BI53" s="93"/>
+      <c r="AT53" s="96"/>
+      <c r="AU53" s="96"/>
+      <c r="AV53" s="96"/>
+      <c r="AW53" s="96"/>
+      <c r="AX53" s="96"/>
+      <c r="AY53" s="96"/>
+      <c r="AZ53" s="96"/>
+      <c r="BA53" s="96"/>
+      <c r="BB53" s="96"/>
+      <c r="BC53" s="96"/>
+      <c r="BD53" s="96"/>
+      <c r="BE53" s="96"/>
+      <c r="BF53" s="96"/>
+      <c r="BG53" s="96"/>
+      <c r="BH53" s="96"/>
+      <c r="BI53" s="97"/>
       <c r="BJ53" s="75"/>
       <c r="BK53" s="88"/>
       <c r="BL53" s="88"/>
@@ -4230,124 +4264,124 @@
       </c>
     </row>
     <row r="58" spans="3:64">
-      <c r="D58" s="97" t="s">
+      <c r="D58" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="E58" s="97"/>
-      <c r="F58" s="97"/>
-      <c r="G58" s="97">
+      <c r="E58" s="91"/>
+      <c r="F58" s="91"/>
+      <c r="G58" s="91">
         <v>1</v>
       </c>
-      <c r="H58" s="97"/>
-      <c r="I58" s="97">
+      <c r="H58" s="91"/>
+      <c r="I58" s="91">
         <v>2</v>
       </c>
-      <c r="J58" s="97"/>
-      <c r="K58" s="97">
+      <c r="J58" s="91"/>
+      <c r="K58" s="91">
         <v>3</v>
       </c>
-      <c r="L58" s="97"/>
-      <c r="M58" s="97">
+      <c r="L58" s="91"/>
+      <c r="M58" s="91">
         <v>4</v>
       </c>
-      <c r="N58" s="97"/>
-      <c r="O58" s="97">
+      <c r="N58" s="91"/>
+      <c r="O58" s="91">
         <v>5</v>
       </c>
-      <c r="P58" s="97"/>
-      <c r="Q58" s="97">
+      <c r="P58" s="91"/>
+      <c r="Q58" s="91">
         <v>6</v>
       </c>
-      <c r="R58" s="97"/>
-      <c r="S58" s="97">
+      <c r="R58" s="91"/>
+      <c r="S58" s="91">
         <v>7</v>
       </c>
-      <c r="T58" s="97"/>
-      <c r="U58" s="97">
+      <c r="T58" s="91"/>
+      <c r="U58" s="91">
         <v>8</v>
       </c>
-      <c r="V58" s="97"/>
-      <c r="W58" s="97" t="s">
+      <c r="V58" s="91"/>
+      <c r="W58" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="X58" s="97"/>
-      <c r="Y58" s="97">
+      <c r="X58" s="91"/>
+      <c r="Y58" s="91">
         <v>1</v>
       </c>
-      <c r="Z58" s="97"/>
-      <c r="AA58" s="97">
+      <c r="Z58" s="91"/>
+      <c r="AA58" s="91">
         <v>2</v>
       </c>
-      <c r="AB58" s="97"/>
-      <c r="AC58" s="97">
+      <c r="AB58" s="91"/>
+      <c r="AC58" s="91">
         <v>3</v>
       </c>
-      <c r="AD58" s="97"/>
-      <c r="AE58" s="97">
+      <c r="AD58" s="91"/>
+      <c r="AE58" s="91">
         <v>4</v>
       </c>
-      <c r="AF58" s="97"/>
-      <c r="AG58" s="97">
+      <c r="AF58" s="91"/>
+      <c r="AG58" s="91">
         <v>5</v>
       </c>
-      <c r="AH58" s="97"/>
-      <c r="AI58" s="97">
+      <c r="AH58" s="91"/>
+      <c r="AI58" s="91">
         <v>6</v>
       </c>
-      <c r="AJ58" s="97"/>
-      <c r="AK58" s="97">
+      <c r="AJ58" s="91"/>
+      <c r="AK58" s="91">
         <v>7</v>
       </c>
-      <c r="AL58" s="97"/>
-      <c r="AM58" s="97">
+      <c r="AL58" s="91"/>
+      <c r="AM58" s="91">
         <v>8</v>
       </c>
-      <c r="AN58" s="97"/>
-      <c r="AO58" s="97" t="s">
+      <c r="AN58" s="91"/>
+      <c r="AO58" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="AP58" s="97"/>
-      <c r="AQ58" s="97">
+      <c r="AP58" s="91"/>
+      <c r="AQ58" s="91">
         <v>1</v>
       </c>
-      <c r="AR58" s="97"/>
-      <c r="AS58" s="97">
+      <c r="AR58" s="91"/>
+      <c r="AS58" s="91">
         <v>2</v>
       </c>
-      <c r="AT58" s="97"/>
-      <c r="AU58" s="97">
+      <c r="AT58" s="91"/>
+      <c r="AU58" s="91">
         <v>3</v>
       </c>
-      <c r="AV58" s="97"/>
-      <c r="AW58" s="97">
+      <c r="AV58" s="91"/>
+      <c r="AW58" s="91">
         <v>4</v>
       </c>
-      <c r="AX58" s="97"/>
-      <c r="AY58" s="97">
+      <c r="AX58" s="91"/>
+      <c r="AY58" s="91">
         <v>5</v>
       </c>
-      <c r="AZ58" s="97"/>
-      <c r="BA58" s="97">
+      <c r="AZ58" s="91"/>
+      <c r="BA58" s="91">
         <v>6</v>
       </c>
-      <c r="BB58" s="97"/>
-      <c r="BC58" s="97">
+      <c r="BB58" s="91"/>
+      <c r="BC58" s="91">
         <v>7</v>
       </c>
-      <c r="BD58" s="97"/>
-      <c r="BE58" s="97">
+      <c r="BD58" s="91"/>
+      <c r="BE58" s="91">
         <v>8</v>
       </c>
-      <c r="BF58" s="97"/>
-      <c r="BG58" s="97" t="s">
+      <c r="BF58" s="91"/>
+      <c r="BG58" s="91" t="s">
         <v>125</v>
       </c>
-      <c r="BH58" s="97"/>
-      <c r="BI58" s="97" t="s">
+      <c r="BH58" s="91"/>
+      <c r="BI58" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="BJ58" s="97"/>
-      <c r="BK58" s="97"/>
+      <c r="BJ58" s="91"/>
+      <c r="BK58" s="91"/>
       <c r="BL58" s="72"/>
     </row>
     <row r="60" spans="3:64">
@@ -4423,76 +4457,76 @@
       <c r="D62" s="78"/>
       <c r="E62" s="78"/>
       <c r="F62" s="79"/>
-      <c r="G62" s="91" t="s">
+      <c r="G62" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="H62" s="92"/>
-      <c r="I62" s="92"/>
-      <c r="J62" s="92"/>
-      <c r="K62" s="92"/>
-      <c r="L62" s="92"/>
-      <c r="M62" s="92"/>
-      <c r="N62" s="92"/>
-      <c r="O62" s="92"/>
-      <c r="P62" s="93"/>
-      <c r="Q62" s="91" t="s">
+      <c r="H62" s="96"/>
+      <c r="I62" s="96"/>
+      <c r="J62" s="96"/>
+      <c r="K62" s="96"/>
+      <c r="L62" s="96"/>
+      <c r="M62" s="96"/>
+      <c r="N62" s="96"/>
+      <c r="O62" s="96"/>
+      <c r="P62" s="97"/>
+      <c r="Q62" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="R62" s="92"/>
-      <c r="S62" s="92"/>
-      <c r="T62" s="93"/>
-      <c r="U62" s="91" t="s">
+      <c r="R62" s="96"/>
+      <c r="S62" s="96"/>
+      <c r="T62" s="97"/>
+      <c r="U62" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="V62" s="93"/>
-      <c r="W62" s="101" t="s">
+      <c r="V62" s="97"/>
+      <c r="W62" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="X62" s="102"/>
-      <c r="Y62" s="94" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z62" s="95"/>
-      <c r="AA62" s="95"/>
-      <c r="AB62" s="95"/>
-      <c r="AC62" s="95"/>
-      <c r="AD62" s="95"/>
-      <c r="AE62" s="95"/>
-      <c r="AF62" s="95"/>
-      <c r="AG62" s="95"/>
-      <c r="AH62" s="95"/>
-      <c r="AI62" s="95"/>
-      <c r="AJ62" s="95"/>
-      <c r="AK62" s="95"/>
-      <c r="AL62" s="95"/>
-      <c r="AM62" s="95"/>
-      <c r="AN62" s="96"/>
-      <c r="AO62" s="103" t="s">
+      <c r="X62" s="101"/>
+      <c r="Y62" s="92" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z62" s="93"/>
+      <c r="AA62" s="93"/>
+      <c r="AB62" s="93"/>
+      <c r="AC62" s="93"/>
+      <c r="AD62" s="93"/>
+      <c r="AE62" s="93"/>
+      <c r="AF62" s="93"/>
+      <c r="AG62" s="93"/>
+      <c r="AH62" s="93"/>
+      <c r="AI62" s="93"/>
+      <c r="AJ62" s="93"/>
+      <c r="AK62" s="93"/>
+      <c r="AL62" s="93"/>
+      <c r="AM62" s="93"/>
+      <c r="AN62" s="94"/>
+      <c r="AO62" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="AP62" s="104"/>
-      <c r="AQ62" s="94" t="s">
+      <c r="AP62" s="103"/>
+      <c r="AQ62" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="AR62" s="95"/>
-      <c r="AS62" s="95"/>
-      <c r="AT62" s="95"/>
-      <c r="AU62" s="95"/>
-      <c r="AV62" s="95"/>
-      <c r="AW62" s="95"/>
-      <c r="AX62" s="95"/>
-      <c r="AY62" s="95"/>
-      <c r="AZ62" s="95"/>
-      <c r="BA62" s="95"/>
-      <c r="BB62" s="95"/>
-      <c r="BC62" s="95"/>
-      <c r="BD62" s="95"/>
-      <c r="BE62" s="95"/>
-      <c r="BF62" s="96"/>
-      <c r="BG62" s="106" t="s">
+      <c r="AR62" s="93"/>
+      <c r="AS62" s="93"/>
+      <c r="AT62" s="93"/>
+      <c r="AU62" s="93"/>
+      <c r="AV62" s="93"/>
+      <c r="AW62" s="93"/>
+      <c r="AX62" s="93"/>
+      <c r="AY62" s="93"/>
+      <c r="AZ62" s="93"/>
+      <c r="BA62" s="93"/>
+      <c r="BB62" s="93"/>
+      <c r="BC62" s="93"/>
+      <c r="BD62" s="93"/>
+      <c r="BE62" s="93"/>
+      <c r="BF62" s="94"/>
+      <c r="BG62" s="98" t="s">
         <v>119</v>
       </c>
-      <c r="BH62" s="107"/>
+      <c r="BH62" s="99"/>
       <c r="BI62" s="82"/>
       <c r="BJ62" s="81"/>
       <c r="BK62" s="80"/>
@@ -4634,29 +4668,29 @@
       <c r="C68" t="s">
         <v>47</v>
       </c>
-      <c r="D68" s="95">
+      <c r="D68" s="93">
         <v>0</v>
       </c>
-      <c r="E68" s="95"/>
-      <c r="F68" s="95"/>
-      <c r="G68" s="95"/>
-      <c r="H68" s="95"/>
-      <c r="I68" s="95"/>
-      <c r="J68" s="95"/>
-      <c r="K68" s="95"/>
-      <c r="L68" s="95"/>
-      <c r="M68" s="95"/>
-      <c r="N68" s="95"/>
-      <c r="O68" s="95"/>
-      <c r="P68" s="95"/>
-      <c r="Q68" s="95"/>
-      <c r="R68" s="95"/>
-      <c r="S68" s="95"/>
-      <c r="T68" s="95"/>
-      <c r="U68" s="95"/>
-      <c r="V68" s="95"/>
-      <c r="W68" s="95"/>
-      <c r="X68" s="96"/>
+      <c r="E68" s="93"/>
+      <c r="F68" s="93"/>
+      <c r="G68" s="93"/>
+      <c r="H68" s="93"/>
+      <c r="I68" s="93"/>
+      <c r="J68" s="93"/>
+      <c r="K68" s="93"/>
+      <c r="L68" s="93"/>
+      <c r="M68" s="93"/>
+      <c r="N68" s="93"/>
+      <c r="O68" s="93"/>
+      <c r="P68" s="93"/>
+      <c r="Q68" s="93"/>
+      <c r="R68" s="93"/>
+      <c r="S68" s="93"/>
+      <c r="T68" s="93"/>
+      <c r="U68" s="93"/>
+      <c r="V68" s="93"/>
+      <c r="W68" s="93"/>
+      <c r="X68" s="94"/>
       <c r="Y68" s="90"/>
       <c r="Z68" s="88"/>
       <c r="AA68" s="88"/>
@@ -4695,10 +4729,10 @@
       <c r="BH68" s="88"/>
       <c r="BI68" s="88"/>
       <c r="BJ68" s="88"/>
-      <c r="BK68" s="94">
+      <c r="BK68" s="92">
         <v>0</v>
       </c>
-      <c r="BL68" s="95"/>
+      <c r="BL68" s="93"/>
     </row>
     <row r="70" spans="3:64">
       <c r="C70" t="s">
@@ -4727,45 +4761,45 @@
       <c r="X70" s="74"/>
       <c r="Y70" s="74"/>
       <c r="Z70" s="74"/>
-      <c r="AA70" s="91" t="s">
+      <c r="AA70" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="AB70" s="92"/>
-      <c r="AC70" s="92"/>
-      <c r="AD70" s="92"/>
-      <c r="AE70" s="92"/>
-      <c r="AF70" s="92"/>
-      <c r="AG70" s="92"/>
-      <c r="AH70" s="92"/>
-      <c r="AI70" s="92"/>
-      <c r="AJ70" s="92"/>
-      <c r="AK70" s="92"/>
-      <c r="AL70" s="92"/>
-      <c r="AM70" s="92"/>
-      <c r="AN70" s="92"/>
-      <c r="AO70" s="92"/>
-      <c r="AP70" s="92"/>
-      <c r="AQ70" s="93"/>
+      <c r="AB70" s="96"/>
+      <c r="AC70" s="96"/>
+      <c r="AD70" s="96"/>
+      <c r="AE70" s="96"/>
+      <c r="AF70" s="96"/>
+      <c r="AG70" s="96"/>
+      <c r="AH70" s="96"/>
+      <c r="AI70" s="96"/>
+      <c r="AJ70" s="96"/>
+      <c r="AK70" s="96"/>
+      <c r="AL70" s="96"/>
+      <c r="AM70" s="96"/>
+      <c r="AN70" s="96"/>
+      <c r="AO70" s="96"/>
+      <c r="AP70" s="96"/>
+      <c r="AQ70" s="97"/>
       <c r="AR70" s="74"/>
-      <c r="AS70" s="91" t="s">
+      <c r="AS70" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="AT70" s="92"/>
-      <c r="AU70" s="92"/>
-      <c r="AV70" s="92"/>
-      <c r="AW70" s="92"/>
-      <c r="AX70" s="92"/>
-      <c r="AY70" s="92"/>
-      <c r="AZ70" s="92"/>
-      <c r="BA70" s="92"/>
-      <c r="BB70" s="92"/>
-      <c r="BC70" s="92"/>
-      <c r="BD70" s="92"/>
-      <c r="BE70" s="92"/>
-      <c r="BF70" s="92"/>
-      <c r="BG70" s="92"/>
-      <c r="BH70" s="92"/>
-      <c r="BI70" s="93"/>
+      <c r="AT70" s="96"/>
+      <c r="AU70" s="96"/>
+      <c r="AV70" s="96"/>
+      <c r="AW70" s="96"/>
+      <c r="AX70" s="96"/>
+      <c r="AY70" s="96"/>
+      <c r="AZ70" s="96"/>
+      <c r="BA70" s="96"/>
+      <c r="BB70" s="96"/>
+      <c r="BC70" s="96"/>
+      <c r="BD70" s="96"/>
+      <c r="BE70" s="96"/>
+      <c r="BF70" s="96"/>
+      <c r="BG70" s="96"/>
+      <c r="BH70" s="96"/>
+      <c r="BI70" s="97"/>
       <c r="BJ70" s="75"/>
       <c r="BK70" s="88"/>
       <c r="BL70" s="88"/>
@@ -4988,72 +5022,72 @@
       <c r="D81" s="69"/>
       <c r="E81" s="69"/>
       <c r="F81" s="69"/>
-      <c r="G81" s="94">
+      <c r="G81" s="92">
         <v>7</v>
       </c>
-      <c r="H81" s="96"/>
-      <c r="I81" s="94">
+      <c r="H81" s="94"/>
+      <c r="I81" s="92">
         <v>6</v>
       </c>
-      <c r="J81" s="96"/>
-      <c r="K81" s="94">
+      <c r="J81" s="94"/>
+      <c r="K81" s="92">
         <v>5</v>
       </c>
-      <c r="L81" s="96"/>
-      <c r="M81" s="94">
+      <c r="L81" s="94"/>
+      <c r="M81" s="92">
         <v>4</v>
       </c>
-      <c r="N81" s="96"/>
-      <c r="O81" s="94">
+      <c r="N81" s="94"/>
+      <c r="O81" s="92">
         <v>3</v>
       </c>
-      <c r="P81" s="96"/>
-      <c r="Q81" s="94">
+      <c r="P81" s="94"/>
+      <c r="Q81" s="92">
         <v>2</v>
       </c>
-      <c r="R81" s="96"/>
-      <c r="S81" s="94">
+      <c r="R81" s="94"/>
+      <c r="S81" s="92">
         <v>1</v>
       </c>
-      <c r="T81" s="96"/>
-      <c r="U81" s="94">
+      <c r="T81" s="94"/>
+      <c r="U81" s="92">
         <v>0</v>
       </c>
-      <c r="V81" s="96"/>
+      <c r="V81" s="94"/>
       <c r="W81" s="69"/>
       <c r="X81" s="69"/>
-      <c r="Y81" s="94">
+      <c r="Y81" s="92">
         <v>7</v>
       </c>
-      <c r="Z81" s="96"/>
-      <c r="AA81" s="94">
+      <c r="Z81" s="94"/>
+      <c r="AA81" s="92">
         <v>6</v>
       </c>
-      <c r="AB81" s="96"/>
-      <c r="AC81" s="94">
+      <c r="AB81" s="94"/>
+      <c r="AC81" s="92">
         <v>5</v>
       </c>
-      <c r="AD81" s="96"/>
-      <c r="AE81" s="94">
+      <c r="AD81" s="94"/>
+      <c r="AE81" s="92">
         <v>4</v>
       </c>
-      <c r="AF81" s="96"/>
-      <c r="AG81" s="94">
+      <c r="AF81" s="94"/>
+      <c r="AG81" s="92">
         <v>3</v>
       </c>
-      <c r="AH81" s="96"/>
-      <c r="AI81" s="94">
+      <c r="AH81" s="94"/>
+      <c r="AI81" s="92">
         <v>2</v>
       </c>
-      <c r="AJ81" s="96"/>
-      <c r="AK81" s="94">
+      <c r="AJ81" s="94"/>
+      <c r="AK81" s="92">
         <v>1</v>
       </c>
-      <c r="AL81" s="96"/>
-      <c r="AM81" s="94">
+      <c r="AL81" s="94"/>
+      <c r="AM81" s="92">
         <v>0</v>
       </c>
-      <c r="AN81" s="96"/>
+      <c r="AN81" s="94"/>
       <c r="AO81" s="69"/>
       <c r="AP81" s="69"/>
       <c r="AQ81" s="69"/>
@@ -5069,72 +5103,72 @@
       <c r="E83" s="69"/>
       <c r="F83" s="69"/>
       <c r="G83" s="69"/>
-      <c r="H83" s="91">
+      <c r="H83" s="95">
         <v>7</v>
       </c>
-      <c r="I83" s="93"/>
-      <c r="J83" s="91">
+      <c r="I83" s="97"/>
+      <c r="J83" s="95">
         <v>6</v>
       </c>
-      <c r="K83" s="93"/>
-      <c r="L83" s="91">
+      <c r="K83" s="97"/>
+      <c r="L83" s="95">
         <v>5</v>
       </c>
-      <c r="M83" s="93"/>
-      <c r="N83" s="91">
+      <c r="M83" s="97"/>
+      <c r="N83" s="95">
         <v>4</v>
       </c>
-      <c r="O83" s="93"/>
-      <c r="P83" s="91">
+      <c r="O83" s="97"/>
+      <c r="P83" s="95">
         <v>3</v>
       </c>
-      <c r="Q83" s="93"/>
-      <c r="R83" s="91">
+      <c r="Q83" s="97"/>
+      <c r="R83" s="95">
         <v>2</v>
       </c>
-      <c r="S83" s="93"/>
-      <c r="T83" s="91">
+      <c r="S83" s="97"/>
+      <c r="T83" s="95">
         <v>1</v>
       </c>
-      <c r="U83" s="93"/>
-      <c r="V83" s="91">
+      <c r="U83" s="97"/>
+      <c r="V83" s="95">
         <v>0</v>
       </c>
-      <c r="W83" s="93"/>
+      <c r="W83" s="97"/>
       <c r="X83" s="69"/>
       <c r="Y83" s="69"/>
-      <c r="Z83" s="91">
+      <c r="Z83" s="95">
         <v>7</v>
       </c>
-      <c r="AA83" s="93"/>
-      <c r="AB83" s="91">
+      <c r="AA83" s="97"/>
+      <c r="AB83" s="95">
         <v>6</v>
       </c>
-      <c r="AC83" s="93"/>
-      <c r="AD83" s="91">
+      <c r="AC83" s="97"/>
+      <c r="AD83" s="95">
         <v>5</v>
       </c>
-      <c r="AE83" s="93"/>
-      <c r="AF83" s="91">
+      <c r="AE83" s="97"/>
+      <c r="AF83" s="95">
         <v>4</v>
       </c>
-      <c r="AG83" s="93"/>
-      <c r="AH83" s="91">
+      <c r="AG83" s="97"/>
+      <c r="AH83" s="95">
         <v>3</v>
       </c>
-      <c r="AI83" s="93"/>
-      <c r="AJ83" s="91">
+      <c r="AI83" s="97"/>
+      <c r="AJ83" s="95">
         <v>2</v>
       </c>
-      <c r="AK83" s="93"/>
-      <c r="AL83" s="91">
+      <c r="AK83" s="97"/>
+      <c r="AL83" s="95">
         <v>1</v>
       </c>
-      <c r="AM83" s="93"/>
-      <c r="AN83" s="91">
+      <c r="AM83" s="97"/>
+      <c r="AN83" s="95">
         <v>0</v>
       </c>
-      <c r="AO83" s="93"/>
+      <c r="AO83" s="97"/>
       <c r="AP83" s="69"/>
       <c r="AQ83" s="69"/>
       <c r="AR83" s="69"/>
@@ -5310,72 +5344,72 @@
       <c r="E92" s="69"/>
       <c r="F92" s="69"/>
       <c r="G92" s="69"/>
-      <c r="H92" s="94">
+      <c r="H92" s="92">
         <v>7</v>
       </c>
-      <c r="I92" s="96"/>
-      <c r="J92" s="94">
+      <c r="I92" s="94"/>
+      <c r="J92" s="92">
         <v>6</v>
       </c>
-      <c r="K92" s="96"/>
-      <c r="L92" s="94">
+      <c r="K92" s="94"/>
+      <c r="L92" s="92">
         <v>5</v>
       </c>
-      <c r="M92" s="96"/>
-      <c r="N92" s="94">
+      <c r="M92" s="94"/>
+      <c r="N92" s="92">
         <v>4</v>
       </c>
-      <c r="O92" s="96"/>
-      <c r="P92" s="94">
+      <c r="O92" s="94"/>
+      <c r="P92" s="92">
         <v>3</v>
       </c>
-      <c r="Q92" s="96"/>
-      <c r="R92" s="94">
+      <c r="Q92" s="94"/>
+      <c r="R92" s="92">
         <v>2</v>
       </c>
-      <c r="S92" s="96"/>
-      <c r="T92" s="94">
+      <c r="S92" s="94"/>
+      <c r="T92" s="92">
         <v>1</v>
       </c>
-      <c r="U92" s="96"/>
-      <c r="V92" s="94">
+      <c r="U92" s="94"/>
+      <c r="V92" s="92">
         <v>0</v>
       </c>
-      <c r="W92" s="96"/>
+      <c r="W92" s="94"/>
       <c r="X92" s="69"/>
       <c r="Y92" s="69"/>
-      <c r="Z92" s="94">
+      <c r="Z92" s="92">
         <v>7</v>
       </c>
-      <c r="AA92" s="96"/>
-      <c r="AB92" s="94">
+      <c r="AA92" s="94"/>
+      <c r="AB92" s="92">
         <v>6</v>
       </c>
-      <c r="AC92" s="96"/>
-      <c r="AD92" s="94">
+      <c r="AC92" s="94"/>
+      <c r="AD92" s="92">
         <v>5</v>
       </c>
-      <c r="AE92" s="96"/>
-      <c r="AF92" s="94">
+      <c r="AE92" s="94"/>
+      <c r="AF92" s="92">
         <v>4</v>
       </c>
-      <c r="AG92" s="96"/>
-      <c r="AH92" s="94">
+      <c r="AG92" s="94"/>
+      <c r="AH92" s="92">
         <v>3</v>
       </c>
-      <c r="AI92" s="96"/>
-      <c r="AJ92" s="94">
+      <c r="AI92" s="94"/>
+      <c r="AJ92" s="92">
         <v>2</v>
       </c>
-      <c r="AK92" s="96"/>
-      <c r="AL92" s="94">
+      <c r="AK92" s="94"/>
+      <c r="AL92" s="92">
         <v>1</v>
       </c>
-      <c r="AM92" s="96"/>
-      <c r="AN92" s="94">
+      <c r="AM92" s="94"/>
+      <c r="AN92" s="92">
         <v>0</v>
       </c>
-      <c r="AO92" s="96"/>
+      <c r="AO92" s="94"/>
       <c r="AP92" s="69"/>
       <c r="AQ92" s="69"/>
       <c r="AR92" s="69"/>
@@ -5389,72 +5423,72 @@
       <c r="D94" s="69"/>
       <c r="E94" s="69"/>
       <c r="F94" s="69"/>
-      <c r="G94" s="91">
+      <c r="G94" s="95">
         <v>7</v>
       </c>
-      <c r="H94" s="93"/>
-      <c r="I94" s="91">
+      <c r="H94" s="97"/>
+      <c r="I94" s="95">
         <v>6</v>
       </c>
-      <c r="J94" s="93"/>
-      <c r="K94" s="91">
+      <c r="J94" s="97"/>
+      <c r="K94" s="95">
         <v>5</v>
       </c>
-      <c r="L94" s="93"/>
-      <c r="M94" s="91">
+      <c r="L94" s="97"/>
+      <c r="M94" s="95">
         <v>4</v>
       </c>
-      <c r="N94" s="93"/>
-      <c r="O94" s="91">
+      <c r="N94" s="97"/>
+      <c r="O94" s="95">
         <v>3</v>
       </c>
-      <c r="P94" s="93"/>
-      <c r="Q94" s="91">
+      <c r="P94" s="97"/>
+      <c r="Q94" s="95">
         <v>2</v>
       </c>
-      <c r="R94" s="93"/>
-      <c r="S94" s="91">
+      <c r="R94" s="97"/>
+      <c r="S94" s="95">
         <v>1</v>
       </c>
-      <c r="T94" s="93"/>
-      <c r="U94" s="91">
+      <c r="T94" s="97"/>
+      <c r="U94" s="95">
         <v>0</v>
       </c>
-      <c r="V94" s="93"/>
+      <c r="V94" s="97"/>
       <c r="W94" s="69"/>
       <c r="X94" s="69"/>
-      <c r="Y94" s="91">
+      <c r="Y94" s="95">
         <v>7</v>
       </c>
-      <c r="Z94" s="93"/>
-      <c r="AA94" s="91">
+      <c r="Z94" s="97"/>
+      <c r="AA94" s="95">
         <v>6</v>
       </c>
-      <c r="AB94" s="93"/>
-      <c r="AC94" s="91">
+      <c r="AB94" s="97"/>
+      <c r="AC94" s="95">
         <v>5</v>
       </c>
-      <c r="AD94" s="93"/>
-      <c r="AE94" s="91">
+      <c r="AD94" s="97"/>
+      <c r="AE94" s="95">
         <v>4</v>
       </c>
-      <c r="AF94" s="93"/>
-      <c r="AG94" s="91">
+      <c r="AF94" s="97"/>
+      <c r="AG94" s="95">
         <v>3</v>
       </c>
-      <c r="AH94" s="93"/>
-      <c r="AI94" s="91">
+      <c r="AH94" s="97"/>
+      <c r="AI94" s="95">
         <v>2</v>
       </c>
-      <c r="AJ94" s="93"/>
-      <c r="AK94" s="91">
+      <c r="AJ94" s="97"/>
+      <c r="AK94" s="95">
         <v>1</v>
       </c>
-      <c r="AL94" s="93"/>
-      <c r="AM94" s="91">
+      <c r="AL94" s="97"/>
+      <c r="AM94" s="95">
         <v>0</v>
       </c>
-      <c r="AN94" s="93"/>
+      <c r="AN94" s="97"/>
       <c r="AO94" s="69"/>
       <c r="AP94" s="69"/>
       <c r="AQ94" s="69"/>
@@ -5629,72 +5663,72 @@
       <c r="D103" s="69"/>
       <c r="E103" s="69"/>
       <c r="F103" s="69"/>
-      <c r="G103" s="94">
+      <c r="G103" s="92">
         <v>7</v>
       </c>
-      <c r="H103" s="96"/>
-      <c r="I103" s="94">
+      <c r="H103" s="94"/>
+      <c r="I103" s="92">
         <v>6</v>
       </c>
-      <c r="J103" s="96"/>
-      <c r="K103" s="94">
+      <c r="J103" s="94"/>
+      <c r="K103" s="92">
         <v>5</v>
       </c>
-      <c r="L103" s="96"/>
-      <c r="M103" s="94">
+      <c r="L103" s="94"/>
+      <c r="M103" s="92">
         <v>4</v>
       </c>
-      <c r="N103" s="96"/>
-      <c r="O103" s="94">
+      <c r="N103" s="94"/>
+      <c r="O103" s="92">
         <v>3</v>
       </c>
-      <c r="P103" s="96"/>
-      <c r="Q103" s="94">
+      <c r="P103" s="94"/>
+      <c r="Q103" s="92">
         <v>2</v>
       </c>
-      <c r="R103" s="96"/>
-      <c r="S103" s="94">
+      <c r="R103" s="94"/>
+      <c r="S103" s="92">
         <v>1</v>
       </c>
-      <c r="T103" s="96"/>
-      <c r="U103" s="94">
+      <c r="T103" s="94"/>
+      <c r="U103" s="92">
         <v>0</v>
       </c>
-      <c r="V103" s="96"/>
+      <c r="V103" s="94"/>
       <c r="W103" s="69"/>
       <c r="X103" s="69"/>
-      <c r="Y103" s="94">
+      <c r="Y103" s="92">
         <v>7</v>
       </c>
-      <c r="Z103" s="96"/>
-      <c r="AA103" s="94">
+      <c r="Z103" s="94"/>
+      <c r="AA103" s="92">
         <v>6</v>
       </c>
-      <c r="AB103" s="96"/>
-      <c r="AC103" s="94">
+      <c r="AB103" s="94"/>
+      <c r="AC103" s="92">
         <v>5</v>
       </c>
-      <c r="AD103" s="96"/>
-      <c r="AE103" s="94">
+      <c r="AD103" s="94"/>
+      <c r="AE103" s="92">
         <v>4</v>
       </c>
-      <c r="AF103" s="96"/>
-      <c r="AG103" s="94">
+      <c r="AF103" s="94"/>
+      <c r="AG103" s="92">
         <v>3</v>
       </c>
-      <c r="AH103" s="96"/>
-      <c r="AI103" s="94">
+      <c r="AH103" s="94"/>
+      <c r="AI103" s="92">
         <v>2</v>
       </c>
-      <c r="AJ103" s="96"/>
-      <c r="AK103" s="94">
+      <c r="AJ103" s="94"/>
+      <c r="AK103" s="92">
         <v>1</v>
       </c>
-      <c r="AL103" s="96"/>
-      <c r="AM103" s="94">
+      <c r="AL103" s="94"/>
+      <c r="AM103" s="92">
         <v>0</v>
       </c>
-      <c r="AN103" s="96"/>
+      <c r="AN103" s="94"/>
       <c r="AO103" s="69"/>
       <c r="AP103" s="69"/>
       <c r="AQ103" s="69"/>
@@ -5710,72 +5744,72 @@
       <c r="E105" s="69"/>
       <c r="F105" s="69"/>
       <c r="G105" s="69"/>
-      <c r="H105" s="91">
+      <c r="H105" s="95">
         <v>7</v>
       </c>
-      <c r="I105" s="93"/>
-      <c r="J105" s="91">
+      <c r="I105" s="97"/>
+      <c r="J105" s="95">
         <v>6</v>
       </c>
-      <c r="K105" s="93"/>
-      <c r="L105" s="91">
+      <c r="K105" s="97"/>
+      <c r="L105" s="95">
         <v>5</v>
       </c>
-      <c r="M105" s="93"/>
-      <c r="N105" s="91">
+      <c r="M105" s="97"/>
+      <c r="N105" s="95">
         <v>4</v>
       </c>
-      <c r="O105" s="93"/>
-      <c r="P105" s="91">
+      <c r="O105" s="97"/>
+      <c r="P105" s="95">
         <v>3</v>
       </c>
-      <c r="Q105" s="93"/>
-      <c r="R105" s="91">
+      <c r="Q105" s="97"/>
+      <c r="R105" s="95">
         <v>2</v>
       </c>
-      <c r="S105" s="93"/>
-      <c r="T105" s="91">
+      <c r="S105" s="97"/>
+      <c r="T105" s="95">
         <v>1</v>
       </c>
-      <c r="U105" s="93"/>
-      <c r="V105" s="91">
+      <c r="U105" s="97"/>
+      <c r="V105" s="95">
         <v>0</v>
       </c>
-      <c r="W105" s="93"/>
+      <c r="W105" s="97"/>
       <c r="X105" s="69"/>
       <c r="Y105" s="69"/>
-      <c r="Z105" s="91">
+      <c r="Z105" s="95">
         <v>7</v>
       </c>
-      <c r="AA105" s="93"/>
-      <c r="AB105" s="91">
+      <c r="AA105" s="97"/>
+      <c r="AB105" s="95">
         <v>6</v>
       </c>
-      <c r="AC105" s="93"/>
-      <c r="AD105" s="91">
+      <c r="AC105" s="97"/>
+      <c r="AD105" s="95">
         <v>5</v>
       </c>
-      <c r="AE105" s="93"/>
-      <c r="AF105" s="91">
+      <c r="AE105" s="97"/>
+      <c r="AF105" s="95">
         <v>4</v>
       </c>
-      <c r="AG105" s="93"/>
-      <c r="AH105" s="91">
+      <c r="AG105" s="97"/>
+      <c r="AH105" s="95">
         <v>3</v>
       </c>
-      <c r="AI105" s="93"/>
-      <c r="AJ105" s="91">
+      <c r="AI105" s="97"/>
+      <c r="AJ105" s="95">
         <v>2</v>
       </c>
-      <c r="AK105" s="93"/>
-      <c r="AL105" s="91">
+      <c r="AK105" s="97"/>
+      <c r="AL105" s="95">
         <v>1</v>
       </c>
-      <c r="AM105" s="93"/>
-      <c r="AN105" s="91">
+      <c r="AM105" s="97"/>
+      <c r="AN105" s="95">
         <v>0</v>
       </c>
-      <c r="AO105" s="93"/>
+      <c r="AO105" s="97"/>
       <c r="AP105" s="69"/>
       <c r="AQ105" s="69"/>
       <c r="AR105" s="69"/>
@@ -5954,72 +5988,72 @@
       <c r="E114" s="69"/>
       <c r="F114" s="69"/>
       <c r="G114" s="69"/>
-      <c r="H114" s="94">
+      <c r="H114" s="92">
         <v>7</v>
       </c>
-      <c r="I114" s="96"/>
-      <c r="J114" s="94">
+      <c r="I114" s="94"/>
+      <c r="J114" s="92">
         <v>6</v>
       </c>
-      <c r="K114" s="96"/>
-      <c r="L114" s="94">
+      <c r="K114" s="94"/>
+      <c r="L114" s="92">
         <v>5</v>
       </c>
-      <c r="M114" s="96"/>
-      <c r="N114" s="94">
+      <c r="M114" s="94"/>
+      <c r="N114" s="92">
         <v>4</v>
       </c>
-      <c r="O114" s="96"/>
-      <c r="P114" s="94">
+      <c r="O114" s="94"/>
+      <c r="P114" s="92">
         <v>3</v>
       </c>
-      <c r="Q114" s="96"/>
-      <c r="R114" s="94">
+      <c r="Q114" s="94"/>
+      <c r="R114" s="92">
         <v>2</v>
       </c>
-      <c r="S114" s="96"/>
-      <c r="T114" s="94">
+      <c r="S114" s="94"/>
+      <c r="T114" s="92">
         <v>1</v>
       </c>
-      <c r="U114" s="96"/>
-      <c r="V114" s="94">
+      <c r="U114" s="94"/>
+      <c r="V114" s="92">
         <v>0</v>
       </c>
-      <c r="W114" s="96"/>
+      <c r="W114" s="94"/>
       <c r="X114" s="69"/>
       <c r="Y114" s="69"/>
-      <c r="Z114" s="94">
+      <c r="Z114" s="92">
         <v>7</v>
       </c>
-      <c r="AA114" s="96"/>
-      <c r="AB114" s="94">
+      <c r="AA114" s="94"/>
+      <c r="AB114" s="92">
         <v>6</v>
       </c>
-      <c r="AC114" s="96"/>
-      <c r="AD114" s="94">
+      <c r="AC114" s="94"/>
+      <c r="AD114" s="92">
         <v>5</v>
       </c>
-      <c r="AE114" s="96"/>
-      <c r="AF114" s="94">
+      <c r="AE114" s="94"/>
+      <c r="AF114" s="92">
         <v>4</v>
       </c>
-      <c r="AG114" s="96"/>
-      <c r="AH114" s="94">
+      <c r="AG114" s="94"/>
+      <c r="AH114" s="92">
         <v>3</v>
       </c>
-      <c r="AI114" s="96"/>
-      <c r="AJ114" s="94">
+      <c r="AI114" s="94"/>
+      <c r="AJ114" s="92">
         <v>2</v>
       </c>
-      <c r="AK114" s="96"/>
-      <c r="AL114" s="94">
+      <c r="AK114" s="94"/>
+      <c r="AL114" s="92">
         <v>1</v>
       </c>
-      <c r="AM114" s="96"/>
-      <c r="AN114" s="94">
+      <c r="AM114" s="94"/>
+      <c r="AN114" s="92">
         <v>0</v>
       </c>
-      <c r="AO114" s="96"/>
+      <c r="AO114" s="94"/>
       <c r="AP114" s="69"/>
       <c r="AQ114" s="69"/>
       <c r="AR114" s="69"/>
@@ -6033,72 +6067,72 @@
       <c r="D116" s="69"/>
       <c r="E116" s="69"/>
       <c r="F116" s="69"/>
-      <c r="G116" s="91">
+      <c r="G116" s="95">
         <v>7</v>
       </c>
-      <c r="H116" s="93"/>
-      <c r="I116" s="91">
+      <c r="H116" s="97"/>
+      <c r="I116" s="95">
         <v>6</v>
       </c>
-      <c r="J116" s="93"/>
-      <c r="K116" s="91">
+      <c r="J116" s="97"/>
+      <c r="K116" s="95">
         <v>5</v>
       </c>
-      <c r="L116" s="93"/>
-      <c r="M116" s="91">
+      <c r="L116" s="97"/>
+      <c r="M116" s="95">
         <v>4</v>
       </c>
-      <c r="N116" s="93"/>
-      <c r="O116" s="91">
+      <c r="N116" s="97"/>
+      <c r="O116" s="95">
         <v>3</v>
       </c>
-      <c r="P116" s="93"/>
-      <c r="Q116" s="91">
+      <c r="P116" s="97"/>
+      <c r="Q116" s="95">
         <v>2</v>
       </c>
-      <c r="R116" s="93"/>
-      <c r="S116" s="91">
+      <c r="R116" s="97"/>
+      <c r="S116" s="95">
         <v>1</v>
       </c>
-      <c r="T116" s="93"/>
-      <c r="U116" s="91">
+      <c r="T116" s="97"/>
+      <c r="U116" s="95">
         <v>0</v>
       </c>
-      <c r="V116" s="93"/>
+      <c r="V116" s="97"/>
       <c r="W116" s="69"/>
       <c r="X116" s="69"/>
-      <c r="Y116" s="91">
+      <c r="Y116" s="95">
         <v>7</v>
       </c>
-      <c r="Z116" s="93"/>
-      <c r="AA116" s="91">
+      <c r="Z116" s="97"/>
+      <c r="AA116" s="95">
         <v>6</v>
       </c>
-      <c r="AB116" s="93"/>
-      <c r="AC116" s="91">
+      <c r="AB116" s="97"/>
+      <c r="AC116" s="95">
         <v>5</v>
       </c>
-      <c r="AD116" s="93"/>
-      <c r="AE116" s="91">
+      <c r="AD116" s="97"/>
+      <c r="AE116" s="95">
         <v>4</v>
       </c>
-      <c r="AF116" s="93"/>
-      <c r="AG116" s="91">
+      <c r="AF116" s="97"/>
+      <c r="AG116" s="95">
         <v>3</v>
       </c>
-      <c r="AH116" s="93"/>
-      <c r="AI116" s="91">
+      <c r="AH116" s="97"/>
+      <c r="AI116" s="95">
         <v>2</v>
       </c>
-      <c r="AJ116" s="93"/>
-      <c r="AK116" s="91">
+      <c r="AJ116" s="97"/>
+      <c r="AK116" s="95">
         <v>1</v>
       </c>
-      <c r="AL116" s="93"/>
-      <c r="AM116" s="91">
+      <c r="AL116" s="97"/>
+      <c r="AM116" s="95">
         <v>0</v>
       </c>
-      <c r="AN116" s="93"/>
+      <c r="AN116" s="97"/>
       <c r="AO116" s="69"/>
       <c r="AP116" s="69"/>
       <c r="AQ116" s="69"/>
@@ -6108,17 +6142,263 @@
     </row>
   </sheetData>
   <mergeCells count="292">
-    <mergeCell ref="BG24:BH24"/>
-    <mergeCell ref="BE24:BF24"/>
-    <mergeCell ref="BC24:BD24"/>
-    <mergeCell ref="AS16:BI16"/>
-    <mergeCell ref="AA34:AQ34"/>
-    <mergeCell ref="AE24:AF24"/>
-    <mergeCell ref="AG24:AH24"/>
-    <mergeCell ref="AI24:AJ24"/>
-    <mergeCell ref="AK24:AL24"/>
-    <mergeCell ref="AM24:AN24"/>
-    <mergeCell ref="AO24:AP24"/>
+    <mergeCell ref="AS53:BI53"/>
+    <mergeCell ref="Y62:AN62"/>
+    <mergeCell ref="BK16:BL16"/>
+    <mergeCell ref="BK51:BL51"/>
+    <mergeCell ref="BK68:BL68"/>
+    <mergeCell ref="D68:X68"/>
+    <mergeCell ref="D34:Z34"/>
+    <mergeCell ref="AR34:AS34"/>
+    <mergeCell ref="F51:X51"/>
+    <mergeCell ref="D16:Z16"/>
+    <mergeCell ref="BE41:BF41"/>
+    <mergeCell ref="BG41:BH41"/>
+    <mergeCell ref="AY41:AZ41"/>
+    <mergeCell ref="BA41:BB41"/>
+    <mergeCell ref="BC41:BD41"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="AY58:AZ58"/>
+    <mergeCell ref="BA58:BB58"/>
+    <mergeCell ref="BC58:BD58"/>
+    <mergeCell ref="BE58:BF58"/>
+    <mergeCell ref="BG58:BH58"/>
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="AI116:AJ116"/>
+    <mergeCell ref="AK116:AL116"/>
+    <mergeCell ref="AM116:AN116"/>
+    <mergeCell ref="U116:V116"/>
+    <mergeCell ref="Y116:Z116"/>
+    <mergeCell ref="AA116:AB116"/>
+    <mergeCell ref="AC116:AD116"/>
+    <mergeCell ref="AE116:AF116"/>
+    <mergeCell ref="AG116:AH116"/>
+    <mergeCell ref="AJ105:AK105"/>
+    <mergeCell ref="AL105:AM105"/>
+    <mergeCell ref="AN105:AO105"/>
+    <mergeCell ref="AB105:AC105"/>
+    <mergeCell ref="AD105:AE105"/>
+    <mergeCell ref="AF105:AG105"/>
+    <mergeCell ref="AH105:AI105"/>
+    <mergeCell ref="AI94:AJ94"/>
+    <mergeCell ref="AK94:AL94"/>
+    <mergeCell ref="AM94:AN94"/>
+    <mergeCell ref="U94:V94"/>
+    <mergeCell ref="AA53:AQ53"/>
+    <mergeCell ref="AN83:AO83"/>
+    <mergeCell ref="V83:W83"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="I116:J116"/>
+    <mergeCell ref="K116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="O116:P116"/>
+    <mergeCell ref="Q116:R116"/>
+    <mergeCell ref="S116:T116"/>
+    <mergeCell ref="V105:W105"/>
+    <mergeCell ref="Z105:AA105"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="L105:M105"/>
+    <mergeCell ref="N105:O105"/>
+    <mergeCell ref="P105:Q105"/>
+    <mergeCell ref="R105:S105"/>
+    <mergeCell ref="T105:U105"/>
+    <mergeCell ref="R114:S114"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="L114:M114"/>
+    <mergeCell ref="N114:O114"/>
+    <mergeCell ref="P114:Q114"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="K94:L94"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="O94:P94"/>
+    <mergeCell ref="Q94:R94"/>
+    <mergeCell ref="S94:T94"/>
+    <mergeCell ref="P83:Q83"/>
+    <mergeCell ref="R83:S83"/>
+    <mergeCell ref="T83:U83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="L83:M83"/>
+    <mergeCell ref="N83:O83"/>
+    <mergeCell ref="AN114:AO114"/>
+    <mergeCell ref="T114:U114"/>
+    <mergeCell ref="V114:W114"/>
+    <mergeCell ref="Z114:AA114"/>
+    <mergeCell ref="AB114:AC114"/>
+    <mergeCell ref="AD114:AE114"/>
+    <mergeCell ref="AF114:AG114"/>
+    <mergeCell ref="AH92:AI92"/>
+    <mergeCell ref="AJ92:AK92"/>
+    <mergeCell ref="AL92:AM92"/>
+    <mergeCell ref="AN92:AO92"/>
+    <mergeCell ref="Y94:Z94"/>
+    <mergeCell ref="AA94:AB94"/>
+    <mergeCell ref="AC94:AD94"/>
+    <mergeCell ref="AE94:AF94"/>
+    <mergeCell ref="AG94:AH94"/>
+    <mergeCell ref="AI103:AJ103"/>
+    <mergeCell ref="AK103:AL103"/>
+    <mergeCell ref="AH114:AI114"/>
+    <mergeCell ref="AJ114:AK114"/>
+    <mergeCell ref="AL114:AM114"/>
+    <mergeCell ref="AL83:AM83"/>
+    <mergeCell ref="U103:V103"/>
+    <mergeCell ref="Y103:Z103"/>
+    <mergeCell ref="AA103:AB103"/>
+    <mergeCell ref="AC103:AD103"/>
+    <mergeCell ref="AE103:AF103"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:W92"/>
+    <mergeCell ref="Z92:AA92"/>
+    <mergeCell ref="AB92:AC92"/>
+    <mergeCell ref="AD92:AE92"/>
+    <mergeCell ref="AF92:AG92"/>
+    <mergeCell ref="AG103:AH103"/>
+    <mergeCell ref="Z83:AA83"/>
+    <mergeCell ref="AB83:AC83"/>
+    <mergeCell ref="AD83:AE83"/>
+    <mergeCell ref="AF83:AG83"/>
+    <mergeCell ref="AH83:AI83"/>
+    <mergeCell ref="AJ83:AK83"/>
+    <mergeCell ref="AG81:AH81"/>
+    <mergeCell ref="AI81:AJ81"/>
+    <mergeCell ref="AK81:AL81"/>
+    <mergeCell ref="AM81:AN81"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="I103:J103"/>
+    <mergeCell ref="K103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="O103:P103"/>
+    <mergeCell ref="Q103:R103"/>
+    <mergeCell ref="S81:T81"/>
+    <mergeCell ref="U81:V81"/>
+    <mergeCell ref="Y81:Z81"/>
+    <mergeCell ref="AA81:AB81"/>
+    <mergeCell ref="AC81:AD81"/>
+    <mergeCell ref="AE81:AF81"/>
+    <mergeCell ref="AM103:AN103"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="L92:M92"/>
+    <mergeCell ref="N92:O92"/>
+    <mergeCell ref="P92:Q92"/>
+    <mergeCell ref="R92:S92"/>
+    <mergeCell ref="S103:T103"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="M81:N81"/>
+    <mergeCell ref="O81:P81"/>
+    <mergeCell ref="Q81:R81"/>
+    <mergeCell ref="AS41:AT41"/>
+    <mergeCell ref="AU41:AV41"/>
+    <mergeCell ref="AW41:AX41"/>
+    <mergeCell ref="AG41:AH41"/>
+    <mergeCell ref="AI41:AJ41"/>
+    <mergeCell ref="AK41:AL41"/>
+    <mergeCell ref="AM41:AN41"/>
+    <mergeCell ref="AO41:AP41"/>
+    <mergeCell ref="AQ41:AR41"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="W41:X41"/>
+    <mergeCell ref="Y41:Z41"/>
+    <mergeCell ref="AA41:AB41"/>
+    <mergeCell ref="AC41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="AK58:AL58"/>
+    <mergeCell ref="AM58:AN58"/>
+    <mergeCell ref="AO58:AP58"/>
+    <mergeCell ref="AQ58:AR58"/>
+    <mergeCell ref="AS58:AT58"/>
+    <mergeCell ref="AU58:AV58"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="BI41:BK41"/>
+    <mergeCell ref="G45:P45"/>
+    <mergeCell ref="Q45:T45"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="W45:X45"/>
+    <mergeCell ref="Y45:AN45"/>
+    <mergeCell ref="AO45:AP45"/>
+    <mergeCell ref="AQ45:BF45"/>
+    <mergeCell ref="G28:P28"/>
+    <mergeCell ref="Q28:T28"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="Y28:AN28"/>
+    <mergeCell ref="AO28:AP28"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="AA24:AB24"/>
+    <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="BG10:BH10"/>
+    <mergeCell ref="Y10:AN10"/>
+    <mergeCell ref="AQ10:BF10"/>
+    <mergeCell ref="G10:P10"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="AO10:AP10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="AA16:AQ16"/>
+    <mergeCell ref="BJ6:BL6"/>
+    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AS6:AT6"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AW6:AX6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="G62:P62"/>
+    <mergeCell ref="Q62:T62"/>
+    <mergeCell ref="U62:V62"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="O58:P58"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="S58:T58"/>
+    <mergeCell ref="U58:V58"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
     <mergeCell ref="AA70:AQ70"/>
     <mergeCell ref="AS70:BI70"/>
     <mergeCell ref="AA36:AQ36"/>
@@ -6143,263 +6423,17 @@
     <mergeCell ref="AY24:AZ24"/>
     <mergeCell ref="AW24:AX24"/>
     <mergeCell ref="AU24:AV24"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="G62:P62"/>
-    <mergeCell ref="Q62:T62"/>
-    <mergeCell ref="U62:V62"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="O58:P58"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="S58:T58"/>
-    <mergeCell ref="U58:V58"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="BJ6:BL6"/>
-    <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AS6:AT6"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AW6:AX6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="AA24:AB24"/>
-    <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="BG10:BH10"/>
-    <mergeCell ref="Y10:AN10"/>
-    <mergeCell ref="AQ10:BF10"/>
-    <mergeCell ref="G10:P10"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="AO10:AP10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AA16:AQ16"/>
-    <mergeCell ref="AK58:AL58"/>
-    <mergeCell ref="AM58:AN58"/>
-    <mergeCell ref="AO58:AP58"/>
-    <mergeCell ref="AQ58:AR58"/>
-    <mergeCell ref="AS58:AT58"/>
-    <mergeCell ref="AU58:AV58"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="BI41:BK41"/>
-    <mergeCell ref="G45:P45"/>
-    <mergeCell ref="Q45:T45"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="W45:X45"/>
-    <mergeCell ref="Y45:AN45"/>
-    <mergeCell ref="AO45:AP45"/>
-    <mergeCell ref="AQ45:BF45"/>
-    <mergeCell ref="G28:P28"/>
-    <mergeCell ref="Q28:T28"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="Y28:AN28"/>
-    <mergeCell ref="AO28:AP28"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="K81:L81"/>
-    <mergeCell ref="M81:N81"/>
-    <mergeCell ref="O81:P81"/>
-    <mergeCell ref="Q81:R81"/>
-    <mergeCell ref="AS41:AT41"/>
-    <mergeCell ref="AU41:AV41"/>
-    <mergeCell ref="AW41:AX41"/>
-    <mergeCell ref="AG41:AH41"/>
-    <mergeCell ref="AI41:AJ41"/>
-    <mergeCell ref="AK41:AL41"/>
-    <mergeCell ref="AM41:AN41"/>
-    <mergeCell ref="AO41:AP41"/>
-    <mergeCell ref="AQ41:AR41"/>
-    <mergeCell ref="U41:V41"/>
-    <mergeCell ref="W41:X41"/>
-    <mergeCell ref="Y41:Z41"/>
-    <mergeCell ref="AA41:AB41"/>
-    <mergeCell ref="AC41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="AG81:AH81"/>
-    <mergeCell ref="AI81:AJ81"/>
-    <mergeCell ref="AK81:AL81"/>
-    <mergeCell ref="AM81:AN81"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="I103:J103"/>
-    <mergeCell ref="K103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="O103:P103"/>
-    <mergeCell ref="Q103:R103"/>
-    <mergeCell ref="S81:T81"/>
-    <mergeCell ref="U81:V81"/>
-    <mergeCell ref="Y81:Z81"/>
-    <mergeCell ref="AA81:AB81"/>
-    <mergeCell ref="AC81:AD81"/>
-    <mergeCell ref="AE81:AF81"/>
-    <mergeCell ref="AM103:AN103"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="L92:M92"/>
-    <mergeCell ref="N92:O92"/>
-    <mergeCell ref="P92:Q92"/>
-    <mergeCell ref="R92:S92"/>
-    <mergeCell ref="S103:T103"/>
-    <mergeCell ref="AL83:AM83"/>
-    <mergeCell ref="U103:V103"/>
-    <mergeCell ref="Y103:Z103"/>
-    <mergeCell ref="AA103:AB103"/>
-    <mergeCell ref="AC103:AD103"/>
-    <mergeCell ref="AE103:AF103"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:W92"/>
-    <mergeCell ref="Z92:AA92"/>
-    <mergeCell ref="AB92:AC92"/>
-    <mergeCell ref="AD92:AE92"/>
-    <mergeCell ref="AF92:AG92"/>
-    <mergeCell ref="AG103:AH103"/>
-    <mergeCell ref="Z83:AA83"/>
-    <mergeCell ref="AB83:AC83"/>
-    <mergeCell ref="AD83:AE83"/>
-    <mergeCell ref="AF83:AG83"/>
-    <mergeCell ref="AH83:AI83"/>
-    <mergeCell ref="AN114:AO114"/>
-    <mergeCell ref="T114:U114"/>
-    <mergeCell ref="V114:W114"/>
-    <mergeCell ref="Z114:AA114"/>
-    <mergeCell ref="AB114:AC114"/>
-    <mergeCell ref="AD114:AE114"/>
-    <mergeCell ref="AF114:AG114"/>
-    <mergeCell ref="AH92:AI92"/>
-    <mergeCell ref="AJ92:AK92"/>
-    <mergeCell ref="AL92:AM92"/>
-    <mergeCell ref="AN92:AO92"/>
-    <mergeCell ref="Y94:Z94"/>
-    <mergeCell ref="AA94:AB94"/>
-    <mergeCell ref="AC94:AD94"/>
-    <mergeCell ref="AE94:AF94"/>
-    <mergeCell ref="AG94:AH94"/>
-    <mergeCell ref="AI103:AJ103"/>
-    <mergeCell ref="AK103:AL103"/>
-    <mergeCell ref="AH114:AI114"/>
-    <mergeCell ref="AJ114:AK114"/>
-    <mergeCell ref="AL114:AM114"/>
-    <mergeCell ref="AJ83:AK83"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="I94:J94"/>
-    <mergeCell ref="K94:L94"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="O94:P94"/>
-    <mergeCell ref="Q94:R94"/>
-    <mergeCell ref="S94:T94"/>
-    <mergeCell ref="P83:Q83"/>
-    <mergeCell ref="R83:S83"/>
-    <mergeCell ref="T83:U83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="L83:M83"/>
-    <mergeCell ref="N83:O83"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="I116:J116"/>
-    <mergeCell ref="K116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="O116:P116"/>
-    <mergeCell ref="Q116:R116"/>
-    <mergeCell ref="S116:T116"/>
-    <mergeCell ref="V105:W105"/>
-    <mergeCell ref="Z105:AA105"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="L105:M105"/>
-    <mergeCell ref="N105:O105"/>
-    <mergeCell ref="P105:Q105"/>
-    <mergeCell ref="R105:S105"/>
-    <mergeCell ref="T105:U105"/>
-    <mergeCell ref="R114:S114"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="L114:M114"/>
-    <mergeCell ref="N114:O114"/>
-    <mergeCell ref="P114:Q114"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="AI116:AJ116"/>
-    <mergeCell ref="AK116:AL116"/>
-    <mergeCell ref="AM116:AN116"/>
-    <mergeCell ref="U116:V116"/>
-    <mergeCell ref="Y116:Z116"/>
-    <mergeCell ref="AA116:AB116"/>
-    <mergeCell ref="AC116:AD116"/>
-    <mergeCell ref="AE116:AF116"/>
-    <mergeCell ref="AG116:AH116"/>
-    <mergeCell ref="AJ105:AK105"/>
-    <mergeCell ref="AL105:AM105"/>
-    <mergeCell ref="AN105:AO105"/>
-    <mergeCell ref="AB105:AC105"/>
-    <mergeCell ref="AD105:AE105"/>
-    <mergeCell ref="AF105:AG105"/>
-    <mergeCell ref="AH105:AI105"/>
-    <mergeCell ref="AI94:AJ94"/>
-    <mergeCell ref="AK94:AL94"/>
-    <mergeCell ref="AM94:AN94"/>
-    <mergeCell ref="U94:V94"/>
-    <mergeCell ref="AA53:AQ53"/>
-    <mergeCell ref="AN83:AO83"/>
-    <mergeCell ref="V83:W83"/>
-    <mergeCell ref="AS53:BI53"/>
-    <mergeCell ref="Y62:AN62"/>
-    <mergeCell ref="BK16:BL16"/>
-    <mergeCell ref="BK51:BL51"/>
-    <mergeCell ref="BK68:BL68"/>
-    <mergeCell ref="D68:X68"/>
-    <mergeCell ref="D34:Z34"/>
-    <mergeCell ref="AR34:AS34"/>
-    <mergeCell ref="F51:X51"/>
-    <mergeCell ref="D16:Z16"/>
-    <mergeCell ref="BE41:BF41"/>
-    <mergeCell ref="BG41:BH41"/>
-    <mergeCell ref="AY41:AZ41"/>
-    <mergeCell ref="BA41:BB41"/>
-    <mergeCell ref="BC41:BD41"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="AY58:AZ58"/>
-    <mergeCell ref="BA58:BB58"/>
-    <mergeCell ref="BC58:BD58"/>
-    <mergeCell ref="BE58:BF58"/>
-    <mergeCell ref="BG58:BH58"/>
+    <mergeCell ref="BG24:BH24"/>
+    <mergeCell ref="BE24:BF24"/>
+    <mergeCell ref="BC24:BD24"/>
+    <mergeCell ref="AS16:BI16"/>
+    <mergeCell ref="AA34:AQ34"/>
+    <mergeCell ref="AE24:AF24"/>
+    <mergeCell ref="AG24:AH24"/>
+    <mergeCell ref="AI24:AJ24"/>
+    <mergeCell ref="AK24:AL24"/>
+    <mergeCell ref="AM24:AN24"/>
+    <mergeCell ref="AO24:AP24"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pin name etc change
</commit_message>
<xml_diff>
--- a/I2C2SPI.xlsx
+++ b/I2C2SPI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="-15" windowWidth="13785" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="345" yWindow="-15" windowWidth="13785" windowHeight="7020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pin assign" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="175">
   <si>
     <t>IO11</t>
   </si>
@@ -687,6 +687,66 @@
   <si>
     <t>Bidirectional SO support for reading
 0x85:read by SI, 0x75:read by SO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[7:0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xB2
+0x3D
+0xDF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x42
+0x43
+0x44</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GPIO2/SS2, GPIO3/SS3 pin funtion select
+0xB2,0x3D,0xDF: GPIO2, GPIO3
+0xCF,0x3F,0xDF: SS2, GPIO3
+0xB2,0x0D,0xFD: GPIO2, SS3
+0xCF,0x0F,0xFD: SS2, SS3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SDI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SDO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I2CSPI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I2CSPI-A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SLA0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SLA1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GPIO2/SS2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GPIO3/SS3</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1106,7 +1166,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1380,6 +1440,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1389,47 +1464,38 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1743,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N23"/>
+  <dimension ref="A2:N36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
@@ -1762,531 +1828,956 @@
     <col min="9" max="9" width="8.875" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.25" style="6" customWidth="1"/>
+    <col min="12" max="12" width="11.125" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.125" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="B2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="F2"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="91"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="F3"/>
+      <c r="L3" s="91"/>
+      <c r="N3" s="91"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="91"/>
+      <c r="B4" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="F4"/>
+      <c r="L4" s="91"/>
+      <c r="N4" s="91"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
-      <c r="B4" s="9" t="s">
+    <row r="6" spans="1:14">
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F6" s="11">
         <v>1</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11">
         <v>20</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="J6" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K6" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L6" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="15"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="B5" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="5">
-        <v>2</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5">
-        <v>19</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="L5" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="B6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="5">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="5">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="M6" s="14"/>
       <c r="N6" s="15"/>
     </row>
     <row r="7" spans="1:14">
       <c r="B7" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F7" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>77</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="B8" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>78</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>4</v>
+        <v>67</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F8" s="5">
-        <v>5</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>36</v>
+        <v>146</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="M8" s="14"/>
       <c r="N8" s="15"/>
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="16" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>7</v>
+        <v>78</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>5</v>
       </c>
       <c r="F9" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="16" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>6</v>
+        <v>78</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>4</v>
       </c>
       <c r="F10" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5">
-        <v>14</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="22" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="14"/>
+      <c r="N10" s="15"/>
     </row>
     <row r="11" spans="1:14">
       <c r="B11" s="16" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="F11" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J11" s="32" t="s">
         <v>148</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="M11" s="14"/>
-      <c r="N11" s="15"/>
+        <v>167</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="15"/>
       <c r="B12" s="16" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>77</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="F12" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5">
+        <v>14</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5">
+        <v>8</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
+        <v>13</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="M13" s="14"/>
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="5">
+        <v>9</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
         <v>12</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I14" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="32" t="s">
+      <c r="J14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L14" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
-      <c r="B13" s="24" t="s">
+    <row r="15" spans="1:14">
+      <c r="B15" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C15" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F15" s="27">
         <v>10</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27">
+      <c r="G15" s="27"/>
+      <c r="H15" s="27">
         <v>11</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I15" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="30" t="s">
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="F14"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="B15" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="I15" s="6"/>
-    </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="F16" s="36" t="s">
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="91"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="91"/>
+      <c r="N16" s="91"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="B17" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="F17"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="91"/>
+      <c r="B18" s="91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="91" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" s="91"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="91"/>
+      <c r="B19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11">
+        <v>20</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="M19" s="14"/>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="91"/>
+      <c r="B20" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5">
+        <v>19</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="N20" s="91"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="91"/>
+      <c r="B21" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="5">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="5">
+        <v>18</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="14"/>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="91"/>
+      <c r="B22" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="5">
+        <v>4</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5">
+        <v>17</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L22" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" s="91"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="91"/>
+      <c r="B23" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="5">
+        <v>5</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5">
+        <v>16</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="14"/>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="91"/>
+      <c r="B24" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="5">
+        <v>6</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5">
+        <v>15</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L24" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="N24" s="91"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="91"/>
+      <c r="B25" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="5">
+        <v>7</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5">
+        <v>14</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="N25" s="91"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="91"/>
+      <c r="B26" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="5">
+        <v>8</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5">
+        <v>13</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L26" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="M26" s="14"/>
+      <c r="N26" s="15"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="5">
+        <v>9</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5">
+        <v>12</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="N27" s="91"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="91"/>
+      <c r="B28" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="27">
+        <v>10</v>
+      </c>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27">
+        <v>11</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="91"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="91"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="F29"/>
+      <c r="I29" s="91"/>
+      <c r="L29" s="91"/>
+      <c r="N29" s="91"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="C30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="F31" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39" t="s">
+      <c r="G31" s="37"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="40"/>
-    </row>
-    <row r="17" spans="2:12" customFormat="1" ht="14.25" thickBot="1">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="F17" s="45" t="s">
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="40"/>
+    </row>
+    <row r="32" spans="1:14" ht="14.25" thickBot="1">
+      <c r="A32"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="F32" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G32" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="H32" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="46" t="s">
+      <c r="I32" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="45" t="s">
+      <c r="J32" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="K17" s="47"/>
-      <c r="L17" s="48" t="s">
+      <c r="K32" s="47"/>
+      <c r="L32" s="48" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" customFormat="1" ht="14.25" thickTop="1">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="F18" s="44" t="s">
+      <c r="N32"/>
+    </row>
+    <row r="33" spans="1:14" ht="14.25" thickTop="1">
+      <c r="A33"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="F33" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G33" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="H33" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="44" t="s">
+      <c r="I33" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="44">
+      <c r="J33" s="44">
         <v>1010100</v>
       </c>
-      <c r="K18" s="41" t="s">
+      <c r="K33" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="L18" s="42" t="str">
-        <f>BIN2HEX(J18,2)</f>
+      <c r="L33" s="42" t="str">
+        <f>BIN2HEX(J33,2)</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" customFormat="1">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="F19" s="34" t="s">
+      <c r="N33"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="F34" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G34" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H34" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I34" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J34" s="34">
         <v>1010101</v>
       </c>
-      <c r="K19" s="43" t="s">
+      <c r="K34" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="L19" s="38" t="str">
-        <f>BIN2HEX(J19,2)</f>
+      <c r="L34" s="38" t="str">
+        <f>BIN2HEX(J34,2)</f>
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="2:12">
-      <c r="F20" s="34" t="s">
+      <c r="N34"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="F35" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G35" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H35" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I35" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="34">
+      <c r="J35" s="34">
         <v>1010110</v>
       </c>
-      <c r="K20" s="43" t="s">
+      <c r="K35" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="L20" s="38" t="str">
-        <f>BIN2HEX(J20,2)</f>
+      <c r="L35" s="38" t="str">
+        <f>BIN2HEX(J35,2)</f>
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
-      <c r="F21" s="34" t="s">
+    <row r="36" spans="1:14">
+      <c r="F36" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="34" t="s">
+      <c r="G36" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="H36" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I36" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="J21" s="34">
+      <c r="J36" s="34">
         <v>1010111</v>
       </c>
-      <c r="K21" s="43" t="s">
+      <c r="K36" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="L21" s="38" t="str">
-        <f>BIN2HEX(J21,2)</f>
+      <c r="L36" s="38" t="str">
+        <f>BIN2HEX(J36,2)</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="2:12">
-      <c r="D23" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2297,10 +2788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H17"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2434,71 +2925,77 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="81">
-      <c r="B10" s="50" t="s">
+    <row r="10" spans="2:8" ht="67.5">
+      <c r="B10" s="109" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="109" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="81">
+      <c r="B11" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C11" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D11" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E11" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F11" s="49" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="81">
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="34" t="s">
+    <row r="12" spans="2:8" ht="81">
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F12" s="49" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="55" t="s">
+    <row r="13" spans="2:8">
+      <c r="B13" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C13" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D13" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E13" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="62" t="s">
+      <c r="F13" s="62" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="58"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="63" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" s="58"/>
       <c r="C14" s="60"/>
-      <c r="D14" s="58"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F14" s="63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -2506,10 +3003,10 @@
       <c r="C15" s="60"/>
       <c r="D15" s="58"/>
       <c r="E15" s="51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" s="63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -2517,20 +3014,31 @@
       <c r="C16" s="60"/>
       <c r="D16" s="58"/>
       <c r="E16" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="58"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="63" t="s">
+      <c r="F17" s="63" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="59"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="56" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" s="59"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F18" s="59" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2544,7 +3052,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:BL116"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="67" zoomScaleNormal="67" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="BZ19" sqref="BZ19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5"/>
   <cols>
@@ -2563,22 +3073,22 @@
       <c r="I4" t="s">
         <v>122</v>
       </c>
-      <c r="O4" s="99" t="s">
+      <c r="O4" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="100" t="s">
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="98" t="s">
+      <c r="S4" s="107"/>
+      <c r="T4" s="107"/>
+      <c r="U4" s="108" t="s">
         <v>152</v>
       </c>
-      <c r="V4" s="98"/>
-      <c r="W4" s="98"/>
-      <c r="X4" s="98"/>
+      <c r="V4" s="108"/>
+      <c r="W4" s="108"/>
+      <c r="X4" s="108"/>
     </row>
     <row r="5" spans="3:64">
       <c r="C5" s="71" t="s">
@@ -2586,124 +3096,124 @@
       </c>
     </row>
     <row r="6" spans="3:64">
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97">
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92">
         <v>1</v>
       </c>
-      <c r="H6" s="97"/>
-      <c r="I6" s="97">
+      <c r="H6" s="92"/>
+      <c r="I6" s="92">
         <v>2</v>
       </c>
-      <c r="J6" s="97"/>
-      <c r="K6" s="97">
+      <c r="J6" s="92"/>
+      <c r="K6" s="92">
         <v>3</v>
       </c>
-      <c r="L6" s="97"/>
-      <c r="M6" s="97">
+      <c r="L6" s="92"/>
+      <c r="M6" s="92">
         <v>4</v>
       </c>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97">
+      <c r="N6" s="92"/>
+      <c r="O6" s="92">
         <v>5</v>
       </c>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="97">
+      <c r="P6" s="92"/>
+      <c r="Q6" s="92">
         <v>6</v>
       </c>
-      <c r="R6" s="97"/>
-      <c r="S6" s="97">
+      <c r="R6" s="92"/>
+      <c r="S6" s="92">
         <v>7</v>
       </c>
-      <c r="T6" s="97"/>
-      <c r="U6" s="97">
+      <c r="T6" s="92"/>
+      <c r="U6" s="92">
         <v>8</v>
       </c>
-      <c r="V6" s="97"/>
-      <c r="W6" s="97" t="s">
+      <c r="V6" s="92"/>
+      <c r="W6" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="X6" s="97"/>
-      <c r="Y6" s="97">
+      <c r="X6" s="92"/>
+      <c r="Y6" s="92">
         <v>1</v>
       </c>
-      <c r="Z6" s="97"/>
-      <c r="AA6" s="97">
+      <c r="Z6" s="92"/>
+      <c r="AA6" s="92">
         <v>2</v>
       </c>
-      <c r="AB6" s="97"/>
-      <c r="AC6" s="97">
+      <c r="AB6" s="92"/>
+      <c r="AC6" s="92">
         <v>3</v>
       </c>
-      <c r="AD6" s="97"/>
-      <c r="AE6" s="97">
+      <c r="AD6" s="92"/>
+      <c r="AE6" s="92">
         <v>4</v>
       </c>
-      <c r="AF6" s="97"/>
-      <c r="AG6" s="97">
+      <c r="AF6" s="92"/>
+      <c r="AG6" s="92">
         <v>5</v>
       </c>
-      <c r="AH6" s="97"/>
-      <c r="AI6" s="97">
+      <c r="AH6" s="92"/>
+      <c r="AI6" s="92">
         <v>6</v>
       </c>
-      <c r="AJ6" s="97"/>
-      <c r="AK6" s="97">
+      <c r="AJ6" s="92"/>
+      <c r="AK6" s="92">
         <v>7</v>
       </c>
-      <c r="AL6" s="97"/>
-      <c r="AM6" s="97">
+      <c r="AL6" s="92"/>
+      <c r="AM6" s="92">
         <v>8</v>
       </c>
-      <c r="AN6" s="97"/>
-      <c r="AO6" s="97" t="s">
+      <c r="AN6" s="92"/>
+      <c r="AO6" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="AP6" s="97"/>
-      <c r="AQ6" s="97">
+      <c r="AP6" s="92"/>
+      <c r="AQ6" s="92">
         <v>1</v>
       </c>
-      <c r="AR6" s="97"/>
-      <c r="AS6" s="97">
+      <c r="AR6" s="92"/>
+      <c r="AS6" s="92">
         <v>2</v>
       </c>
-      <c r="AT6" s="97"/>
-      <c r="AU6" s="97">
+      <c r="AT6" s="92"/>
+      <c r="AU6" s="92">
         <v>3</v>
       </c>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97">
+      <c r="AV6" s="92"/>
+      <c r="AW6" s="92">
         <v>4</v>
       </c>
-      <c r="AX6" s="97"/>
-      <c r="AY6" s="97">
+      <c r="AX6" s="92"/>
+      <c r="AY6" s="92">
         <v>5</v>
       </c>
-      <c r="AZ6" s="97"/>
-      <c r="BA6" s="97">
+      <c r="AZ6" s="92"/>
+      <c r="BA6" s="92">
         <v>6</v>
       </c>
-      <c r="BB6" s="97"/>
-      <c r="BC6" s="97">
+      <c r="BB6" s="92"/>
+      <c r="BC6" s="92">
         <v>7</v>
       </c>
-      <c r="BD6" s="97"/>
-      <c r="BE6" s="97">
+      <c r="BD6" s="92"/>
+      <c r="BE6" s="92">
         <v>8</v>
       </c>
-      <c r="BF6" s="97"/>
-      <c r="BG6" s="97" t="s">
+      <c r="BF6" s="92"/>
+      <c r="BG6" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="BH6" s="97"/>
-      <c r="BJ6" s="97" t="s">
+      <c r="BH6" s="92"/>
+      <c r="BJ6" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="BK6" s="97"/>
-      <c r="BL6" s="97"/>
+      <c r="BK6" s="92"/>
+      <c r="BL6" s="92"/>
     </row>
     <row r="8" spans="3:64">
       <c r="C8" t="s">
@@ -2778,72 +3288,72 @@
       <c r="D10" s="78"/>
       <c r="E10" s="78"/>
       <c r="F10" s="79"/>
-      <c r="G10" s="91" t="s">
+      <c r="G10" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="92"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="92"/>
-      <c r="O10" s="92"/>
-      <c r="P10" s="93"/>
-      <c r="Q10" s="91" t="s">
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
+      <c r="N10" s="97"/>
+      <c r="O10" s="97"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="R10" s="92"/>
-      <c r="S10" s="92"/>
-      <c r="T10" s="93"/>
-      <c r="U10" s="91" t="s">
+      <c r="R10" s="97"/>
+      <c r="S10" s="97"/>
+      <c r="T10" s="98"/>
+      <c r="U10" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="V10" s="93"/>
+      <c r="V10" s="98"/>
       <c r="W10" s="101" t="s">
         <v>106</v>
       </c>
       <c r="X10" s="102"/>
-      <c r="Y10" s="91" t="s">
+      <c r="Y10" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="Z10" s="92"/>
-      <c r="AA10" s="92"/>
-      <c r="AB10" s="92"/>
-      <c r="AC10" s="92"/>
-      <c r="AD10" s="92"/>
-      <c r="AE10" s="92"/>
-      <c r="AF10" s="92"/>
-      <c r="AG10" s="92"/>
-      <c r="AH10" s="92"/>
-      <c r="AI10" s="92"/>
-      <c r="AJ10" s="92"/>
-      <c r="AK10" s="92"/>
-      <c r="AL10" s="92"/>
-      <c r="AM10" s="92"/>
-      <c r="AN10" s="93"/>
+      <c r="Z10" s="97"/>
+      <c r="AA10" s="97"/>
+      <c r="AB10" s="97"/>
+      <c r="AC10" s="97"/>
+      <c r="AD10" s="97"/>
+      <c r="AE10" s="97"/>
+      <c r="AF10" s="97"/>
+      <c r="AG10" s="97"/>
+      <c r="AH10" s="97"/>
+      <c r="AI10" s="97"/>
+      <c r="AJ10" s="97"/>
+      <c r="AK10" s="97"/>
+      <c r="AL10" s="97"/>
+      <c r="AM10" s="97"/>
+      <c r="AN10" s="98"/>
       <c r="AO10" s="101" t="s">
         <v>106</v>
       </c>
       <c r="AP10" s="102"/>
-      <c r="AQ10" s="91" t="s">
+      <c r="AQ10" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="AR10" s="92"/>
-      <c r="AS10" s="92"/>
-      <c r="AT10" s="92"/>
-      <c r="AU10" s="92"/>
-      <c r="AV10" s="92"/>
-      <c r="AW10" s="92"/>
-      <c r="AX10" s="92"/>
-      <c r="AY10" s="92"/>
-      <c r="AZ10" s="92"/>
-      <c r="BA10" s="92"/>
-      <c r="BB10" s="92"/>
-      <c r="BC10" s="92"/>
-      <c r="BD10" s="92"/>
-      <c r="BE10" s="92"/>
-      <c r="BF10" s="93"/>
+      <c r="AR10" s="97"/>
+      <c r="AS10" s="97"/>
+      <c r="AT10" s="97"/>
+      <c r="AU10" s="97"/>
+      <c r="AV10" s="97"/>
+      <c r="AW10" s="97"/>
+      <c r="AX10" s="97"/>
+      <c r="AY10" s="97"/>
+      <c r="AZ10" s="97"/>
+      <c r="BA10" s="97"/>
+      <c r="BB10" s="97"/>
+      <c r="BC10" s="97"/>
+      <c r="BD10" s="97"/>
+      <c r="BE10" s="97"/>
+      <c r="BF10" s="98"/>
       <c r="BG10" s="101" t="s">
         <v>106</v>
       </c>
@@ -2989,75 +3499,75 @@
       <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="95">
+      <c r="D16" s="94">
         <v>0</v>
       </c>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="95"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="95"/>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
-      <c r="P16" s="95"/>
-      <c r="Q16" s="95"/>
-      <c r="R16" s="95"/>
-      <c r="S16" s="95"/>
-      <c r="T16" s="95"/>
-      <c r="U16" s="95"/>
-      <c r="V16" s="95"/>
-      <c r="W16" s="95"/>
-      <c r="X16" s="95"/>
-      <c r="Y16" s="95"/>
-      <c r="Z16" s="96"/>
-      <c r="AA16" s="94" t="s">
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="94"/>
+      <c r="N16" s="94"/>
+      <c r="O16" s="94"/>
+      <c r="P16" s="94"/>
+      <c r="Q16" s="94"/>
+      <c r="R16" s="94"/>
+      <c r="S16" s="94"/>
+      <c r="T16" s="94"/>
+      <c r="U16" s="94"/>
+      <c r="V16" s="94"/>
+      <c r="W16" s="94"/>
+      <c r="X16" s="94"/>
+      <c r="Y16" s="94"/>
+      <c r="Z16" s="95"/>
+      <c r="AA16" s="93" t="s">
         <v>111</v>
       </c>
-      <c r="AB16" s="95"/>
-      <c r="AC16" s="95"/>
-      <c r="AD16" s="95"/>
-      <c r="AE16" s="95"/>
-      <c r="AF16" s="95"/>
-      <c r="AG16" s="95"/>
-      <c r="AH16" s="95"/>
-      <c r="AI16" s="95"/>
-      <c r="AJ16" s="95"/>
-      <c r="AK16" s="95"/>
-      <c r="AL16" s="95"/>
-      <c r="AM16" s="95"/>
-      <c r="AN16" s="95"/>
-      <c r="AO16" s="95"/>
-      <c r="AP16" s="95"/>
-      <c r="AQ16" s="96"/>
+      <c r="AB16" s="94"/>
+      <c r="AC16" s="94"/>
+      <c r="AD16" s="94"/>
+      <c r="AE16" s="94"/>
+      <c r="AF16" s="94"/>
+      <c r="AG16" s="94"/>
+      <c r="AH16" s="94"/>
+      <c r="AI16" s="94"/>
+      <c r="AJ16" s="94"/>
+      <c r="AK16" s="94"/>
+      <c r="AL16" s="94"/>
+      <c r="AM16" s="94"/>
+      <c r="AN16" s="94"/>
+      <c r="AO16" s="94"/>
+      <c r="AP16" s="94"/>
+      <c r="AQ16" s="95"/>
       <c r="AR16" s="77"/>
-      <c r="AS16" s="94" t="s">
+      <c r="AS16" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="AT16" s="95"/>
-      <c r="AU16" s="95"/>
-      <c r="AV16" s="95"/>
-      <c r="AW16" s="95"/>
-      <c r="AX16" s="95"/>
-      <c r="AY16" s="95"/>
-      <c r="AZ16" s="95"/>
-      <c r="BA16" s="95"/>
-      <c r="BB16" s="95"/>
-      <c r="BC16" s="95"/>
-      <c r="BD16" s="95"/>
-      <c r="BE16" s="95"/>
-      <c r="BF16" s="95"/>
-      <c r="BG16" s="95"/>
-      <c r="BH16" s="95"/>
-      <c r="BI16" s="96"/>
+      <c r="AT16" s="94"/>
+      <c r="AU16" s="94"/>
+      <c r="AV16" s="94"/>
+      <c r="AW16" s="94"/>
+      <c r="AX16" s="94"/>
+      <c r="AY16" s="94"/>
+      <c r="AZ16" s="94"/>
+      <c r="BA16" s="94"/>
+      <c r="BB16" s="94"/>
+      <c r="BC16" s="94"/>
+      <c r="BD16" s="94"/>
+      <c r="BE16" s="94"/>
+      <c r="BF16" s="94"/>
+      <c r="BG16" s="94"/>
+      <c r="BH16" s="94"/>
+      <c r="BI16" s="95"/>
       <c r="BJ16" s="77"/>
-      <c r="BK16" s="94">
+      <c r="BK16" s="93">
         <v>0</v>
       </c>
-      <c r="BL16" s="95"/>
+      <c r="BL16" s="94"/>
     </row>
     <row r="18" spans="3:64">
       <c r="C18" t="s">
@@ -3086,45 +3596,45 @@
       <c r="X18" s="74"/>
       <c r="Y18" s="74"/>
       <c r="Z18" s="74"/>
-      <c r="AA18" s="91" t="s">
+      <c r="AA18" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="AB18" s="92"/>
-      <c r="AC18" s="92"/>
-      <c r="AD18" s="92"/>
-      <c r="AE18" s="92"/>
-      <c r="AF18" s="92"/>
-      <c r="AG18" s="92"/>
-      <c r="AH18" s="92"/>
-      <c r="AI18" s="92"/>
-      <c r="AJ18" s="92"/>
-      <c r="AK18" s="92"/>
-      <c r="AL18" s="92"/>
-      <c r="AM18" s="92"/>
-      <c r="AN18" s="92"/>
-      <c r="AO18" s="92"/>
-      <c r="AP18" s="92"/>
-      <c r="AQ18" s="93"/>
+      <c r="AB18" s="97"/>
+      <c r="AC18" s="97"/>
+      <c r="AD18" s="97"/>
+      <c r="AE18" s="97"/>
+      <c r="AF18" s="97"/>
+      <c r="AG18" s="97"/>
+      <c r="AH18" s="97"/>
+      <c r="AI18" s="97"/>
+      <c r="AJ18" s="97"/>
+      <c r="AK18" s="97"/>
+      <c r="AL18" s="97"/>
+      <c r="AM18" s="97"/>
+      <c r="AN18" s="97"/>
+      <c r="AO18" s="97"/>
+      <c r="AP18" s="97"/>
+      <c r="AQ18" s="98"/>
       <c r="AR18" s="74"/>
-      <c r="AS18" s="91" t="s">
+      <c r="AS18" s="96" t="s">
         <v>131</v>
       </c>
-      <c r="AT18" s="92"/>
-      <c r="AU18" s="92"/>
-      <c r="AV18" s="92"/>
-      <c r="AW18" s="92"/>
-      <c r="AX18" s="92"/>
-      <c r="AY18" s="92"/>
-      <c r="AZ18" s="92"/>
-      <c r="BA18" s="92"/>
-      <c r="BB18" s="92"/>
-      <c r="BC18" s="92"/>
-      <c r="BD18" s="92"/>
-      <c r="BE18" s="92"/>
-      <c r="BF18" s="92"/>
-      <c r="BG18" s="92"/>
-      <c r="BH18" s="92"/>
-      <c r="BI18" s="93"/>
+      <c r="AT18" s="97"/>
+      <c r="AU18" s="97"/>
+      <c r="AV18" s="97"/>
+      <c r="AW18" s="97"/>
+      <c r="AX18" s="97"/>
+      <c r="AY18" s="97"/>
+      <c r="AZ18" s="97"/>
+      <c r="BA18" s="97"/>
+      <c r="BB18" s="97"/>
+      <c r="BC18" s="97"/>
+      <c r="BD18" s="97"/>
+      <c r="BE18" s="97"/>
+      <c r="BF18" s="97"/>
+      <c r="BG18" s="97"/>
+      <c r="BH18" s="97"/>
+      <c r="BI18" s="98"/>
       <c r="BJ18" s="74"/>
       <c r="BK18" s="89"/>
       <c r="BL18" s="88"/>
@@ -3133,67 +3643,67 @@
       <c r="C20" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="82"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="82"/>
-      <c r="R20" s="82"/>
-      <c r="S20" s="82"/>
-      <c r="T20" s="82"/>
-      <c r="U20" s="82"/>
-      <c r="V20" s="82"/>
-      <c r="W20" s="82"/>
-      <c r="X20" s="82"/>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="82"/>
-      <c r="AA20" s="82"/>
-      <c r="AB20" s="82"/>
-      <c r="AC20" s="82"/>
-      <c r="AD20" s="82"/>
-      <c r="AE20" s="82"/>
-      <c r="AF20" s="82"/>
-      <c r="AG20" s="82"/>
-      <c r="AH20" s="82"/>
-      <c r="AI20" s="82"/>
-      <c r="AJ20" s="82"/>
-      <c r="AK20" s="82"/>
-      <c r="AL20" s="82"/>
-      <c r="AM20" s="82"/>
-      <c r="AN20" s="82"/>
-      <c r="AO20" s="82"/>
-      <c r="AP20" s="82"/>
-      <c r="AQ20" s="80"/>
-      <c r="AR20" s="78"/>
-      <c r="AS20" s="78"/>
-      <c r="AT20" s="78"/>
-      <c r="AU20" s="78"/>
-      <c r="AV20" s="78"/>
-      <c r="AW20" s="78"/>
-      <c r="AX20" s="78"/>
-      <c r="AY20" s="78"/>
-      <c r="AZ20" s="78"/>
-      <c r="BA20" s="78"/>
-      <c r="BB20" s="78"/>
-      <c r="BC20" s="78"/>
-      <c r="BD20" s="78"/>
-      <c r="BE20" s="78"/>
-      <c r="BF20" s="78"/>
-      <c r="BG20" s="78"/>
-      <c r="BH20" s="78"/>
-      <c r="BI20" s="78"/>
-      <c r="BJ20" s="78"/>
-      <c r="BK20" s="79"/>
-      <c r="BL20" s="82"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
+      <c r="L20" s="85"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="85"/>
+      <c r="O20" s="85"/>
+      <c r="P20" s="85"/>
+      <c r="Q20" s="85"/>
+      <c r="R20" s="85"/>
+      <c r="S20" s="85"/>
+      <c r="T20" s="85"/>
+      <c r="U20" s="85"/>
+      <c r="V20" s="85"/>
+      <c r="W20" s="85"/>
+      <c r="X20" s="85"/>
+      <c r="Y20" s="85"/>
+      <c r="Z20" s="85"/>
+      <c r="AA20" s="85"/>
+      <c r="AB20" s="85"/>
+      <c r="AC20" s="85"/>
+      <c r="AD20" s="85"/>
+      <c r="AE20" s="85"/>
+      <c r="AF20" s="85"/>
+      <c r="AG20" s="85"/>
+      <c r="AH20" s="85"/>
+      <c r="AI20" s="85"/>
+      <c r="AJ20" s="85"/>
+      <c r="AK20" s="85"/>
+      <c r="AL20" s="85"/>
+      <c r="AM20" s="85"/>
+      <c r="AN20" s="85"/>
+      <c r="AO20" s="85"/>
+      <c r="AP20" s="85"/>
+      <c r="AQ20" s="86"/>
+      <c r="AR20" s="83"/>
+      <c r="AS20" s="83"/>
+      <c r="AT20" s="83"/>
+      <c r="AU20" s="83"/>
+      <c r="AV20" s="83"/>
+      <c r="AW20" s="83"/>
+      <c r="AX20" s="83"/>
+      <c r="AY20" s="83"/>
+      <c r="AZ20" s="83"/>
+      <c r="BA20" s="83"/>
+      <c r="BB20" s="83"/>
+      <c r="BC20" s="83"/>
+      <c r="BD20" s="83"/>
+      <c r="BE20" s="83"/>
+      <c r="BF20" s="83"/>
+      <c r="BG20" s="83"/>
+      <c r="BH20" s="83"/>
+      <c r="BI20" s="83"/>
+      <c r="BJ20" s="83"/>
+      <c r="BK20" s="84"/>
+      <c r="BL20" s="85"/>
     </row>
     <row r="23" spans="3:64">
       <c r="C23" s="71" t="s">
@@ -3201,102 +3711,102 @@
       </c>
     </row>
     <row r="24" spans="3:64">
-      <c r="D24" s="97" t="s">
+      <c r="D24" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="97">
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92">
         <v>1</v>
       </c>
-      <c r="H24" s="97"/>
-      <c r="I24" s="97">
+      <c r="H24" s="92"/>
+      <c r="I24" s="92">
         <v>2</v>
       </c>
-      <c r="J24" s="97"/>
-      <c r="K24" s="97">
+      <c r="J24" s="92"/>
+      <c r="K24" s="92">
         <v>3</v>
       </c>
-      <c r="L24" s="97"/>
-      <c r="M24" s="97">
+      <c r="L24" s="92"/>
+      <c r="M24" s="92">
         <v>4</v>
       </c>
-      <c r="N24" s="97"/>
-      <c r="O24" s="97">
+      <c r="N24" s="92"/>
+      <c r="O24" s="92">
         <v>5</v>
       </c>
-      <c r="P24" s="97"/>
-      <c r="Q24" s="97">
+      <c r="P24" s="92"/>
+      <c r="Q24" s="92">
         <v>6</v>
       </c>
-      <c r="R24" s="97"/>
-      <c r="S24" s="97">
+      <c r="R24" s="92"/>
+      <c r="S24" s="92">
         <v>7</v>
       </c>
-      <c r="T24" s="97"/>
-      <c r="U24" s="97">
+      <c r="T24" s="92"/>
+      <c r="U24" s="92">
         <v>8</v>
       </c>
-      <c r="V24" s="97"/>
-      <c r="W24" s="97" t="s">
+      <c r="V24" s="92"/>
+      <c r="W24" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="X24" s="97"/>
-      <c r="Y24" s="97">
+      <c r="X24" s="92"/>
+      <c r="Y24" s="92">
         <v>1</v>
       </c>
-      <c r="Z24" s="97"/>
-      <c r="AA24" s="97">
+      <c r="Z24" s="92"/>
+      <c r="AA24" s="92">
         <v>2</v>
       </c>
-      <c r="AB24" s="97"/>
-      <c r="AC24" s="97">
+      <c r="AB24" s="92"/>
+      <c r="AC24" s="92">
         <v>3</v>
       </c>
-      <c r="AD24" s="97"/>
-      <c r="AE24" s="97">
+      <c r="AD24" s="92"/>
+      <c r="AE24" s="92">
         <v>4</v>
       </c>
-      <c r="AF24" s="97"/>
-      <c r="AG24" s="97">
+      <c r="AF24" s="92"/>
+      <c r="AG24" s="92">
         <v>5</v>
       </c>
-      <c r="AH24" s="97"/>
-      <c r="AI24" s="97">
+      <c r="AH24" s="92"/>
+      <c r="AI24" s="92">
         <v>6</v>
       </c>
-      <c r="AJ24" s="97"/>
-      <c r="AK24" s="97">
+      <c r="AJ24" s="92"/>
+      <c r="AK24" s="92">
         <v>7</v>
       </c>
-      <c r="AL24" s="97"/>
-      <c r="AM24" s="97">
+      <c r="AL24" s="92"/>
+      <c r="AM24" s="92">
         <v>8</v>
       </c>
-      <c r="AN24" s="97"/>
-      <c r="AO24" s="97" t="s">
+      <c r="AN24" s="92"/>
+      <c r="AO24" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="AP24" s="97"/>
-      <c r="AQ24" s="97" t="s">
+      <c r="AP24" s="92"/>
+      <c r="AQ24" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="AR24" s="97"/>
-      <c r="AS24" s="97"/>
-      <c r="AU24" s="97"/>
-      <c r="AV24" s="97"/>
-      <c r="AW24" s="97"/>
-      <c r="AX24" s="97"/>
-      <c r="AY24" s="97"/>
-      <c r="AZ24" s="97"/>
-      <c r="BA24" s="97"/>
-      <c r="BB24" s="97"/>
-      <c r="BC24" s="97"/>
-      <c r="BD24" s="97"/>
-      <c r="BE24" s="97"/>
-      <c r="BF24" s="97"/>
-      <c r="BG24" s="97"/>
-      <c r="BH24" s="97"/>
+      <c r="AR24" s="92"/>
+      <c r="AS24" s="92"/>
+      <c r="AU24" s="92"/>
+      <c r="AV24" s="92"/>
+      <c r="AW24" s="92"/>
+      <c r="AX24" s="92"/>
+      <c r="AY24" s="92"/>
+      <c r="AZ24" s="92"/>
+      <c r="BA24" s="92"/>
+      <c r="BB24" s="92"/>
+      <c r="BC24" s="92"/>
+      <c r="BD24" s="92"/>
+      <c r="BE24" s="92"/>
+      <c r="BF24" s="92"/>
+      <c r="BG24" s="92"/>
+      <c r="BH24" s="92"/>
     </row>
     <row r="26" spans="3:64">
       <c r="C26" t="s">
@@ -3352,50 +3862,50 @@
       <c r="D28" s="78"/>
       <c r="E28" s="78"/>
       <c r="F28" s="79"/>
-      <c r="G28" s="91" t="s">
+      <c r="G28" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="92"/>
-      <c r="M28" s="92"/>
-      <c r="N28" s="92"/>
-      <c r="O28" s="92"/>
-      <c r="P28" s="93"/>
-      <c r="Q28" s="91" t="s">
+      <c r="H28" s="97"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="97"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="97"/>
+      <c r="N28" s="97"/>
+      <c r="O28" s="97"/>
+      <c r="P28" s="98"/>
+      <c r="Q28" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="R28" s="92"/>
-      <c r="S28" s="92"/>
-      <c r="T28" s="93"/>
-      <c r="U28" s="91" t="s">
+      <c r="R28" s="97"/>
+      <c r="S28" s="97"/>
+      <c r="T28" s="98"/>
+      <c r="U28" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="V28" s="93"/>
+      <c r="V28" s="98"/>
       <c r="W28" s="101" t="s">
         <v>106</v>
       </c>
       <c r="X28" s="102"/>
-      <c r="Y28" s="91" t="s">
+      <c r="Y28" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="Z28" s="92"/>
-      <c r="AA28" s="92"/>
-      <c r="AB28" s="92"/>
-      <c r="AC28" s="92"/>
-      <c r="AD28" s="92"/>
-      <c r="AE28" s="92"/>
-      <c r="AF28" s="92"/>
-      <c r="AG28" s="92"/>
-      <c r="AH28" s="92"/>
-      <c r="AI28" s="92"/>
-      <c r="AJ28" s="92"/>
-      <c r="AK28" s="92"/>
-      <c r="AL28" s="92"/>
-      <c r="AM28" s="92"/>
-      <c r="AN28" s="93"/>
+      <c r="Z28" s="97"/>
+      <c r="AA28" s="97"/>
+      <c r="AB28" s="97"/>
+      <c r="AC28" s="97"/>
+      <c r="AD28" s="97"/>
+      <c r="AE28" s="97"/>
+      <c r="AF28" s="97"/>
+      <c r="AG28" s="97"/>
+      <c r="AH28" s="97"/>
+      <c r="AI28" s="97"/>
+      <c r="AJ28" s="97"/>
+      <c r="AK28" s="97"/>
+      <c r="AL28" s="97"/>
+      <c r="AM28" s="97"/>
+      <c r="AN28" s="98"/>
       <c r="AO28" s="101" t="s">
         <v>106</v>
       </c>
@@ -3502,54 +4012,54 @@
       <c r="C34" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="95">
+      <c r="D34" s="94">
         <v>0</v>
       </c>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="95"/>
-      <c r="K34" s="95"/>
-      <c r="L34" s="95"/>
-      <c r="M34" s="95"/>
-      <c r="N34" s="95"/>
-      <c r="O34" s="95"/>
-      <c r="P34" s="95"/>
-      <c r="Q34" s="95"/>
-      <c r="R34" s="95"/>
-      <c r="S34" s="95"/>
-      <c r="T34" s="95"/>
-      <c r="U34" s="95"/>
-      <c r="V34" s="95"/>
-      <c r="W34" s="95"/>
-      <c r="X34" s="95"/>
-      <c r="Y34" s="95"/>
-      <c r="Z34" s="96"/>
-      <c r="AA34" s="94" t="s">
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="94"/>
+      <c r="I34" s="94"/>
+      <c r="J34" s="94"/>
+      <c r="K34" s="94"/>
+      <c r="L34" s="94"/>
+      <c r="M34" s="94"/>
+      <c r="N34" s="94"/>
+      <c r="O34" s="94"/>
+      <c r="P34" s="94"/>
+      <c r="Q34" s="94"/>
+      <c r="R34" s="94"/>
+      <c r="S34" s="94"/>
+      <c r="T34" s="94"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="94"/>
+      <c r="W34" s="94"/>
+      <c r="X34" s="94"/>
+      <c r="Y34" s="94"/>
+      <c r="Z34" s="95"/>
+      <c r="AA34" s="93" t="s">
         <v>111</v>
       </c>
-      <c r="AB34" s="95"/>
-      <c r="AC34" s="95"/>
-      <c r="AD34" s="95"/>
-      <c r="AE34" s="95"/>
-      <c r="AF34" s="95"/>
-      <c r="AG34" s="95"/>
-      <c r="AH34" s="95"/>
-      <c r="AI34" s="95"/>
-      <c r="AJ34" s="95"/>
-      <c r="AK34" s="95"/>
-      <c r="AL34" s="95"/>
-      <c r="AM34" s="95"/>
-      <c r="AN34" s="95"/>
-      <c r="AO34" s="95"/>
-      <c r="AP34" s="95"/>
-      <c r="AQ34" s="96"/>
-      <c r="AR34" s="94">
+      <c r="AB34" s="94"/>
+      <c r="AC34" s="94"/>
+      <c r="AD34" s="94"/>
+      <c r="AE34" s="94"/>
+      <c r="AF34" s="94"/>
+      <c r="AG34" s="94"/>
+      <c r="AH34" s="94"/>
+      <c r="AI34" s="94"/>
+      <c r="AJ34" s="94"/>
+      <c r="AK34" s="94"/>
+      <c r="AL34" s="94"/>
+      <c r="AM34" s="94"/>
+      <c r="AN34" s="94"/>
+      <c r="AO34" s="94"/>
+      <c r="AP34" s="94"/>
+      <c r="AQ34" s="95"/>
+      <c r="AR34" s="93">
         <v>0</v>
       </c>
-      <c r="AS34" s="95"/>
+      <c r="AS34" s="94"/>
     </row>
     <row r="36" spans="3:64">
       <c r="C36" t="s">
@@ -3578,25 +4088,25 @@
       <c r="X36" s="74"/>
       <c r="Y36" s="74"/>
       <c r="Z36" s="74"/>
-      <c r="AA36" s="91" t="s">
+      <c r="AA36" s="96" t="s">
         <v>149</v>
       </c>
-      <c r="AB36" s="92"/>
-      <c r="AC36" s="92"/>
-      <c r="AD36" s="92"/>
-      <c r="AE36" s="92"/>
-      <c r="AF36" s="92"/>
-      <c r="AG36" s="92"/>
-      <c r="AH36" s="92"/>
-      <c r="AI36" s="92"/>
-      <c r="AJ36" s="92"/>
-      <c r="AK36" s="92"/>
-      <c r="AL36" s="92"/>
-      <c r="AM36" s="92"/>
-      <c r="AN36" s="92"/>
-      <c r="AO36" s="92"/>
-      <c r="AP36" s="92"/>
-      <c r="AQ36" s="93"/>
+      <c r="AB36" s="97"/>
+      <c r="AC36" s="97"/>
+      <c r="AD36" s="97"/>
+      <c r="AE36" s="97"/>
+      <c r="AF36" s="97"/>
+      <c r="AG36" s="97"/>
+      <c r="AH36" s="97"/>
+      <c r="AI36" s="97"/>
+      <c r="AJ36" s="97"/>
+      <c r="AK36" s="97"/>
+      <c r="AL36" s="97"/>
+      <c r="AM36" s="97"/>
+      <c r="AN36" s="97"/>
+      <c r="AO36" s="97"/>
+      <c r="AP36" s="97"/>
+      <c r="AQ36" s="98"/>
       <c r="AR36" s="74"/>
       <c r="AS36" s="74"/>
     </row>
@@ -3648,119 +4158,119 @@
       <c r="AS38" s="83"/>
     </row>
     <row r="41" spans="3:64">
-      <c r="G41" s="97">
+      <c r="G41" s="92">
         <v>1</v>
       </c>
-      <c r="H41" s="97"/>
-      <c r="I41" s="97">
+      <c r="H41" s="92"/>
+      <c r="I41" s="92">
         <v>2</v>
       </c>
-      <c r="J41" s="97"/>
-      <c r="K41" s="97">
+      <c r="J41" s="92"/>
+      <c r="K41" s="92">
         <v>3</v>
       </c>
-      <c r="L41" s="97"/>
-      <c r="M41" s="97">
+      <c r="L41" s="92"/>
+      <c r="M41" s="92">
         <v>4</v>
       </c>
-      <c r="N41" s="97"/>
-      <c r="O41" s="97">
+      <c r="N41" s="92"/>
+      <c r="O41" s="92">
         <v>5</v>
       </c>
-      <c r="P41" s="97"/>
-      <c r="Q41" s="97">
+      <c r="P41" s="92"/>
+      <c r="Q41" s="92">
         <v>6</v>
       </c>
-      <c r="R41" s="97"/>
-      <c r="S41" s="97">
+      <c r="R41" s="92"/>
+      <c r="S41" s="92">
         <v>7</v>
       </c>
-      <c r="T41" s="97"/>
-      <c r="U41" s="97">
+      <c r="T41" s="92"/>
+      <c r="U41" s="92">
         <v>8</v>
       </c>
-      <c r="V41" s="97"/>
-      <c r="W41" s="97" t="s">
+      <c r="V41" s="92"/>
+      <c r="W41" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="X41" s="97"/>
-      <c r="Y41" s="97">
+      <c r="X41" s="92"/>
+      <c r="Y41" s="92">
         <v>1</v>
       </c>
-      <c r="Z41" s="97"/>
-      <c r="AA41" s="97">
+      <c r="Z41" s="92"/>
+      <c r="AA41" s="92">
         <v>2</v>
       </c>
-      <c r="AB41" s="97"/>
-      <c r="AC41" s="97">
+      <c r="AB41" s="92"/>
+      <c r="AC41" s="92">
         <v>3</v>
       </c>
-      <c r="AD41" s="97"/>
-      <c r="AE41" s="97">
+      <c r="AD41" s="92"/>
+      <c r="AE41" s="92">
         <v>4</v>
       </c>
-      <c r="AF41" s="97"/>
-      <c r="AG41" s="97">
+      <c r="AF41" s="92"/>
+      <c r="AG41" s="92">
         <v>5</v>
       </c>
-      <c r="AH41" s="97"/>
-      <c r="AI41" s="97">
+      <c r="AH41" s="92"/>
+      <c r="AI41" s="92">
         <v>6</v>
       </c>
-      <c r="AJ41" s="97"/>
-      <c r="AK41" s="97">
+      <c r="AJ41" s="92"/>
+      <c r="AK41" s="92">
         <v>7</v>
       </c>
-      <c r="AL41" s="97"/>
-      <c r="AM41" s="97">
+      <c r="AL41" s="92"/>
+      <c r="AM41" s="92">
         <v>8</v>
       </c>
-      <c r="AN41" s="97"/>
-      <c r="AO41" s="97" t="s">
+      <c r="AN41" s="92"/>
+      <c r="AO41" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="AP41" s="97"/>
-      <c r="AQ41" s="97">
+      <c r="AP41" s="92"/>
+      <c r="AQ41" s="92">
         <v>1</v>
       </c>
-      <c r="AR41" s="97"/>
-      <c r="AS41" s="97">
+      <c r="AR41" s="92"/>
+      <c r="AS41" s="92">
         <v>2</v>
       </c>
-      <c r="AT41" s="97"/>
-      <c r="AU41" s="97">
+      <c r="AT41" s="92"/>
+      <c r="AU41" s="92">
         <v>3</v>
       </c>
-      <c r="AV41" s="97"/>
-      <c r="AW41" s="97">
+      <c r="AV41" s="92"/>
+      <c r="AW41" s="92">
         <v>4</v>
       </c>
-      <c r="AX41" s="97"/>
-      <c r="AY41" s="97">
+      <c r="AX41" s="92"/>
+      <c r="AY41" s="92">
         <v>5</v>
       </c>
-      <c r="AZ41" s="97"/>
-      <c r="BA41" s="97">
+      <c r="AZ41" s="92"/>
+      <c r="BA41" s="92">
         <v>6</v>
       </c>
-      <c r="BB41" s="97"/>
-      <c r="BC41" s="97">
+      <c r="BB41" s="92"/>
+      <c r="BC41" s="92">
         <v>7</v>
       </c>
-      <c r="BD41" s="97"/>
-      <c r="BE41" s="97">
+      <c r="BD41" s="92"/>
+      <c r="BE41" s="92">
         <v>8</v>
       </c>
-      <c r="BF41" s="97"/>
-      <c r="BG41" s="97" t="s">
+      <c r="BF41" s="92"/>
+      <c r="BG41" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="BH41" s="97"/>
-      <c r="BI41" s="97" t="s">
+      <c r="BH41" s="92"/>
+      <c r="BI41" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="BJ41" s="97"/>
-      <c r="BK41" s="97"/>
+      <c r="BJ41" s="92"/>
+      <c r="BK41" s="92"/>
       <c r="BL41" s="72"/>
     </row>
     <row r="43" spans="3:64">
@@ -3827,76 +4337,76 @@
     <row r="45" spans="3:64">
       <c r="E45" s="1"/>
       <c r="F45" s="81"/>
-      <c r="G45" s="91" t="s">
+      <c r="G45" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="H45" s="92"/>
-      <c r="I45" s="92"/>
-      <c r="J45" s="92"/>
-      <c r="K45" s="92"/>
-      <c r="L45" s="92"/>
-      <c r="M45" s="92"/>
-      <c r="N45" s="92"/>
-      <c r="O45" s="92"/>
-      <c r="P45" s="93"/>
-      <c r="Q45" s="91" t="s">
+      <c r="H45" s="97"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="97"/>
+      <c r="K45" s="97"/>
+      <c r="L45" s="97"/>
+      <c r="M45" s="97"/>
+      <c r="N45" s="97"/>
+      <c r="O45" s="97"/>
+      <c r="P45" s="98"/>
+      <c r="Q45" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="R45" s="92"/>
-      <c r="S45" s="92"/>
-      <c r="T45" s="93"/>
-      <c r="U45" s="91" t="s">
+      <c r="R45" s="97"/>
+      <c r="S45" s="97"/>
+      <c r="T45" s="98"/>
+      <c r="U45" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="V45" s="93"/>
+      <c r="V45" s="98"/>
       <c r="W45" s="101" t="s">
         <v>106</v>
       </c>
       <c r="X45" s="102"/>
-      <c r="Y45" s="94" t="s">
+      <c r="Y45" s="93" t="s">
         <v>129</v>
       </c>
-      <c r="Z45" s="95"/>
-      <c r="AA45" s="95"/>
-      <c r="AB45" s="95"/>
-      <c r="AC45" s="95"/>
-      <c r="AD45" s="95"/>
-      <c r="AE45" s="95"/>
-      <c r="AF45" s="95"/>
-      <c r="AG45" s="95"/>
-      <c r="AH45" s="95"/>
-      <c r="AI45" s="95"/>
-      <c r="AJ45" s="95"/>
-      <c r="AK45" s="95"/>
-      <c r="AL45" s="95"/>
-      <c r="AM45" s="95"/>
-      <c r="AN45" s="96"/>
+      <c r="Z45" s="94"/>
+      <c r="AA45" s="94"/>
+      <c r="AB45" s="94"/>
+      <c r="AC45" s="94"/>
+      <c r="AD45" s="94"/>
+      <c r="AE45" s="94"/>
+      <c r="AF45" s="94"/>
+      <c r="AG45" s="94"/>
+      <c r="AH45" s="94"/>
+      <c r="AI45" s="94"/>
+      <c r="AJ45" s="94"/>
+      <c r="AK45" s="94"/>
+      <c r="AL45" s="94"/>
+      <c r="AM45" s="94"/>
+      <c r="AN45" s="95"/>
       <c r="AO45" s="103" t="s">
         <v>106</v>
       </c>
       <c r="AP45" s="104"/>
-      <c r="AQ45" s="94" t="s">
+      <c r="AQ45" s="93" t="s">
         <v>130</v>
       </c>
-      <c r="AR45" s="95"/>
-      <c r="AS45" s="95"/>
-      <c r="AT45" s="95"/>
-      <c r="AU45" s="95"/>
-      <c r="AV45" s="95"/>
-      <c r="AW45" s="95"/>
-      <c r="AX45" s="95"/>
-      <c r="AY45" s="95"/>
-      <c r="AZ45" s="95"/>
-      <c r="BA45" s="95"/>
-      <c r="BB45" s="95"/>
-      <c r="BC45" s="95"/>
-      <c r="BD45" s="95"/>
-      <c r="BE45" s="95"/>
-      <c r="BF45" s="96"/>
-      <c r="BG45" s="106" t="s">
+      <c r="AR45" s="94"/>
+      <c r="AS45" s="94"/>
+      <c r="AT45" s="94"/>
+      <c r="AU45" s="94"/>
+      <c r="AV45" s="94"/>
+      <c r="AW45" s="94"/>
+      <c r="AX45" s="94"/>
+      <c r="AY45" s="94"/>
+      <c r="AZ45" s="94"/>
+      <c r="BA45" s="94"/>
+      <c r="BB45" s="94"/>
+      <c r="BC45" s="94"/>
+      <c r="BD45" s="94"/>
+      <c r="BE45" s="94"/>
+      <c r="BF45" s="95"/>
+      <c r="BG45" s="99" t="s">
         <v>118</v>
       </c>
-      <c r="BH45" s="107"/>
+      <c r="BH45" s="100"/>
       <c r="BI45" s="82"/>
       <c r="BJ45" s="81"/>
       <c r="BK45" s="80"/>
@@ -4025,27 +4535,27 @@
       <c r="BL49" s="85"/>
     </row>
     <row r="51" spans="3:64">
-      <c r="F51" s="95">
+      <c r="F51" s="94">
         <v>0</v>
       </c>
-      <c r="G51" s="95"/>
-      <c r="H51" s="95"/>
-      <c r="I51" s="95"/>
-      <c r="J51" s="95"/>
-      <c r="K51" s="95"/>
-      <c r="L51" s="95"/>
-      <c r="M51" s="95"/>
-      <c r="N51" s="95"/>
-      <c r="O51" s="95"/>
-      <c r="P51" s="95"/>
-      <c r="Q51" s="95"/>
-      <c r="R51" s="95"/>
-      <c r="S51" s="95"/>
-      <c r="T51" s="95"/>
-      <c r="U51" s="95"/>
-      <c r="V51" s="95"/>
-      <c r="W51" s="95"/>
-      <c r="X51" s="96"/>
+      <c r="G51" s="94"/>
+      <c r="H51" s="94"/>
+      <c r="I51" s="94"/>
+      <c r="J51" s="94"/>
+      <c r="K51" s="94"/>
+      <c r="L51" s="94"/>
+      <c r="M51" s="94"/>
+      <c r="N51" s="94"/>
+      <c r="O51" s="94"/>
+      <c r="P51" s="94"/>
+      <c r="Q51" s="94"/>
+      <c r="R51" s="94"/>
+      <c r="S51" s="94"/>
+      <c r="T51" s="94"/>
+      <c r="U51" s="94"/>
+      <c r="V51" s="94"/>
+      <c r="W51" s="94"/>
+      <c r="X51" s="95"/>
       <c r="Y51" s="90"/>
       <c r="Z51" s="88"/>
       <c r="AA51" s="88"/>
@@ -4084,10 +4594,10 @@
       <c r="BH51" s="88"/>
       <c r="BI51" s="88"/>
       <c r="BJ51" s="88"/>
-      <c r="BK51" s="94">
+      <c r="BK51" s="93">
         <v>0</v>
       </c>
-      <c r="BL51" s="95"/>
+      <c r="BL51" s="94"/>
     </row>
     <row r="53" spans="3:64">
       <c r="F53" s="73"/>
@@ -4111,45 +4621,45 @@
       <c r="X53" s="74"/>
       <c r="Y53" s="74"/>
       <c r="Z53" s="74"/>
-      <c r="AA53" s="91" t="s">
+      <c r="AA53" s="96" t="s">
         <v>150</v>
       </c>
-      <c r="AB53" s="92"/>
-      <c r="AC53" s="92"/>
-      <c r="AD53" s="92"/>
-      <c r="AE53" s="92"/>
-      <c r="AF53" s="92"/>
-      <c r="AG53" s="92"/>
-      <c r="AH53" s="92"/>
-      <c r="AI53" s="92"/>
-      <c r="AJ53" s="92"/>
-      <c r="AK53" s="92"/>
-      <c r="AL53" s="92"/>
-      <c r="AM53" s="92"/>
-      <c r="AN53" s="92"/>
-      <c r="AO53" s="92"/>
-      <c r="AP53" s="92"/>
-      <c r="AQ53" s="93"/>
+      <c r="AB53" s="97"/>
+      <c r="AC53" s="97"/>
+      <c r="AD53" s="97"/>
+      <c r="AE53" s="97"/>
+      <c r="AF53" s="97"/>
+      <c r="AG53" s="97"/>
+      <c r="AH53" s="97"/>
+      <c r="AI53" s="97"/>
+      <c r="AJ53" s="97"/>
+      <c r="AK53" s="97"/>
+      <c r="AL53" s="97"/>
+      <c r="AM53" s="97"/>
+      <c r="AN53" s="97"/>
+      <c r="AO53" s="97"/>
+      <c r="AP53" s="97"/>
+      <c r="AQ53" s="98"/>
       <c r="AR53" s="74"/>
-      <c r="AS53" s="91" t="s">
+      <c r="AS53" s="96" t="s">
         <v>132</v>
       </c>
-      <c r="AT53" s="92"/>
-      <c r="AU53" s="92"/>
-      <c r="AV53" s="92"/>
-      <c r="AW53" s="92"/>
-      <c r="AX53" s="92"/>
-      <c r="AY53" s="92"/>
-      <c r="AZ53" s="92"/>
-      <c r="BA53" s="92"/>
-      <c r="BB53" s="92"/>
-      <c r="BC53" s="92"/>
-      <c r="BD53" s="92"/>
-      <c r="BE53" s="92"/>
-      <c r="BF53" s="92"/>
-      <c r="BG53" s="92"/>
-      <c r="BH53" s="92"/>
-      <c r="BI53" s="93"/>
+      <c r="AT53" s="97"/>
+      <c r="AU53" s="97"/>
+      <c r="AV53" s="97"/>
+      <c r="AW53" s="97"/>
+      <c r="AX53" s="97"/>
+      <c r="AY53" s="97"/>
+      <c r="AZ53" s="97"/>
+      <c r="BA53" s="97"/>
+      <c r="BB53" s="97"/>
+      <c r="BC53" s="97"/>
+      <c r="BD53" s="97"/>
+      <c r="BE53" s="97"/>
+      <c r="BF53" s="97"/>
+      <c r="BG53" s="97"/>
+      <c r="BH53" s="97"/>
+      <c r="BI53" s="98"/>
       <c r="BJ53" s="75"/>
       <c r="BK53" s="88"/>
       <c r="BL53" s="88"/>
@@ -4230,124 +4740,124 @@
       </c>
     </row>
     <row r="58" spans="3:64">
-      <c r="D58" s="97" t="s">
+      <c r="D58" s="92" t="s">
         <v>119</v>
       </c>
-      <c r="E58" s="97"/>
-      <c r="F58" s="97"/>
-      <c r="G58" s="97">
+      <c r="E58" s="92"/>
+      <c r="F58" s="92"/>
+      <c r="G58" s="92">
         <v>1</v>
       </c>
-      <c r="H58" s="97"/>
-      <c r="I58" s="97">
+      <c r="H58" s="92"/>
+      <c r="I58" s="92">
         <v>2</v>
       </c>
-      <c r="J58" s="97"/>
-      <c r="K58" s="97">
+      <c r="J58" s="92"/>
+      <c r="K58" s="92">
         <v>3</v>
       </c>
-      <c r="L58" s="97"/>
-      <c r="M58" s="97">
+      <c r="L58" s="92"/>
+      <c r="M58" s="92">
         <v>4</v>
       </c>
-      <c r="N58" s="97"/>
-      <c r="O58" s="97">
+      <c r="N58" s="92"/>
+      <c r="O58" s="92">
         <v>5</v>
       </c>
-      <c r="P58" s="97"/>
-      <c r="Q58" s="97">
+      <c r="P58" s="92"/>
+      <c r="Q58" s="92">
         <v>6</v>
       </c>
-      <c r="R58" s="97"/>
-      <c r="S58" s="97">
+      <c r="R58" s="92"/>
+      <c r="S58" s="92">
         <v>7</v>
       </c>
-      <c r="T58" s="97"/>
-      <c r="U58" s="97">
+      <c r="T58" s="92"/>
+      <c r="U58" s="92">
         <v>8</v>
       </c>
-      <c r="V58" s="97"/>
-      <c r="W58" s="97" t="s">
+      <c r="V58" s="92"/>
+      <c r="W58" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="X58" s="97"/>
-      <c r="Y58" s="97">
+      <c r="X58" s="92"/>
+      <c r="Y58" s="92">
         <v>1</v>
       </c>
-      <c r="Z58" s="97"/>
-      <c r="AA58" s="97">
+      <c r="Z58" s="92"/>
+      <c r="AA58" s="92">
         <v>2</v>
       </c>
-      <c r="AB58" s="97"/>
-      <c r="AC58" s="97">
+      <c r="AB58" s="92"/>
+      <c r="AC58" s="92">
         <v>3</v>
       </c>
-      <c r="AD58" s="97"/>
-      <c r="AE58" s="97">
+      <c r="AD58" s="92"/>
+      <c r="AE58" s="92">
         <v>4</v>
       </c>
-      <c r="AF58" s="97"/>
-      <c r="AG58" s="97">
+      <c r="AF58" s="92"/>
+      <c r="AG58" s="92">
         <v>5</v>
       </c>
-      <c r="AH58" s="97"/>
-      <c r="AI58" s="97">
+      <c r="AH58" s="92"/>
+      <c r="AI58" s="92">
         <v>6</v>
       </c>
-      <c r="AJ58" s="97"/>
-      <c r="AK58" s="97">
+      <c r="AJ58" s="92"/>
+      <c r="AK58" s="92">
         <v>7</v>
       </c>
-      <c r="AL58" s="97"/>
-      <c r="AM58" s="97">
+      <c r="AL58" s="92"/>
+      <c r="AM58" s="92">
         <v>8</v>
       </c>
-      <c r="AN58" s="97"/>
-      <c r="AO58" s="97" t="s">
+      <c r="AN58" s="92"/>
+      <c r="AO58" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="AP58" s="97"/>
-      <c r="AQ58" s="97">
+      <c r="AP58" s="92"/>
+      <c r="AQ58" s="92">
         <v>1</v>
       </c>
-      <c r="AR58" s="97"/>
-      <c r="AS58" s="97">
+      <c r="AR58" s="92"/>
+      <c r="AS58" s="92">
         <v>2</v>
       </c>
-      <c r="AT58" s="97"/>
-      <c r="AU58" s="97">
+      <c r="AT58" s="92"/>
+      <c r="AU58" s="92">
         <v>3</v>
       </c>
-      <c r="AV58" s="97"/>
-      <c r="AW58" s="97">
+      <c r="AV58" s="92"/>
+      <c r="AW58" s="92">
         <v>4</v>
       </c>
-      <c r="AX58" s="97"/>
-      <c r="AY58" s="97">
+      <c r="AX58" s="92"/>
+      <c r="AY58" s="92">
         <v>5</v>
       </c>
-      <c r="AZ58" s="97"/>
-      <c r="BA58" s="97">
+      <c r="AZ58" s="92"/>
+      <c r="BA58" s="92">
         <v>6</v>
       </c>
-      <c r="BB58" s="97"/>
-      <c r="BC58" s="97">
+      <c r="BB58" s="92"/>
+      <c r="BC58" s="92">
         <v>7</v>
       </c>
-      <c r="BD58" s="97"/>
-      <c r="BE58" s="97">
+      <c r="BD58" s="92"/>
+      <c r="BE58" s="92">
         <v>8</v>
       </c>
-      <c r="BF58" s="97"/>
-      <c r="BG58" s="97" t="s">
+      <c r="BF58" s="92"/>
+      <c r="BG58" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="BH58" s="97"/>
-      <c r="BI58" s="97" t="s">
+      <c r="BH58" s="92"/>
+      <c r="BI58" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="BJ58" s="97"/>
-      <c r="BK58" s="97"/>
+      <c r="BJ58" s="92"/>
+      <c r="BK58" s="92"/>
       <c r="BL58" s="72"/>
     </row>
     <row r="60" spans="3:64">
@@ -4423,76 +4933,76 @@
       <c r="D62" s="78"/>
       <c r="E62" s="78"/>
       <c r="F62" s="79"/>
-      <c r="G62" s="91" t="s">
+      <c r="G62" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="H62" s="92"/>
-      <c r="I62" s="92"/>
-      <c r="J62" s="92"/>
-      <c r="K62" s="92"/>
-      <c r="L62" s="92"/>
-      <c r="M62" s="92"/>
-      <c r="N62" s="92"/>
-      <c r="O62" s="92"/>
-      <c r="P62" s="93"/>
-      <c r="Q62" s="91" t="s">
+      <c r="H62" s="97"/>
+      <c r="I62" s="97"/>
+      <c r="J62" s="97"/>
+      <c r="K62" s="97"/>
+      <c r="L62" s="97"/>
+      <c r="M62" s="97"/>
+      <c r="N62" s="97"/>
+      <c r="O62" s="97"/>
+      <c r="P62" s="98"/>
+      <c r="Q62" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="R62" s="92"/>
-      <c r="S62" s="92"/>
-      <c r="T62" s="93"/>
-      <c r="U62" s="91" t="s">
+      <c r="R62" s="97"/>
+      <c r="S62" s="97"/>
+      <c r="T62" s="98"/>
+      <c r="U62" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="V62" s="93"/>
+      <c r="V62" s="98"/>
       <c r="W62" s="101" t="s">
         <v>106</v>
       </c>
       <c r="X62" s="102"/>
-      <c r="Y62" s="94" t="s">
+      <c r="Y62" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="Z62" s="95"/>
-      <c r="AA62" s="95"/>
-      <c r="AB62" s="95"/>
-      <c r="AC62" s="95"/>
-      <c r="AD62" s="95"/>
-      <c r="AE62" s="95"/>
-      <c r="AF62" s="95"/>
-      <c r="AG62" s="95"/>
-      <c r="AH62" s="95"/>
-      <c r="AI62" s="95"/>
-      <c r="AJ62" s="95"/>
-      <c r="AK62" s="95"/>
-      <c r="AL62" s="95"/>
-      <c r="AM62" s="95"/>
-      <c r="AN62" s="96"/>
+      <c r="Z62" s="94"/>
+      <c r="AA62" s="94"/>
+      <c r="AB62" s="94"/>
+      <c r="AC62" s="94"/>
+      <c r="AD62" s="94"/>
+      <c r="AE62" s="94"/>
+      <c r="AF62" s="94"/>
+      <c r="AG62" s="94"/>
+      <c r="AH62" s="94"/>
+      <c r="AI62" s="94"/>
+      <c r="AJ62" s="94"/>
+      <c r="AK62" s="94"/>
+      <c r="AL62" s="94"/>
+      <c r="AM62" s="94"/>
+      <c r="AN62" s="95"/>
       <c r="AO62" s="103" t="s">
         <v>106</v>
       </c>
       <c r="AP62" s="104"/>
-      <c r="AQ62" s="94" t="s">
+      <c r="AQ62" s="93" t="s">
         <v>129</v>
       </c>
-      <c r="AR62" s="95"/>
-      <c r="AS62" s="95"/>
-      <c r="AT62" s="95"/>
-      <c r="AU62" s="95"/>
-      <c r="AV62" s="95"/>
-      <c r="AW62" s="95"/>
-      <c r="AX62" s="95"/>
-      <c r="AY62" s="95"/>
-      <c r="AZ62" s="95"/>
-      <c r="BA62" s="95"/>
-      <c r="BB62" s="95"/>
-      <c r="BC62" s="95"/>
-      <c r="BD62" s="95"/>
-      <c r="BE62" s="95"/>
-      <c r="BF62" s="96"/>
-      <c r="BG62" s="106" t="s">
+      <c r="AR62" s="94"/>
+      <c r="AS62" s="94"/>
+      <c r="AT62" s="94"/>
+      <c r="AU62" s="94"/>
+      <c r="AV62" s="94"/>
+      <c r="AW62" s="94"/>
+      <c r="AX62" s="94"/>
+      <c r="AY62" s="94"/>
+      <c r="AZ62" s="94"/>
+      <c r="BA62" s="94"/>
+      <c r="BB62" s="94"/>
+      <c r="BC62" s="94"/>
+      <c r="BD62" s="94"/>
+      <c r="BE62" s="94"/>
+      <c r="BF62" s="95"/>
+      <c r="BG62" s="99" t="s">
         <v>118</v>
       </c>
-      <c r="BH62" s="107"/>
+      <c r="BH62" s="100"/>
       <c r="BI62" s="82"/>
       <c r="BJ62" s="81"/>
       <c r="BK62" s="80"/>
@@ -4634,29 +5144,29 @@
       <c r="C68" t="s">
         <v>47</v>
       </c>
-      <c r="D68" s="95">
+      <c r="D68" s="94">
         <v>0</v>
       </c>
-      <c r="E68" s="95"/>
-      <c r="F68" s="95"/>
-      <c r="G68" s="95"/>
-      <c r="H68" s="95"/>
-      <c r="I68" s="95"/>
-      <c r="J68" s="95"/>
-      <c r="K68" s="95"/>
-      <c r="L68" s="95"/>
-      <c r="M68" s="95"/>
-      <c r="N68" s="95"/>
-      <c r="O68" s="95"/>
-      <c r="P68" s="95"/>
-      <c r="Q68" s="95"/>
-      <c r="R68" s="95"/>
-      <c r="S68" s="95"/>
-      <c r="T68" s="95"/>
-      <c r="U68" s="95"/>
-      <c r="V68" s="95"/>
-      <c r="W68" s="95"/>
-      <c r="X68" s="96"/>
+      <c r="E68" s="94"/>
+      <c r="F68" s="94"/>
+      <c r="G68" s="94"/>
+      <c r="H68" s="94"/>
+      <c r="I68" s="94"/>
+      <c r="J68" s="94"/>
+      <c r="K68" s="94"/>
+      <c r="L68" s="94"/>
+      <c r="M68" s="94"/>
+      <c r="N68" s="94"/>
+      <c r="O68" s="94"/>
+      <c r="P68" s="94"/>
+      <c r="Q68" s="94"/>
+      <c r="R68" s="94"/>
+      <c r="S68" s="94"/>
+      <c r="T68" s="94"/>
+      <c r="U68" s="94"/>
+      <c r="V68" s="94"/>
+      <c r="W68" s="94"/>
+      <c r="X68" s="95"/>
       <c r="Y68" s="90"/>
       <c r="Z68" s="88"/>
       <c r="AA68" s="88"/>
@@ -4695,10 +5205,10 @@
       <c r="BH68" s="88"/>
       <c r="BI68" s="88"/>
       <c r="BJ68" s="88"/>
-      <c r="BK68" s="94">
+      <c r="BK68" s="93">
         <v>0</v>
       </c>
-      <c r="BL68" s="95"/>
+      <c r="BL68" s="94"/>
     </row>
     <row r="70" spans="3:64">
       <c r="C70" t="s">
@@ -4727,45 +5237,45 @@
       <c r="X70" s="74"/>
       <c r="Y70" s="74"/>
       <c r="Z70" s="74"/>
-      <c r="AA70" s="91" t="s">
+      <c r="AA70" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="AB70" s="92"/>
-      <c r="AC70" s="92"/>
-      <c r="AD70" s="92"/>
-      <c r="AE70" s="92"/>
-      <c r="AF70" s="92"/>
-      <c r="AG70" s="92"/>
-      <c r="AH70" s="92"/>
-      <c r="AI70" s="92"/>
-      <c r="AJ70" s="92"/>
-      <c r="AK70" s="92"/>
-      <c r="AL70" s="92"/>
-      <c r="AM70" s="92"/>
-      <c r="AN70" s="92"/>
-      <c r="AO70" s="92"/>
-      <c r="AP70" s="92"/>
-      <c r="AQ70" s="93"/>
+      <c r="AB70" s="97"/>
+      <c r="AC70" s="97"/>
+      <c r="AD70" s="97"/>
+      <c r="AE70" s="97"/>
+      <c r="AF70" s="97"/>
+      <c r="AG70" s="97"/>
+      <c r="AH70" s="97"/>
+      <c r="AI70" s="97"/>
+      <c r="AJ70" s="97"/>
+      <c r="AK70" s="97"/>
+      <c r="AL70" s="97"/>
+      <c r="AM70" s="97"/>
+      <c r="AN70" s="97"/>
+      <c r="AO70" s="97"/>
+      <c r="AP70" s="97"/>
+      <c r="AQ70" s="98"/>
       <c r="AR70" s="74"/>
-      <c r="AS70" s="91" t="s">
+      <c r="AS70" s="96" t="s">
         <v>131</v>
       </c>
-      <c r="AT70" s="92"/>
-      <c r="AU70" s="92"/>
-      <c r="AV70" s="92"/>
-      <c r="AW70" s="92"/>
-      <c r="AX70" s="92"/>
-      <c r="AY70" s="92"/>
-      <c r="AZ70" s="92"/>
-      <c r="BA70" s="92"/>
-      <c r="BB70" s="92"/>
-      <c r="BC70" s="92"/>
-      <c r="BD70" s="92"/>
-      <c r="BE70" s="92"/>
-      <c r="BF70" s="92"/>
-      <c r="BG70" s="92"/>
-      <c r="BH70" s="92"/>
-      <c r="BI70" s="93"/>
+      <c r="AT70" s="97"/>
+      <c r="AU70" s="97"/>
+      <c r="AV70" s="97"/>
+      <c r="AW70" s="97"/>
+      <c r="AX70" s="97"/>
+      <c r="AY70" s="97"/>
+      <c r="AZ70" s="97"/>
+      <c r="BA70" s="97"/>
+      <c r="BB70" s="97"/>
+      <c r="BC70" s="97"/>
+      <c r="BD70" s="97"/>
+      <c r="BE70" s="97"/>
+      <c r="BF70" s="97"/>
+      <c r="BG70" s="97"/>
+      <c r="BH70" s="97"/>
+      <c r="BI70" s="98"/>
       <c r="BJ70" s="75"/>
       <c r="BK70" s="88"/>
       <c r="BL70" s="88"/>
@@ -4988,72 +5498,72 @@
       <c r="D81" s="69"/>
       <c r="E81" s="69"/>
       <c r="F81" s="69"/>
-      <c r="G81" s="94">
+      <c r="G81" s="93">
         <v>7</v>
       </c>
-      <c r="H81" s="96"/>
-      <c r="I81" s="94">
+      <c r="H81" s="95"/>
+      <c r="I81" s="93">
         <v>6</v>
       </c>
-      <c r="J81" s="96"/>
-      <c r="K81" s="94">
+      <c r="J81" s="95"/>
+      <c r="K81" s="93">
         <v>5</v>
       </c>
-      <c r="L81" s="96"/>
-      <c r="M81" s="94">
+      <c r="L81" s="95"/>
+      <c r="M81" s="93">
         <v>4</v>
       </c>
-      <c r="N81" s="96"/>
-      <c r="O81" s="94">
+      <c r="N81" s="95"/>
+      <c r="O81" s="93">
         <v>3</v>
       </c>
-      <c r="P81" s="96"/>
-      <c r="Q81" s="94">
+      <c r="P81" s="95"/>
+      <c r="Q81" s="93">
         <v>2</v>
       </c>
-      <c r="R81" s="96"/>
-      <c r="S81" s="94">
+      <c r="R81" s="95"/>
+      <c r="S81" s="93">
         <v>1</v>
       </c>
-      <c r="T81" s="96"/>
-      <c r="U81" s="94">
+      <c r="T81" s="95"/>
+      <c r="U81" s="93">
         <v>0</v>
       </c>
-      <c r="V81" s="96"/>
+      <c r="V81" s="95"/>
       <c r="W81" s="69"/>
       <c r="X81" s="69"/>
-      <c r="Y81" s="94">
+      <c r="Y81" s="93">
         <v>7</v>
       </c>
-      <c r="Z81" s="96"/>
-      <c r="AA81" s="94">
+      <c r="Z81" s="95"/>
+      <c r="AA81" s="93">
         <v>6</v>
       </c>
-      <c r="AB81" s="96"/>
-      <c r="AC81" s="94">
+      <c r="AB81" s="95"/>
+      <c r="AC81" s="93">
         <v>5</v>
       </c>
-      <c r="AD81" s="96"/>
-      <c r="AE81" s="94">
+      <c r="AD81" s="95"/>
+      <c r="AE81" s="93">
         <v>4</v>
       </c>
-      <c r="AF81" s="96"/>
-      <c r="AG81" s="94">
+      <c r="AF81" s="95"/>
+      <c r="AG81" s="93">
         <v>3</v>
       </c>
-      <c r="AH81" s="96"/>
-      <c r="AI81" s="94">
+      <c r="AH81" s="95"/>
+      <c r="AI81" s="93">
         <v>2</v>
       </c>
-      <c r="AJ81" s="96"/>
-      <c r="AK81" s="94">
+      <c r="AJ81" s="95"/>
+      <c r="AK81" s="93">
         <v>1</v>
       </c>
-      <c r="AL81" s="96"/>
-      <c r="AM81" s="94">
+      <c r="AL81" s="95"/>
+      <c r="AM81" s="93">
         <v>0</v>
       </c>
-      <c r="AN81" s="96"/>
+      <c r="AN81" s="95"/>
       <c r="AO81" s="69"/>
       <c r="AP81" s="69"/>
       <c r="AQ81" s="69"/>
@@ -5069,72 +5579,72 @@
       <c r="E83" s="69"/>
       <c r="F83" s="69"/>
       <c r="G83" s="69"/>
-      <c r="H83" s="91">
+      <c r="H83" s="96">
         <v>7</v>
       </c>
-      <c r="I83" s="93"/>
-      <c r="J83" s="91">
+      <c r="I83" s="98"/>
+      <c r="J83" s="96">
         <v>6</v>
       </c>
-      <c r="K83" s="93"/>
-      <c r="L83" s="91">
+      <c r="K83" s="98"/>
+      <c r="L83" s="96">
         <v>5</v>
       </c>
-      <c r="M83" s="93"/>
-      <c r="N83" s="91">
+      <c r="M83" s="98"/>
+      <c r="N83" s="96">
         <v>4</v>
       </c>
-      <c r="O83" s="93"/>
-      <c r="P83" s="91">
+      <c r="O83" s="98"/>
+      <c r="P83" s="96">
         <v>3</v>
       </c>
-      <c r="Q83" s="93"/>
-      <c r="R83" s="91">
+      <c r="Q83" s="98"/>
+      <c r="R83" s="96">
         <v>2</v>
       </c>
-      <c r="S83" s="93"/>
-      <c r="T83" s="91">
+      <c r="S83" s="98"/>
+      <c r="T83" s="96">
         <v>1</v>
       </c>
-      <c r="U83" s="93"/>
-      <c r="V83" s="91">
+      <c r="U83" s="98"/>
+      <c r="V83" s="96">
         <v>0</v>
       </c>
-      <c r="W83" s="93"/>
+      <c r="W83" s="98"/>
       <c r="X83" s="69"/>
       <c r="Y83" s="69"/>
-      <c r="Z83" s="91">
+      <c r="Z83" s="96">
         <v>7</v>
       </c>
-      <c r="AA83" s="93"/>
-      <c r="AB83" s="91">
+      <c r="AA83" s="98"/>
+      <c r="AB83" s="96">
         <v>6</v>
       </c>
-      <c r="AC83" s="93"/>
-      <c r="AD83" s="91">
+      <c r="AC83" s="98"/>
+      <c r="AD83" s="96">
         <v>5</v>
       </c>
-      <c r="AE83" s="93"/>
-      <c r="AF83" s="91">
+      <c r="AE83" s="98"/>
+      <c r="AF83" s="96">
         <v>4</v>
       </c>
-      <c r="AG83" s="93"/>
-      <c r="AH83" s="91">
+      <c r="AG83" s="98"/>
+      <c r="AH83" s="96">
         <v>3</v>
       </c>
-      <c r="AI83" s="93"/>
-      <c r="AJ83" s="91">
+      <c r="AI83" s="98"/>
+      <c r="AJ83" s="96">
         <v>2</v>
       </c>
-      <c r="AK83" s="93"/>
-      <c r="AL83" s="91">
+      <c r="AK83" s="98"/>
+      <c r="AL83" s="96">
         <v>1</v>
       </c>
-      <c r="AM83" s="93"/>
-      <c r="AN83" s="91">
+      <c r="AM83" s="98"/>
+      <c r="AN83" s="96">
         <v>0</v>
       </c>
-      <c r="AO83" s="93"/>
+      <c r="AO83" s="98"/>
       <c r="AP83" s="69"/>
       <c r="AQ83" s="69"/>
       <c r="AR83" s="69"/>
@@ -5310,72 +5820,72 @@
       <c r="E92" s="69"/>
       <c r="F92" s="69"/>
       <c r="G92" s="69"/>
-      <c r="H92" s="94">
+      <c r="H92" s="93">
         <v>7</v>
       </c>
-      <c r="I92" s="96"/>
-      <c r="J92" s="94">
+      <c r="I92" s="95"/>
+      <c r="J92" s="93">
         <v>6</v>
       </c>
-      <c r="K92" s="96"/>
-      <c r="L92" s="94">
+      <c r="K92" s="95"/>
+      <c r="L92" s="93">
         <v>5</v>
       </c>
-      <c r="M92" s="96"/>
-      <c r="N92" s="94">
+      <c r="M92" s="95"/>
+      <c r="N92" s="93">
         <v>4</v>
       </c>
-      <c r="O92" s="96"/>
-      <c r="P92" s="94">
+      <c r="O92" s="95"/>
+      <c r="P92" s="93">
         <v>3</v>
       </c>
-      <c r="Q92" s="96"/>
-      <c r="R92" s="94">
+      <c r="Q92" s="95"/>
+      <c r="R92" s="93">
         <v>2</v>
       </c>
-      <c r="S92" s="96"/>
-      <c r="T92" s="94">
+      <c r="S92" s="95"/>
+      <c r="T92" s="93">
         <v>1</v>
       </c>
-      <c r="U92" s="96"/>
-      <c r="V92" s="94">
+      <c r="U92" s="95"/>
+      <c r="V92" s="93">
         <v>0</v>
       </c>
-      <c r="W92" s="96"/>
+      <c r="W92" s="95"/>
       <c r="X92" s="69"/>
       <c r="Y92" s="69"/>
-      <c r="Z92" s="94">
+      <c r="Z92" s="93">
         <v>7</v>
       </c>
-      <c r="AA92" s="96"/>
-      <c r="AB92" s="94">
+      <c r="AA92" s="95"/>
+      <c r="AB92" s="93">
         <v>6</v>
       </c>
-      <c r="AC92" s="96"/>
-      <c r="AD92" s="94">
+      <c r="AC92" s="95"/>
+      <c r="AD92" s="93">
         <v>5</v>
       </c>
-      <c r="AE92" s="96"/>
-      <c r="AF92" s="94">
+      <c r="AE92" s="95"/>
+      <c r="AF92" s="93">
         <v>4</v>
       </c>
-      <c r="AG92" s="96"/>
-      <c r="AH92" s="94">
+      <c r="AG92" s="95"/>
+      <c r="AH92" s="93">
         <v>3</v>
       </c>
-      <c r="AI92" s="96"/>
-      <c r="AJ92" s="94">
+      <c r="AI92" s="95"/>
+      <c r="AJ92" s="93">
         <v>2</v>
       </c>
-      <c r="AK92" s="96"/>
-      <c r="AL92" s="94">
+      <c r="AK92" s="95"/>
+      <c r="AL92" s="93">
         <v>1</v>
       </c>
-      <c r="AM92" s="96"/>
-      <c r="AN92" s="94">
+      <c r="AM92" s="95"/>
+      <c r="AN92" s="93">
         <v>0</v>
       </c>
-      <c r="AO92" s="96"/>
+      <c r="AO92" s="95"/>
       <c r="AP92" s="69"/>
       <c r="AQ92" s="69"/>
       <c r="AR92" s="69"/>
@@ -5389,72 +5899,72 @@
       <c r="D94" s="69"/>
       <c r="E94" s="69"/>
       <c r="F94" s="69"/>
-      <c r="G94" s="91">
+      <c r="G94" s="96">
         <v>7</v>
       </c>
-      <c r="H94" s="93"/>
-      <c r="I94" s="91">
+      <c r="H94" s="98"/>
+      <c r="I94" s="96">
         <v>6</v>
       </c>
-      <c r="J94" s="93"/>
-      <c r="K94" s="91">
+      <c r="J94" s="98"/>
+      <c r="K94" s="96">
         <v>5</v>
       </c>
-      <c r="L94" s="93"/>
-      <c r="M94" s="91">
+      <c r="L94" s="98"/>
+      <c r="M94" s="96">
         <v>4</v>
       </c>
-      <c r="N94" s="93"/>
-      <c r="O94" s="91">
+      <c r="N94" s="98"/>
+      <c r="O94" s="96">
         <v>3</v>
       </c>
-      <c r="P94" s="93"/>
-      <c r="Q94" s="91">
+      <c r="P94" s="98"/>
+      <c r="Q94" s="96">
         <v>2</v>
       </c>
-      <c r="R94" s="93"/>
-      <c r="S94" s="91">
+      <c r="R94" s="98"/>
+      <c r="S94" s="96">
         <v>1</v>
       </c>
-      <c r="T94" s="93"/>
-      <c r="U94" s="91">
+      <c r="T94" s="98"/>
+      <c r="U94" s="96">
         <v>0</v>
       </c>
-      <c r="V94" s="93"/>
+      <c r="V94" s="98"/>
       <c r="W94" s="69"/>
       <c r="X94" s="69"/>
-      <c r="Y94" s="91">
+      <c r="Y94" s="96">
         <v>7</v>
       </c>
-      <c r="Z94" s="93"/>
-      <c r="AA94" s="91">
+      <c r="Z94" s="98"/>
+      <c r="AA94" s="96">
         <v>6</v>
       </c>
-      <c r="AB94" s="93"/>
-      <c r="AC94" s="91">
+      <c r="AB94" s="98"/>
+      <c r="AC94" s="96">
         <v>5</v>
       </c>
-      <c r="AD94" s="93"/>
-      <c r="AE94" s="91">
+      <c r="AD94" s="98"/>
+      <c r="AE94" s="96">
         <v>4</v>
       </c>
-      <c r="AF94" s="93"/>
-      <c r="AG94" s="91">
+      <c r="AF94" s="98"/>
+      <c r="AG94" s="96">
         <v>3</v>
       </c>
-      <c r="AH94" s="93"/>
-      <c r="AI94" s="91">
+      <c r="AH94" s="98"/>
+      <c r="AI94" s="96">
         <v>2</v>
       </c>
-      <c r="AJ94" s="93"/>
-      <c r="AK94" s="91">
+      <c r="AJ94" s="98"/>
+      <c r="AK94" s="96">
         <v>1</v>
       </c>
-      <c r="AL94" s="93"/>
-      <c r="AM94" s="91">
+      <c r="AL94" s="98"/>
+      <c r="AM94" s="96">
         <v>0</v>
       </c>
-      <c r="AN94" s="93"/>
+      <c r="AN94" s="98"/>
       <c r="AO94" s="69"/>
       <c r="AP94" s="69"/>
       <c r="AQ94" s="69"/>
@@ -5629,72 +6139,72 @@
       <c r="D103" s="69"/>
       <c r="E103" s="69"/>
       <c r="F103" s="69"/>
-      <c r="G103" s="94">
+      <c r="G103" s="93">
         <v>7</v>
       </c>
-      <c r="H103" s="96"/>
-      <c r="I103" s="94">
+      <c r="H103" s="95"/>
+      <c r="I103" s="93">
         <v>6</v>
       </c>
-      <c r="J103" s="96"/>
-      <c r="K103" s="94">
+      <c r="J103" s="95"/>
+      <c r="K103" s="93">
         <v>5</v>
       </c>
-      <c r="L103" s="96"/>
-      <c r="M103" s="94">
+      <c r="L103" s="95"/>
+      <c r="M103" s="93">
         <v>4</v>
       </c>
-      <c r="N103" s="96"/>
-      <c r="O103" s="94">
+      <c r="N103" s="95"/>
+      <c r="O103" s="93">
         <v>3</v>
       </c>
-      <c r="P103" s="96"/>
-      <c r="Q103" s="94">
+      <c r="P103" s="95"/>
+      <c r="Q103" s="93">
         <v>2</v>
       </c>
-      <c r="R103" s="96"/>
-      <c r="S103" s="94">
+      <c r="R103" s="95"/>
+      <c r="S103" s="93">
         <v>1</v>
       </c>
-      <c r="T103" s="96"/>
-      <c r="U103" s="94">
+      <c r="T103" s="95"/>
+      <c r="U103" s="93">
         <v>0</v>
       </c>
-      <c r="V103" s="96"/>
+      <c r="V103" s="95"/>
       <c r="W103" s="69"/>
       <c r="X103" s="69"/>
-      <c r="Y103" s="94">
+      <c r="Y103" s="93">
         <v>7</v>
       </c>
-      <c r="Z103" s="96"/>
-      <c r="AA103" s="94">
+      <c r="Z103" s="95"/>
+      <c r="AA103" s="93">
         <v>6</v>
       </c>
-      <c r="AB103" s="96"/>
-      <c r="AC103" s="94">
+      <c r="AB103" s="95"/>
+      <c r="AC103" s="93">
         <v>5</v>
       </c>
-      <c r="AD103" s="96"/>
-      <c r="AE103" s="94">
+      <c r="AD103" s="95"/>
+      <c r="AE103" s="93">
         <v>4</v>
       </c>
-      <c r="AF103" s="96"/>
-      <c r="AG103" s="94">
+      <c r="AF103" s="95"/>
+      <c r="AG103" s="93">
         <v>3</v>
       </c>
-      <c r="AH103" s="96"/>
-      <c r="AI103" s="94">
+      <c r="AH103" s="95"/>
+      <c r="AI103" s="93">
         <v>2</v>
       </c>
-      <c r="AJ103" s="96"/>
-      <c r="AK103" s="94">
+      <c r="AJ103" s="95"/>
+      <c r="AK103" s="93">
         <v>1</v>
       </c>
-      <c r="AL103" s="96"/>
-      <c r="AM103" s="94">
+      <c r="AL103" s="95"/>
+      <c r="AM103" s="93">
         <v>0</v>
       </c>
-      <c r="AN103" s="96"/>
+      <c r="AN103" s="95"/>
       <c r="AO103" s="69"/>
       <c r="AP103" s="69"/>
       <c r="AQ103" s="69"/>
@@ -5710,72 +6220,72 @@
       <c r="E105" s="69"/>
       <c r="F105" s="69"/>
       <c r="G105" s="69"/>
-      <c r="H105" s="91">
+      <c r="H105" s="96">
         <v>7</v>
       </c>
-      <c r="I105" s="93"/>
-      <c r="J105" s="91">
+      <c r="I105" s="98"/>
+      <c r="J105" s="96">
         <v>6</v>
       </c>
-      <c r="K105" s="93"/>
-      <c r="L105" s="91">
+      <c r="K105" s="98"/>
+      <c r="L105" s="96">
         <v>5</v>
       </c>
-      <c r="M105" s="93"/>
-      <c r="N105" s="91">
+      <c r="M105" s="98"/>
+      <c r="N105" s="96">
         <v>4</v>
       </c>
-      <c r="O105" s="93"/>
-      <c r="P105" s="91">
+      <c r="O105" s="98"/>
+      <c r="P105" s="96">
         <v>3</v>
       </c>
-      <c r="Q105" s="93"/>
-      <c r="R105" s="91">
+      <c r="Q105" s="98"/>
+      <c r="R105" s="96">
         <v>2</v>
       </c>
-      <c r="S105" s="93"/>
-      <c r="T105" s="91">
+      <c r="S105" s="98"/>
+      <c r="T105" s="96">
         <v>1</v>
       </c>
-      <c r="U105" s="93"/>
-      <c r="V105" s="91">
+      <c r="U105" s="98"/>
+      <c r="V105" s="96">
         <v>0</v>
       </c>
-      <c r="W105" s="93"/>
+      <c r="W105" s="98"/>
       <c r="X105" s="69"/>
       <c r="Y105" s="69"/>
-      <c r="Z105" s="91">
+      <c r="Z105" s="96">
         <v>7</v>
       </c>
-      <c r="AA105" s="93"/>
-      <c r="AB105" s="91">
+      <c r="AA105" s="98"/>
+      <c r="AB105" s="96">
         <v>6</v>
       </c>
-      <c r="AC105" s="93"/>
-      <c r="AD105" s="91">
+      <c r="AC105" s="98"/>
+      <c r="AD105" s="96">
         <v>5</v>
       </c>
-      <c r="AE105" s="93"/>
-      <c r="AF105" s="91">
+      <c r="AE105" s="98"/>
+      <c r="AF105" s="96">
         <v>4</v>
       </c>
-      <c r="AG105" s="93"/>
-      <c r="AH105" s="91">
+      <c r="AG105" s="98"/>
+      <c r="AH105" s="96">
         <v>3</v>
       </c>
-      <c r="AI105" s="93"/>
-      <c r="AJ105" s="91">
+      <c r="AI105" s="98"/>
+      <c r="AJ105" s="96">
         <v>2</v>
       </c>
-      <c r="AK105" s="93"/>
-      <c r="AL105" s="91">
+      <c r="AK105" s="98"/>
+      <c r="AL105" s="96">
         <v>1</v>
       </c>
-      <c r="AM105" s="93"/>
-      <c r="AN105" s="91">
+      <c r="AM105" s="98"/>
+      <c r="AN105" s="96">
         <v>0</v>
       </c>
-      <c r="AO105" s="93"/>
+      <c r="AO105" s="98"/>
       <c r="AP105" s="69"/>
       <c r="AQ105" s="69"/>
       <c r="AR105" s="69"/>
@@ -5954,72 +6464,72 @@
       <c r="E114" s="69"/>
       <c r="F114" s="69"/>
       <c r="G114" s="69"/>
-      <c r="H114" s="94">
+      <c r="H114" s="93">
         <v>7</v>
       </c>
-      <c r="I114" s="96"/>
-      <c r="J114" s="94">
+      <c r="I114" s="95"/>
+      <c r="J114" s="93">
         <v>6</v>
       </c>
-      <c r="K114" s="96"/>
-      <c r="L114" s="94">
+      <c r="K114" s="95"/>
+      <c r="L114" s="93">
         <v>5</v>
       </c>
-      <c r="M114" s="96"/>
-      <c r="N114" s="94">
+      <c r="M114" s="95"/>
+      <c r="N114" s="93">
         <v>4</v>
       </c>
-      <c r="O114" s="96"/>
-      <c r="P114" s="94">
+      <c r="O114" s="95"/>
+      <c r="P114" s="93">
         <v>3</v>
       </c>
-      <c r="Q114" s="96"/>
-      <c r="R114" s="94">
+      <c r="Q114" s="95"/>
+      <c r="R114" s="93">
         <v>2</v>
       </c>
-      <c r="S114" s="96"/>
-      <c r="T114" s="94">
+      <c r="S114" s="95"/>
+      <c r="T114" s="93">
         <v>1</v>
       </c>
-      <c r="U114" s="96"/>
-      <c r="V114" s="94">
+      <c r="U114" s="95"/>
+      <c r="V114" s="93">
         <v>0</v>
       </c>
-      <c r="W114" s="96"/>
+      <c r="W114" s="95"/>
       <c r="X114" s="69"/>
       <c r="Y114" s="69"/>
-      <c r="Z114" s="94">
+      <c r="Z114" s="93">
         <v>7</v>
       </c>
-      <c r="AA114" s="96"/>
-      <c r="AB114" s="94">
+      <c r="AA114" s="95"/>
+      <c r="AB114" s="93">
         <v>6</v>
       </c>
-      <c r="AC114" s="96"/>
-      <c r="AD114" s="94">
+      <c r="AC114" s="95"/>
+      <c r="AD114" s="93">
         <v>5</v>
       </c>
-      <c r="AE114" s="96"/>
-      <c r="AF114" s="94">
+      <c r="AE114" s="95"/>
+      <c r="AF114" s="93">
         <v>4</v>
       </c>
-      <c r="AG114" s="96"/>
-      <c r="AH114" s="94">
+      <c r="AG114" s="95"/>
+      <c r="AH114" s="93">
         <v>3</v>
       </c>
-      <c r="AI114" s="96"/>
-      <c r="AJ114" s="94">
+      <c r="AI114" s="95"/>
+      <c r="AJ114" s="93">
         <v>2</v>
       </c>
-      <c r="AK114" s="96"/>
-      <c r="AL114" s="94">
+      <c r="AK114" s="95"/>
+      <c r="AL114" s="93">
         <v>1</v>
       </c>
-      <c r="AM114" s="96"/>
-      <c r="AN114" s="94">
+      <c r="AM114" s="95"/>
+      <c r="AN114" s="93">
         <v>0</v>
       </c>
-      <c r="AO114" s="96"/>
+      <c r="AO114" s="95"/>
       <c r="AP114" s="69"/>
       <c r="AQ114" s="69"/>
       <c r="AR114" s="69"/>
@@ -6033,72 +6543,72 @@
       <c r="D116" s="69"/>
       <c r="E116" s="69"/>
       <c r="F116" s="69"/>
-      <c r="G116" s="91">
+      <c r="G116" s="96">
         <v>7</v>
       </c>
-      <c r="H116" s="93"/>
-      <c r="I116" s="91">
+      <c r="H116" s="98"/>
+      <c r="I116" s="96">
         <v>6</v>
       </c>
-      <c r="J116" s="93"/>
-      <c r="K116" s="91">
+      <c r="J116" s="98"/>
+      <c r="K116" s="96">
         <v>5</v>
       </c>
-      <c r="L116" s="93"/>
-      <c r="M116" s="91">
+      <c r="L116" s="98"/>
+      <c r="M116" s="96">
         <v>4</v>
       </c>
-      <c r="N116" s="93"/>
-      <c r="O116" s="91">
+      <c r="N116" s="98"/>
+      <c r="O116" s="96">
         <v>3</v>
       </c>
-      <c r="P116" s="93"/>
-      <c r="Q116" s="91">
+      <c r="P116" s="98"/>
+      <c r="Q116" s="96">
         <v>2</v>
       </c>
-      <c r="R116" s="93"/>
-      <c r="S116" s="91">
+      <c r="R116" s="98"/>
+      <c r="S116" s="96">
         <v>1</v>
       </c>
-      <c r="T116" s="93"/>
-      <c r="U116" s="91">
+      <c r="T116" s="98"/>
+      <c r="U116" s="96">
         <v>0</v>
       </c>
-      <c r="V116" s="93"/>
+      <c r="V116" s="98"/>
       <c r="W116" s="69"/>
       <c r="X116" s="69"/>
-      <c r="Y116" s="91">
+      <c r="Y116" s="96">
         <v>7</v>
       </c>
-      <c r="Z116" s="93"/>
-      <c r="AA116" s="91">
+      <c r="Z116" s="98"/>
+      <c r="AA116" s="96">
         <v>6</v>
       </c>
-      <c r="AB116" s="93"/>
-      <c r="AC116" s="91">
+      <c r="AB116" s="98"/>
+      <c r="AC116" s="96">
         <v>5</v>
       </c>
-      <c r="AD116" s="93"/>
-      <c r="AE116" s="91">
+      <c r="AD116" s="98"/>
+      <c r="AE116" s="96">
         <v>4</v>
       </c>
-      <c r="AF116" s="93"/>
-      <c r="AG116" s="91">
+      <c r="AF116" s="98"/>
+      <c r="AG116" s="96">
         <v>3</v>
       </c>
-      <c r="AH116" s="93"/>
-      <c r="AI116" s="91">
+      <c r="AH116" s="98"/>
+      <c r="AI116" s="96">
         <v>2</v>
       </c>
-      <c r="AJ116" s="93"/>
-      <c r="AK116" s="91">
+      <c r="AJ116" s="98"/>
+      <c r="AK116" s="96">
         <v>1</v>
       </c>
-      <c r="AL116" s="93"/>
-      <c r="AM116" s="91">
+      <c r="AL116" s="98"/>
+      <c r="AM116" s="96">
         <v>0</v>
       </c>
-      <c r="AN116" s="93"/>
+      <c r="AN116" s="98"/>
       <c r="AO116" s="69"/>
       <c r="AP116" s="69"/>
       <c r="AQ116" s="69"/>
@@ -6108,17 +6618,263 @@
     </row>
   </sheetData>
   <mergeCells count="292">
-    <mergeCell ref="BG24:BH24"/>
-    <mergeCell ref="BE24:BF24"/>
-    <mergeCell ref="BC24:BD24"/>
-    <mergeCell ref="AS16:BI16"/>
-    <mergeCell ref="AA34:AQ34"/>
-    <mergeCell ref="AE24:AF24"/>
-    <mergeCell ref="AG24:AH24"/>
-    <mergeCell ref="AI24:AJ24"/>
-    <mergeCell ref="AK24:AL24"/>
-    <mergeCell ref="AM24:AN24"/>
-    <mergeCell ref="AO24:AP24"/>
+    <mergeCell ref="AS53:BI53"/>
+    <mergeCell ref="Y62:AN62"/>
+    <mergeCell ref="BK16:BL16"/>
+    <mergeCell ref="BK51:BL51"/>
+    <mergeCell ref="BK68:BL68"/>
+    <mergeCell ref="D68:X68"/>
+    <mergeCell ref="D34:Z34"/>
+    <mergeCell ref="AR34:AS34"/>
+    <mergeCell ref="F51:X51"/>
+    <mergeCell ref="D16:Z16"/>
+    <mergeCell ref="BE41:BF41"/>
+    <mergeCell ref="BG41:BH41"/>
+    <mergeCell ref="AY41:AZ41"/>
+    <mergeCell ref="BA41:BB41"/>
+    <mergeCell ref="BC41:BD41"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="AY58:AZ58"/>
+    <mergeCell ref="BA58:BB58"/>
+    <mergeCell ref="BC58:BD58"/>
+    <mergeCell ref="BE58:BF58"/>
+    <mergeCell ref="BG58:BH58"/>
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="AI116:AJ116"/>
+    <mergeCell ref="AK116:AL116"/>
+    <mergeCell ref="AM116:AN116"/>
+    <mergeCell ref="U116:V116"/>
+    <mergeCell ref="Y116:Z116"/>
+    <mergeCell ref="AA116:AB116"/>
+    <mergeCell ref="AC116:AD116"/>
+    <mergeCell ref="AE116:AF116"/>
+    <mergeCell ref="AG116:AH116"/>
+    <mergeCell ref="AJ105:AK105"/>
+    <mergeCell ref="AL105:AM105"/>
+    <mergeCell ref="AN105:AO105"/>
+    <mergeCell ref="AB105:AC105"/>
+    <mergeCell ref="AD105:AE105"/>
+    <mergeCell ref="AF105:AG105"/>
+    <mergeCell ref="AH105:AI105"/>
+    <mergeCell ref="AI94:AJ94"/>
+    <mergeCell ref="AK94:AL94"/>
+    <mergeCell ref="AM94:AN94"/>
+    <mergeCell ref="U94:V94"/>
+    <mergeCell ref="AA53:AQ53"/>
+    <mergeCell ref="AN83:AO83"/>
+    <mergeCell ref="V83:W83"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="I116:J116"/>
+    <mergeCell ref="K116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="O116:P116"/>
+    <mergeCell ref="Q116:R116"/>
+    <mergeCell ref="S116:T116"/>
+    <mergeCell ref="V105:W105"/>
+    <mergeCell ref="Z105:AA105"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="L105:M105"/>
+    <mergeCell ref="N105:O105"/>
+    <mergeCell ref="P105:Q105"/>
+    <mergeCell ref="R105:S105"/>
+    <mergeCell ref="T105:U105"/>
+    <mergeCell ref="R114:S114"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="L114:M114"/>
+    <mergeCell ref="N114:O114"/>
+    <mergeCell ref="P114:Q114"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="K94:L94"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="O94:P94"/>
+    <mergeCell ref="Q94:R94"/>
+    <mergeCell ref="S94:T94"/>
+    <mergeCell ref="P83:Q83"/>
+    <mergeCell ref="R83:S83"/>
+    <mergeCell ref="T83:U83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="L83:M83"/>
+    <mergeCell ref="N83:O83"/>
+    <mergeCell ref="AN114:AO114"/>
+    <mergeCell ref="T114:U114"/>
+    <mergeCell ref="V114:W114"/>
+    <mergeCell ref="Z114:AA114"/>
+    <mergeCell ref="AB114:AC114"/>
+    <mergeCell ref="AD114:AE114"/>
+    <mergeCell ref="AF114:AG114"/>
+    <mergeCell ref="AH92:AI92"/>
+    <mergeCell ref="AJ92:AK92"/>
+    <mergeCell ref="AL92:AM92"/>
+    <mergeCell ref="AN92:AO92"/>
+    <mergeCell ref="Y94:Z94"/>
+    <mergeCell ref="AA94:AB94"/>
+    <mergeCell ref="AC94:AD94"/>
+    <mergeCell ref="AE94:AF94"/>
+    <mergeCell ref="AG94:AH94"/>
+    <mergeCell ref="AI103:AJ103"/>
+    <mergeCell ref="AK103:AL103"/>
+    <mergeCell ref="AH114:AI114"/>
+    <mergeCell ref="AJ114:AK114"/>
+    <mergeCell ref="AL114:AM114"/>
+    <mergeCell ref="AL83:AM83"/>
+    <mergeCell ref="U103:V103"/>
+    <mergeCell ref="Y103:Z103"/>
+    <mergeCell ref="AA103:AB103"/>
+    <mergeCell ref="AC103:AD103"/>
+    <mergeCell ref="AE103:AF103"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:W92"/>
+    <mergeCell ref="Z92:AA92"/>
+    <mergeCell ref="AB92:AC92"/>
+    <mergeCell ref="AD92:AE92"/>
+    <mergeCell ref="AF92:AG92"/>
+    <mergeCell ref="AG103:AH103"/>
+    <mergeCell ref="Z83:AA83"/>
+    <mergeCell ref="AB83:AC83"/>
+    <mergeCell ref="AD83:AE83"/>
+    <mergeCell ref="AF83:AG83"/>
+    <mergeCell ref="AH83:AI83"/>
+    <mergeCell ref="AJ83:AK83"/>
+    <mergeCell ref="AG81:AH81"/>
+    <mergeCell ref="AI81:AJ81"/>
+    <mergeCell ref="AK81:AL81"/>
+    <mergeCell ref="AM81:AN81"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="I103:J103"/>
+    <mergeCell ref="K103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="O103:P103"/>
+    <mergeCell ref="Q103:R103"/>
+    <mergeCell ref="S81:T81"/>
+    <mergeCell ref="U81:V81"/>
+    <mergeCell ref="Y81:Z81"/>
+    <mergeCell ref="AA81:AB81"/>
+    <mergeCell ref="AC81:AD81"/>
+    <mergeCell ref="AE81:AF81"/>
+    <mergeCell ref="AM103:AN103"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="L92:M92"/>
+    <mergeCell ref="N92:O92"/>
+    <mergeCell ref="P92:Q92"/>
+    <mergeCell ref="R92:S92"/>
+    <mergeCell ref="S103:T103"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="M81:N81"/>
+    <mergeCell ref="O81:P81"/>
+    <mergeCell ref="Q81:R81"/>
+    <mergeCell ref="AS41:AT41"/>
+    <mergeCell ref="AU41:AV41"/>
+    <mergeCell ref="AW41:AX41"/>
+    <mergeCell ref="AG41:AH41"/>
+    <mergeCell ref="AI41:AJ41"/>
+    <mergeCell ref="AK41:AL41"/>
+    <mergeCell ref="AM41:AN41"/>
+    <mergeCell ref="AO41:AP41"/>
+    <mergeCell ref="AQ41:AR41"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="W41:X41"/>
+    <mergeCell ref="Y41:Z41"/>
+    <mergeCell ref="AA41:AB41"/>
+    <mergeCell ref="AC41:AD41"/>
+    <mergeCell ref="AE41:AF41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="AK58:AL58"/>
+    <mergeCell ref="AM58:AN58"/>
+    <mergeCell ref="AO58:AP58"/>
+    <mergeCell ref="AQ58:AR58"/>
+    <mergeCell ref="AS58:AT58"/>
+    <mergeCell ref="AU58:AV58"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="BI41:BK41"/>
+    <mergeCell ref="G45:P45"/>
+    <mergeCell ref="Q45:T45"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="W45:X45"/>
+    <mergeCell ref="Y45:AN45"/>
+    <mergeCell ref="AO45:AP45"/>
+    <mergeCell ref="AQ45:BF45"/>
+    <mergeCell ref="G28:P28"/>
+    <mergeCell ref="Q28:T28"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="Y28:AN28"/>
+    <mergeCell ref="AO28:AP28"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="AA24:AB24"/>
+    <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="BG10:BH10"/>
+    <mergeCell ref="Y10:AN10"/>
+    <mergeCell ref="AQ10:BF10"/>
+    <mergeCell ref="G10:P10"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="AO10:AP10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="AA16:AQ16"/>
+    <mergeCell ref="BJ6:BL6"/>
+    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AS6:AT6"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AW6:AX6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="G62:P62"/>
+    <mergeCell ref="Q62:T62"/>
+    <mergeCell ref="U62:V62"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="O58:P58"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="S58:T58"/>
+    <mergeCell ref="U58:V58"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
     <mergeCell ref="AA70:AQ70"/>
     <mergeCell ref="AS70:BI70"/>
     <mergeCell ref="AA36:AQ36"/>
@@ -6143,263 +6899,17 @@
     <mergeCell ref="AY24:AZ24"/>
     <mergeCell ref="AW24:AX24"/>
     <mergeCell ref="AU24:AV24"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="G62:P62"/>
-    <mergeCell ref="Q62:T62"/>
-    <mergeCell ref="U62:V62"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="O58:P58"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="S58:T58"/>
-    <mergeCell ref="U58:V58"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="BJ6:BL6"/>
-    <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AS6:AT6"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AW6:AX6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="AA24:AB24"/>
-    <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="BG10:BH10"/>
-    <mergeCell ref="Y10:AN10"/>
-    <mergeCell ref="AQ10:BF10"/>
-    <mergeCell ref="G10:P10"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="AO10:AP10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AA16:AQ16"/>
-    <mergeCell ref="AK58:AL58"/>
-    <mergeCell ref="AM58:AN58"/>
-    <mergeCell ref="AO58:AP58"/>
-    <mergeCell ref="AQ58:AR58"/>
-    <mergeCell ref="AS58:AT58"/>
-    <mergeCell ref="AU58:AV58"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="BI41:BK41"/>
-    <mergeCell ref="G45:P45"/>
-    <mergeCell ref="Q45:T45"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="W45:X45"/>
-    <mergeCell ref="Y45:AN45"/>
-    <mergeCell ref="AO45:AP45"/>
-    <mergeCell ref="AQ45:BF45"/>
-    <mergeCell ref="G28:P28"/>
-    <mergeCell ref="Q28:T28"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="Y28:AN28"/>
-    <mergeCell ref="AO28:AP28"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="K81:L81"/>
-    <mergeCell ref="M81:N81"/>
-    <mergeCell ref="O81:P81"/>
-    <mergeCell ref="Q81:R81"/>
-    <mergeCell ref="AS41:AT41"/>
-    <mergeCell ref="AU41:AV41"/>
-    <mergeCell ref="AW41:AX41"/>
-    <mergeCell ref="AG41:AH41"/>
-    <mergeCell ref="AI41:AJ41"/>
-    <mergeCell ref="AK41:AL41"/>
-    <mergeCell ref="AM41:AN41"/>
-    <mergeCell ref="AO41:AP41"/>
-    <mergeCell ref="AQ41:AR41"/>
-    <mergeCell ref="U41:V41"/>
-    <mergeCell ref="W41:X41"/>
-    <mergeCell ref="Y41:Z41"/>
-    <mergeCell ref="AA41:AB41"/>
-    <mergeCell ref="AC41:AD41"/>
-    <mergeCell ref="AE41:AF41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="AG81:AH81"/>
-    <mergeCell ref="AI81:AJ81"/>
-    <mergeCell ref="AK81:AL81"/>
-    <mergeCell ref="AM81:AN81"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="I103:J103"/>
-    <mergeCell ref="K103:L103"/>
-    <mergeCell ref="M103:N103"/>
-    <mergeCell ref="O103:P103"/>
-    <mergeCell ref="Q103:R103"/>
-    <mergeCell ref="S81:T81"/>
-    <mergeCell ref="U81:V81"/>
-    <mergeCell ref="Y81:Z81"/>
-    <mergeCell ref="AA81:AB81"/>
-    <mergeCell ref="AC81:AD81"/>
-    <mergeCell ref="AE81:AF81"/>
-    <mergeCell ref="AM103:AN103"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="L92:M92"/>
-    <mergeCell ref="N92:O92"/>
-    <mergeCell ref="P92:Q92"/>
-    <mergeCell ref="R92:S92"/>
-    <mergeCell ref="S103:T103"/>
-    <mergeCell ref="AL83:AM83"/>
-    <mergeCell ref="U103:V103"/>
-    <mergeCell ref="Y103:Z103"/>
-    <mergeCell ref="AA103:AB103"/>
-    <mergeCell ref="AC103:AD103"/>
-    <mergeCell ref="AE103:AF103"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:W92"/>
-    <mergeCell ref="Z92:AA92"/>
-    <mergeCell ref="AB92:AC92"/>
-    <mergeCell ref="AD92:AE92"/>
-    <mergeCell ref="AF92:AG92"/>
-    <mergeCell ref="AG103:AH103"/>
-    <mergeCell ref="Z83:AA83"/>
-    <mergeCell ref="AB83:AC83"/>
-    <mergeCell ref="AD83:AE83"/>
-    <mergeCell ref="AF83:AG83"/>
-    <mergeCell ref="AH83:AI83"/>
-    <mergeCell ref="AJ83:AK83"/>
-    <mergeCell ref="AN114:AO114"/>
-    <mergeCell ref="T114:U114"/>
-    <mergeCell ref="V114:W114"/>
-    <mergeCell ref="Z114:AA114"/>
-    <mergeCell ref="AB114:AC114"/>
-    <mergeCell ref="AD114:AE114"/>
-    <mergeCell ref="AF114:AG114"/>
-    <mergeCell ref="AH92:AI92"/>
-    <mergeCell ref="AJ92:AK92"/>
-    <mergeCell ref="AL92:AM92"/>
-    <mergeCell ref="AN92:AO92"/>
-    <mergeCell ref="Y94:Z94"/>
-    <mergeCell ref="AA94:AB94"/>
-    <mergeCell ref="AC94:AD94"/>
-    <mergeCell ref="AE94:AF94"/>
-    <mergeCell ref="AG94:AH94"/>
-    <mergeCell ref="AI103:AJ103"/>
-    <mergeCell ref="AK103:AL103"/>
-    <mergeCell ref="AH114:AI114"/>
-    <mergeCell ref="AJ114:AK114"/>
-    <mergeCell ref="AL114:AM114"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="I94:J94"/>
-    <mergeCell ref="K94:L94"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="O94:P94"/>
-    <mergeCell ref="Q94:R94"/>
-    <mergeCell ref="S94:T94"/>
-    <mergeCell ref="P83:Q83"/>
-    <mergeCell ref="R83:S83"/>
-    <mergeCell ref="T83:U83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="L83:M83"/>
-    <mergeCell ref="N83:O83"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="I116:J116"/>
-    <mergeCell ref="K116:L116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="O116:P116"/>
-    <mergeCell ref="Q116:R116"/>
-    <mergeCell ref="S116:T116"/>
-    <mergeCell ref="V105:W105"/>
-    <mergeCell ref="Z105:AA105"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="L105:M105"/>
-    <mergeCell ref="N105:O105"/>
-    <mergeCell ref="P105:Q105"/>
-    <mergeCell ref="R105:S105"/>
-    <mergeCell ref="T105:U105"/>
-    <mergeCell ref="R114:S114"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="L114:M114"/>
-    <mergeCell ref="N114:O114"/>
-    <mergeCell ref="P114:Q114"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="AI116:AJ116"/>
-    <mergeCell ref="AK116:AL116"/>
-    <mergeCell ref="AM116:AN116"/>
-    <mergeCell ref="U116:V116"/>
-    <mergeCell ref="Y116:Z116"/>
-    <mergeCell ref="AA116:AB116"/>
-    <mergeCell ref="AC116:AD116"/>
-    <mergeCell ref="AE116:AF116"/>
-    <mergeCell ref="AG116:AH116"/>
-    <mergeCell ref="AJ105:AK105"/>
-    <mergeCell ref="AL105:AM105"/>
-    <mergeCell ref="AN105:AO105"/>
-    <mergeCell ref="AB105:AC105"/>
-    <mergeCell ref="AD105:AE105"/>
-    <mergeCell ref="AF105:AG105"/>
-    <mergeCell ref="AH105:AI105"/>
-    <mergeCell ref="AI94:AJ94"/>
-    <mergeCell ref="AK94:AL94"/>
-    <mergeCell ref="AM94:AN94"/>
-    <mergeCell ref="U94:V94"/>
-    <mergeCell ref="AA53:AQ53"/>
-    <mergeCell ref="AN83:AO83"/>
-    <mergeCell ref="V83:W83"/>
-    <mergeCell ref="AS53:BI53"/>
-    <mergeCell ref="Y62:AN62"/>
-    <mergeCell ref="BK16:BL16"/>
-    <mergeCell ref="BK51:BL51"/>
-    <mergeCell ref="BK68:BL68"/>
-    <mergeCell ref="D68:X68"/>
-    <mergeCell ref="D34:Z34"/>
-    <mergeCell ref="AR34:AS34"/>
-    <mergeCell ref="F51:X51"/>
-    <mergeCell ref="D16:Z16"/>
-    <mergeCell ref="BE41:BF41"/>
-    <mergeCell ref="BG41:BH41"/>
-    <mergeCell ref="AY41:AZ41"/>
-    <mergeCell ref="BA41:BB41"/>
-    <mergeCell ref="BC41:BD41"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="AY58:AZ58"/>
-    <mergeCell ref="BA58:BB58"/>
-    <mergeCell ref="BC58:BD58"/>
-    <mergeCell ref="BE58:BF58"/>
-    <mergeCell ref="BG58:BH58"/>
+    <mergeCell ref="BG24:BH24"/>
+    <mergeCell ref="BE24:BF24"/>
+    <mergeCell ref="BC24:BD24"/>
+    <mergeCell ref="AS16:BI16"/>
+    <mergeCell ref="AA34:AQ34"/>
+    <mergeCell ref="AE24:AF24"/>
+    <mergeCell ref="AG24:AH24"/>
+    <mergeCell ref="AI24:AJ24"/>
+    <mergeCell ref="AK24:AL24"/>
+    <mergeCell ref="AM24:AN24"/>
+    <mergeCell ref="AO24:AP24"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>